<commit_message>
added alacohol or drug use disorder data
</commit_message>
<xml_diff>
--- a/data_tables/Total_data_cleaned.xlsx
+++ b/data_tables/Total_data_cleaned.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ulrikaeriksson/Documents/Data_Mining/DataMining-Group23/data_tables/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F6213089-2CE5-8F48-99AD-447EB8DDEFBF}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8C4AE9E6-1175-B548-8A4C-4A95053398D3}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="22200" windowHeight="12560" xr2:uid="{196242FC-4F62-234C-ABAE-90D7B6224D3F}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="158" uniqueCount="158">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="159" uniqueCount="159">
   <si>
     <t>Afghanistan</t>
   </si>
@@ -499,6 +499,9 @@
   </si>
   <si>
     <t>Population density</t>
+  </si>
+  <si>
+    <t>Alcohol or drug use disorder</t>
   </si>
 </sst>
 </file>
@@ -967,10 +970,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{67CF83BE-F021-5E44-A4B8-2C5D9BB127DA}">
-  <dimension ref="A1:K148"/>
+  <dimension ref="A1:L148"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="K1" sqref="K1"/>
+    <sheetView tabSelected="1" topLeftCell="A24" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="H16" sqref="H16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="16"/>
@@ -986,7 +989,7 @@
     <col min="9" max="9" width="14.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="17">
+    <row r="1" spans="1:12" ht="17">
       <c r="A1" s="1" t="s">
         <v>147</v>
       </c>
@@ -1020,8 +1023,11 @@
       <c r="K1" s="16" t="s">
         <v>157</v>
       </c>
-    </row>
-    <row r="2" spans="1:11">
+      <c r="L1" s="16" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12">
       <c r="A2" s="8" t="s">
         <v>0</v>
       </c>
@@ -1049,8 +1055,11 @@
       <c r="K2" s="15">
         <v>54.422205373280597</v>
       </c>
-    </row>
-    <row r="3" spans="1:11">
+      <c r="L2" s="15">
+        <v>1.809624516</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12">
       <c r="A3" s="8" t="s">
         <v>1</v>
       </c>
@@ -1081,8 +1090,11 @@
       <c r="K3" s="15">
         <v>104.870693430657</v>
       </c>
-    </row>
-    <row r="4" spans="1:11">
+      <c r="L3" s="15">
+        <v>2.3255375310000002</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12">
       <c r="A4" s="8" t="s">
         <v>2</v>
       </c>
@@ -1113,8 +1125,11 @@
       <c r="K4" s="15">
         <v>17.347873677280599</v>
       </c>
-    </row>
-    <row r="5" spans="1:11">
+      <c r="L4" s="15">
+        <v>1.485914602</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12">
       <c r="A5" s="8" t="s">
         <v>3</v>
       </c>
@@ -1149,8 +1164,11 @@
       <c r="K5" s="15">
         <v>16.176856348362399</v>
       </c>
-    </row>
-    <row r="6" spans="1:11">
+      <c r="L5" s="15">
+        <v>3.1186833850000002</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12">
       <c r="A6" s="8" t="s">
         <v>4</v>
       </c>
@@ -1181,8 +1199,11 @@
       <c r="K6" s="15">
         <v>102.931155602388</v>
       </c>
-    </row>
-    <row r="7" spans="1:11">
+      <c r="L6" s="15">
+        <v>2.3654491160000002</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12">
       <c r="A7" s="8" t="s">
         <v>5</v>
       </c>
@@ -1217,8 +1238,11 @@
       <c r="K7" s="15">
         <v>3.20202712729261</v>
       </c>
-    </row>
-    <row r="8" spans="1:11">
+      <c r="L7" s="15">
+        <v>3.8037627660000002</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12">
       <c r="A8" s="8" t="s">
         <v>6</v>
       </c>
@@ -1253,8 +1277,11 @@
       <c r="K8" s="15">
         <v>106.748567066151</v>
       </c>
-    </row>
-    <row r="9" spans="1:11">
+      <c r="L8" s="15">
+        <v>2.8291145819999999</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12">
       <c r="A9" s="8" t="s">
         <v>7</v>
       </c>
@@ -1289,8 +1316,11 @@
       <c r="K9" s="15">
         <v>119.308868538524</v>
       </c>
-    </row>
-    <row r="10" spans="1:11">
+      <c r="L9" s="15">
+        <v>3.2560069280000001</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12">
       <c r="A10" s="8" t="s">
         <v>8</v>
       </c>
@@ -1319,8 +1349,11 @@
       <c r="K10" s="15">
         <v>1935.9066147859901</v>
       </c>
-    </row>
-    <row r="11" spans="1:11">
+      <c r="L10" s="15">
+        <v>1.615647681</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12">
       <c r="A11" s="8" t="s">
         <v>9</v>
       </c>
@@ -1351,8 +1384,11 @@
       <c r="K11" s="15">
         <v>1265.0361143120499</v>
       </c>
-    </row>
-    <row r="12" spans="1:11">
+      <c r="L11" s="15">
+        <v>2.031842132</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12">
       <c r="A12" s="8" t="s">
         <v>10</v>
       </c>
@@ -1387,8 +1423,11 @@
       <c r="K12" s="15">
         <v>46.8575969641713</v>
       </c>
-    </row>
-    <row r="13" spans="1:11">
+      <c r="L12" s="15">
+        <v>5.1028469349999996</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12">
       <c r="A13" s="8" t="s">
         <v>11</v>
       </c>
@@ -1423,8 +1462,11 @@
       <c r="K13" s="15">
         <v>375.56367239101701</v>
       </c>
-    </row>
-    <row r="14" spans="1:11">
+      <c r="L13" s="15">
+        <v>2.2844173109999999</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12">
       <c r="A14" s="8" t="s">
         <v>12</v>
       </c>
@@ -1455,8 +1497,11 @@
       <c r="K14" s="15">
         <v>99.110429230223502</v>
       </c>
-    </row>
-    <row r="15" spans="1:11">
+      <c r="L14" s="15">
+        <v>1.6706470899999999</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12">
       <c r="A15" s="8" t="s">
         <v>13</v>
       </c>
@@ -1489,8 +1534,11 @@
       <c r="K15" s="15">
         <v>10.2017908243331</v>
       </c>
-    </row>
-    <row r="16" spans="1:11">
+      <c r="L15" s="15">
+        <v>2.434164628</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12">
       <c r="A16" s="8" t="s">
         <v>14</v>
       </c>
@@ -1521,8 +1569,11 @@
       <c r="K16" s="15">
         <v>68.496425781249997</v>
       </c>
-    </row>
-    <row r="17" spans="1:11">
+      <c r="L16" s="15">
+        <v>3.526306038</v>
+      </c>
+    </row>
+    <row r="17" spans="1:12">
       <c r="A17" s="8" t="s">
         <v>15</v>
       </c>
@@ -1553,8 +1604,11 @@
       <c r="K17" s="15">
         <v>4.04365570906781</v>
       </c>
-    </row>
-    <row r="18" spans="1:11">
+      <c r="L17" s="15">
+        <v>2.3786810370000002</v>
+      </c>
+    </row>
+    <row r="18" spans="1:12">
       <c r="A18" s="8" t="s">
         <v>16</v>
       </c>
@@ -1589,8 +1643,11 @@
       <c r="K18" s="15">
         <v>25.040054126875098</v>
       </c>
-    </row>
-    <row r="19" spans="1:11">
+      <c r="L18" s="15">
+        <v>3.730609555</v>
+      </c>
+    </row>
+    <row r="19" spans="1:12">
       <c r="A19" s="8" t="s">
         <v>17</v>
       </c>
@@ -1625,8 +1682,11 @@
       <c r="K19" s="15">
         <v>65.180462417096507</v>
       </c>
-    </row>
-    <row r="20" spans="1:11">
+      <c r="L19" s="15">
+        <v>2.3871194039999999</v>
+      </c>
+    </row>
+    <row r="20" spans="1:12">
       <c r="A20" s="8" t="s">
         <v>18</v>
       </c>
@@ -1661,8 +1721,11 @@
       <c r="K20" s="15">
         <v>70.151250000000005</v>
       </c>
-    </row>
-    <row r="21" spans="1:11">
+      <c r="L20" s="15">
+        <v>1.6203995840000001</v>
+      </c>
+    </row>
+    <row r="21" spans="1:12">
       <c r="A21" s="8" t="s">
         <v>19</v>
       </c>
@@ -1693,8 +1756,11 @@
       <c r="K21" s="15">
         <v>90.671725583503303</v>
       </c>
-    </row>
-    <row r="22" spans="1:11">
+      <c r="L21" s="15">
+        <v>1.5939582269999999</v>
+      </c>
+    </row>
+    <row r="22" spans="1:12">
       <c r="A22" s="8" t="s">
         <v>20</v>
       </c>
@@ -1723,8 +1789,11 @@
       <c r="K22" s="15">
         <v>50.884743288697102</v>
       </c>
-    </row>
-    <row r="23" spans="1:11">
+      <c r="L22" s="15">
+        <v>1.8031018350000001</v>
+      </c>
+    </row>
+    <row r="23" spans="1:12">
       <c r="A23" s="8" t="s">
         <v>21</v>
       </c>
@@ -1759,8 +1828,11 @@
       <c r="K23" s="15">
         <v>4.03673422033956</v>
       </c>
-    </row>
-    <row r="24" spans="1:11">
+      <c r="L23" s="15">
+        <v>3.7945346299999998</v>
+      </c>
+    </row>
+    <row r="24" spans="1:12">
       <c r="A24" s="8" t="s">
         <v>22</v>
       </c>
@@ -1789,8 +1861,11 @@
       <c r="K24" s="15">
         <v>7.47869915567113</v>
       </c>
-    </row>
-    <row r="25" spans="1:11">
+      <c r="L24" s="15">
+        <v>1.8895983300000001</v>
+      </c>
+    </row>
+    <row r="25" spans="1:12">
       <c r="A25" s="8" t="s">
         <v>23</v>
       </c>
@@ -1819,8 +1894,11 @@
       <c r="K25" s="15">
         <v>11.8329050190597</v>
       </c>
-    </row>
-    <row r="26" spans="1:11">
+      <c r="L25" s="15">
+        <v>1.612914776</v>
+      </c>
+    </row>
+    <row r="26" spans="1:12">
       <c r="A26" s="8" t="s">
         <v>24</v>
       </c>
@@ -1851,8 +1929,11 @@
       <c r="K26" s="15">
         <v>24.2823792385533</v>
       </c>
-    </row>
-    <row r="27" spans="1:11">
+      <c r="L26" s="15">
+        <v>3.461463626</v>
+      </c>
+    </row>
+    <row r="27" spans="1:12">
       <c r="A27" s="8" t="s">
         <v>25</v>
       </c>
@@ -1884,8 +1965,11 @@
       <c r="K27" s="15">
         <v>147.67403502115599</v>
       </c>
-    </row>
-    <row r="28" spans="1:11">
+      <c r="L27" s="15">
+        <v>1.9578983599999999</v>
+      </c>
+    </row>
+    <row r="28" spans="1:12">
       <c r="A28" s="8" t="s">
         <v>26</v>
       </c>
@@ -1920,8 +2004,11 @@
       <c r="K28" s="15">
         <v>44.223177106804897</v>
       </c>
-    </row>
-    <row r="29" spans="1:11">
+      <c r="L28" s="15">
+        <v>2.3728377520000001</v>
+      </c>
+    </row>
+    <row r="29" spans="1:12">
       <c r="A29" s="8" t="s">
         <v>27</v>
       </c>
@@ -1949,8 +2036,11 @@
       <c r="K29" s="15">
         <v>15.404831625183</v>
       </c>
-    </row>
-    <row r="30" spans="1:11">
+      <c r="L29" s="15">
+        <v>1.9430276660000001</v>
+      </c>
+    </row>
+    <row r="30" spans="1:12">
       <c r="A30" s="8" t="s">
         <v>28</v>
       </c>
@@ -1979,8 +2069,11 @@
       <c r="K30" s="15">
         <v>35.879221014093197</v>
       </c>
-    </row>
-    <row r="31" spans="1:11">
+      <c r="L30" s="15">
+        <v>1.8587189340000001</v>
+      </c>
+    </row>
+    <row r="31" spans="1:12">
       <c r="A31" s="8" t="s">
         <v>29</v>
       </c>
@@ -2015,8 +2108,11 @@
       <c r="K31" s="15">
         <v>96.078515471993697</v>
       </c>
-    </row>
-    <row r="32" spans="1:11">
+      <c r="L31" s="15">
+        <v>1.9148140069999999</v>
+      </c>
+    </row>
+    <row r="32" spans="1:12">
       <c r="A32" s="8" t="s">
         <v>30</v>
       </c>
@@ -2051,8 +2147,11 @@
       <c r="K32" s="15">
         <v>73.725875625446704</v>
       </c>
-    </row>
-    <row r="33" spans="1:11">
+      <c r="L32" s="15">
+        <v>2.7405460929999998</v>
+      </c>
+    </row>
+    <row r="33" spans="1:12">
       <c r="A33" s="8" t="s">
         <v>31</v>
       </c>
@@ -2087,8 +2186,11 @@
       <c r="K33" s="15">
         <v>127.65703463203501</v>
       </c>
-    </row>
-    <row r="34" spans="1:11">
+      <c r="L33" s="15">
+        <v>1.7680723469999999</v>
+      </c>
+    </row>
+    <row r="34" spans="1:12">
       <c r="A34" s="8" t="s">
         <v>32</v>
       </c>
@@ -2119,8 +2221,11 @@
       <c r="K34" s="15">
         <v>137.17553425722099</v>
       </c>
-    </row>
-    <row r="35" spans="1:11">
+      <c r="L34" s="15">
+        <v>2.7127169690000001</v>
+      </c>
+    </row>
+    <row r="35" spans="1:12">
       <c r="A35" s="8" t="s">
         <v>33</v>
       </c>
@@ -2151,8 +2256,11 @@
       <c r="K35" s="15">
         <v>136.51987601154701</v>
       </c>
-    </row>
-    <row r="36" spans="1:11">
+      <c r="L35" s="15">
+        <v>2.8271041879999999</v>
+      </c>
+    </row>
+    <row r="36" spans="1:12">
       <c r="A36" s="8" t="s">
         <v>34</v>
       </c>
@@ -2187,8 +2295,11 @@
       <c r="K36" s="15">
         <v>222.87306975781399</v>
       </c>
-    </row>
-    <row r="37" spans="1:11">
+      <c r="L36" s="15">
+        <v>2.1777191999999999</v>
+      </c>
+    </row>
+    <row r="37" spans="1:12">
       <c r="A37" s="8" t="s">
         <v>35</v>
       </c>
@@ -2219,8 +2330,11 @@
       <c r="K37" s="15">
         <v>66.938548880657095</v>
       </c>
-    </row>
-    <row r="38" spans="1:11">
+      <c r="L37" s="15">
+        <v>2.31497332</v>
+      </c>
+    </row>
+    <row r="38" spans="1:12">
       <c r="A38" s="8" t="s">
         <v>36</v>
       </c>
@@ -2251,8 +2365,11 @@
       <c r="K38" s="15">
         <v>97.999046662313503</v>
       </c>
-    </row>
-    <row r="39" spans="1:11">
+      <c r="L38" s="15">
+        <v>1.446643887</v>
+      </c>
+    </row>
+    <row r="39" spans="1:12">
       <c r="A39" s="8" t="s">
         <v>37</v>
       </c>
@@ -2283,8 +2400,11 @@
       <c r="K39" s="15">
         <v>307.81143822393801</v>
       </c>
-    </row>
-    <row r="40" spans="1:11">
+      <c r="L39" s="15">
+        <v>3.0883517739999999</v>
+      </c>
+    </row>
+    <row r="40" spans="1:12">
       <c r="A40" s="8" t="s">
         <v>38</v>
       </c>
@@ -2319,8 +2439,11 @@
       <c r="K40" s="15">
         <v>31.032790752535998</v>
       </c>
-    </row>
-    <row r="41" spans="1:11">
+      <c r="L40" s="15">
+        <v>5.4835234560000004</v>
+      </c>
+    </row>
+    <row r="41" spans="1:12">
       <c r="A41" s="8" t="s">
         <v>39</v>
       </c>
@@ -2351,8 +2474,11 @@
       <c r="K41" s="15">
         <v>104.957438</v>
       </c>
-    </row>
-    <row r="42" spans="1:11">
+      <c r="L41" s="15">
+        <v>2.616682548</v>
+      </c>
+    </row>
+    <row r="42" spans="1:12">
       <c r="A42" s="8" t="s">
         <v>40</v>
       </c>
@@ -2387,8 +2513,11 @@
       <c r="K42" s="15">
         <v>18.1358484978117</v>
       </c>
-    </row>
-    <row r="43" spans="1:11">
+      <c r="L42" s="15">
+        <v>4.0242325509999999</v>
+      </c>
+    </row>
+    <row r="43" spans="1:12">
       <c r="A43" s="8" t="s">
         <v>41</v>
       </c>
@@ -2423,8 +2552,11 @@
       <c r="K43" s="15">
         <v>122.57837631516</v>
       </c>
-    </row>
-    <row r="44" spans="1:11">
+      <c r="L43" s="15">
+        <v>2.7333169019999999</v>
+      </c>
+    </row>
+    <row r="44" spans="1:12">
       <c r="A44" s="8" t="s">
         <v>42</v>
       </c>
@@ -2450,8 +2582,11 @@
       <c r="K44" s="15">
         <v>7.8594209647999396</v>
       </c>
-    </row>
-    <row r="45" spans="1:11">
+      <c r="L44" s="15">
+        <v>2.0146800420000002</v>
+      </c>
+    </row>
+    <row r="45" spans="1:12">
       <c r="A45" s="8" t="s">
         <v>43</v>
       </c>
@@ -2479,8 +2614,11 @@
       <c r="K45" s="15">
         <v>207.56600790513801</v>
       </c>
-    </row>
-    <row r="46" spans="1:11">
+      <c r="L45" s="15">
+        <v>1.576080782</v>
+      </c>
+    </row>
+    <row r="46" spans="1:12">
       <c r="A46" s="8" t="s">
         <v>44</v>
       </c>
@@ -2515,8 +2653,11 @@
       <c r="K46" s="15">
         <v>65.032016515623397</v>
       </c>
-    </row>
-    <row r="47" spans="1:11">
+      <c r="L46" s="15">
+        <v>2.4086422789999999</v>
+      </c>
+    </row>
+    <row r="47" spans="1:12">
       <c r="A47" s="8" t="s">
         <v>45</v>
       </c>
@@ -2551,8 +2692,11 @@
       <c r="K47" s="15">
         <v>237.016337059329</v>
       </c>
-    </row>
-    <row r="48" spans="1:11">
+      <c r="L47" s="15">
+        <v>2.827630079</v>
+      </c>
+    </row>
+    <row r="48" spans="1:12">
       <c r="A48" s="8" t="s">
         <v>46</v>
       </c>
@@ -2587,8 +2731,11 @@
       <c r="K48" s="15">
         <v>126.71894611936401</v>
       </c>
-    </row>
-    <row r="49" spans="1:11">
+      <c r="L48" s="15">
+        <v>1.6884604519999999</v>
+      </c>
+    </row>
+    <row r="49" spans="1:12">
       <c r="A49" s="8" t="s">
         <v>47</v>
       </c>
@@ -2623,8 +2770,11 @@
       <c r="K49" s="15">
         <v>83.478828549263</v>
       </c>
-    </row>
-    <row r="50" spans="1:11">
+      <c r="L49" s="15">
+        <v>1.8782843119999999</v>
+      </c>
+    </row>
+    <row r="50" spans="1:12">
       <c r="A50" s="8" t="s">
         <v>48</v>
       </c>
@@ -2653,8 +2803,11 @@
       <c r="K50" s="15">
         <v>157.83410787607301</v>
       </c>
-    </row>
-    <row r="51" spans="1:11">
+      <c r="L50" s="15">
+        <v>3.162466411</v>
+      </c>
+    </row>
+    <row r="51" spans="1:12">
       <c r="A51" s="8" t="s">
         <v>49</v>
       </c>
@@ -2683,8 +2836,11 @@
       <c r="K51" s="15">
         <v>51.754745238482798</v>
       </c>
-    </row>
-    <row r="52" spans="1:11">
+      <c r="L51" s="15">
+        <v>1.590701079</v>
+      </c>
+    </row>
+    <row r="52" spans="1:12">
       <c r="A52" s="8" t="s">
         <v>50</v>
       </c>
@@ -2713,8 +2869,11 @@
       <c r="K52" s="15">
         <v>398.448076923077</v>
       </c>
-    </row>
-    <row r="53" spans="1:11">
+      <c r="L52" s="15">
+        <v>2.334270047</v>
+      </c>
+    </row>
+    <row r="53" spans="1:12">
       <c r="A53" s="8" t="s">
         <v>51</v>
       </c>
@@ -2745,8 +2904,11 @@
       <c r="K53" s="15">
         <v>82.805138975779798</v>
       </c>
-    </row>
-    <row r="54" spans="1:11">
+      <c r="L53" s="15">
+        <v>2.1300707230000002</v>
+      </c>
+    </row>
+    <row r="54" spans="1:12">
       <c r="A54" s="8" t="s">
         <v>52</v>
       </c>
@@ -2769,8 +2931,9 @@
       <c r="K54" s="15">
         <v>7039.7142857142899</v>
       </c>
-    </row>
-    <row r="55" spans="1:11">
+      <c r="L54" s="15"/>
+    </row>
+    <row r="55" spans="1:12">
       <c r="A55" s="8" t="s">
         <v>53</v>
       </c>
@@ -2805,8 +2968,11 @@
       <c r="K55" s="15">
         <v>108.042936043301</v>
       </c>
-    </row>
-    <row r="56" spans="1:11">
+      <c r="L55" s="15">
+        <v>2.6101259950000002</v>
+      </c>
+    </row>
+    <row r="56" spans="1:12">
       <c r="A56" s="8" t="s">
         <v>54</v>
       </c>
@@ -2834,8 +3000,11 @@
       <c r="K56" s="15">
         <v>3.40432917705736</v>
       </c>
-    </row>
-    <row r="57" spans="1:11">
+      <c r="L56" s="15">
+        <v>2.1393359009999999</v>
+      </c>
+    </row>
+    <row r="57" spans="1:12">
       <c r="A57" s="8" t="s">
         <v>55</v>
       </c>
@@ -2866,8 +3035,11 @@
       <c r="K57" s="15">
         <v>450.41861670461702</v>
       </c>
-    </row>
-    <row r="58" spans="1:11">
+      <c r="L57" s="15">
+        <v>1.7448725620000001</v>
+      </c>
+    </row>
+    <row r="58" spans="1:12">
       <c r="A58" s="8" t="s">
         <v>56</v>
       </c>
@@ -2898,8 +3070,11 @@
       <c r="K58" s="15">
         <v>145.72518809651299</v>
       </c>
-    </row>
-    <row r="59" spans="1:11">
+      <c r="L58" s="15">
+        <v>1.2969102939999999</v>
+      </c>
+    </row>
+    <row r="59" spans="1:12">
       <c r="A59" s="8" t="s">
         <v>57</v>
       </c>
@@ -2930,8 +3105,11 @@
       <c r="K59" s="15">
         <v>49.831029740416</v>
       </c>
-    </row>
-    <row r="60" spans="1:11">
+      <c r="L59" s="15">
+        <v>1.7879851849999999</v>
+      </c>
+    </row>
+    <row r="60" spans="1:12">
       <c r="A60" s="8" t="s">
         <v>58</v>
       </c>
@@ -2960,8 +3138,11 @@
       <c r="K60" s="15">
         <v>88.125386811567495</v>
       </c>
-    </row>
-    <row r="61" spans="1:11">
+      <c r="L60" s="15">
+        <v>2.1814031009999999</v>
+      </c>
+    </row>
+    <row r="61" spans="1:12">
       <c r="A61" s="8" t="s">
         <v>59</v>
       </c>
@@ -2996,8 +3177,11 @@
       <c r="K61" s="15">
         <v>69.873827841486403</v>
       </c>
-    </row>
-    <row r="62" spans="1:11">
+      <c r="L61" s="15">
+        <v>3.2364014619999999</v>
+      </c>
+    </row>
+    <row r="62" spans="1:12">
       <c r="A62" s="8" t="s">
         <v>60</v>
       </c>
@@ -3032,8 +3216,11 @@
       <c r="K62" s="15">
         <v>402.60628465804098</v>
       </c>
-    </row>
-    <row r="63" spans="1:11">
+      <c r="L62" s="15">
+        <v>1.3260031560000001</v>
+      </c>
+    </row>
+    <row r="63" spans="1:12">
       <c r="A63" s="8" t="s">
         <v>61</v>
       </c>
@@ -3068,8 +3255,11 @@
       <c r="K63" s="15">
         <v>205.85916910314799</v>
       </c>
-    </row>
-    <row r="64" spans="1:11">
+      <c r="L63" s="15">
+        <v>1.683797108</v>
+      </c>
+    </row>
+    <row r="64" spans="1:12">
       <c r="A64" s="8" t="s">
         <v>62</v>
       </c>
@@ -3098,8 +3288,11 @@
       <c r="K64" s="15">
         <v>76.3985849056604</v>
       </c>
-    </row>
-    <row r="65" spans="1:11">
+      <c r="L64" s="15">
+        <v>1.720200808</v>
+      </c>
+    </row>
+    <row r="65" spans="1:12">
       <c r="A65" s="8" t="s">
         <v>63</v>
       </c>
@@ -3134,8 +3327,11 @@
       <c r="K65" s="15">
         <v>266.878947368421</v>
       </c>
-    </row>
-    <row r="66" spans="1:11">
+      <c r="L65" s="15">
+        <v>2.3290716069999999</v>
+      </c>
+    </row>
+    <row r="66" spans="1:12">
       <c r="A66" s="8" t="s">
         <v>64</v>
       </c>
@@ -3170,8 +3366,11 @@
       <c r="K66" s="15">
         <v>347.77758667983301</v>
       </c>
-    </row>
-    <row r="67" spans="1:11">
+      <c r="L66" s="15">
+        <v>1.5638960449999999</v>
+      </c>
+    </row>
+    <row r="67" spans="1:12">
       <c r="A67" s="8" t="s">
         <v>65</v>
       </c>
@@ -3200,8 +3399,11 @@
       <c r="K67" s="15">
         <v>109.285345798603</v>
       </c>
-    </row>
-    <row r="68" spans="1:11">
+      <c r="L67" s="15">
+        <v>1.61326719</v>
+      </c>
+    </row>
+    <row r="68" spans="1:12">
       <c r="A68" s="8" t="s">
         <v>66</v>
       </c>
@@ -3232,8 +3434,11 @@
       <c r="K68" s="15">
         <v>6.6813520020743002</v>
       </c>
-    </row>
-    <row r="69" spans="1:11">
+      <c r="L68" s="15">
+        <v>3.3750323070000001</v>
+      </c>
+    </row>
+    <row r="69" spans="1:12">
       <c r="A69" s="8" t="s">
         <v>67</v>
       </c>
@@ -3264,8 +3469,11 @@
       <c r="K69" s="15">
         <v>87.324493094844897</v>
       </c>
-    </row>
-    <row r="70" spans="1:11">
+      <c r="L69" s="15">
+        <v>1.5311732680000001</v>
+      </c>
+    </row>
+    <row r="70" spans="1:12">
       <c r="A70" s="8" t="s">
         <v>68</v>
       </c>
@@ -3290,8 +3498,9 @@
       <c r="K70" s="15">
         <v>168.154679893451</v>
       </c>
-    </row>
-    <row r="71" spans="1:11">
+      <c r="L70" s="15"/>
+    </row>
+    <row r="71" spans="1:12">
       <c r="A71" s="8" t="s">
         <v>69</v>
       </c>
@@ -3322,8 +3531,11 @@
       <c r="K71" s="15">
         <v>232.12839506172801</v>
       </c>
-    </row>
-    <row r="72" spans="1:11">
+      <c r="L71" s="15">
+        <v>1.5134735370000001</v>
+      </c>
+    </row>
+    <row r="72" spans="1:12">
       <c r="A72" s="8" t="s">
         <v>70</v>
       </c>
@@ -3354,8 +3566,11 @@
       <c r="K72" s="15">
         <v>32.333159541188699</v>
       </c>
-    </row>
-    <row r="73" spans="1:11">
+      <c r="L72" s="15">
+        <v>3.336949615</v>
+      </c>
+    </row>
+    <row r="73" spans="1:12">
       <c r="A73" s="8" t="s">
         <v>71</v>
       </c>
@@ -3386,8 +3601,11 @@
       <c r="K73" s="15">
         <v>29.714731369150801</v>
       </c>
-    </row>
-    <row r="74" spans="1:11">
+      <c r="L73" s="15">
+        <v>1.6259996080000001</v>
+      </c>
+    </row>
+    <row r="74" spans="1:12">
       <c r="A74" s="8" t="s">
         <v>72</v>
       </c>
@@ -3422,8 +3640,11 @@
       <c r="K74" s="15">
         <v>31.2116436153104</v>
       </c>
-    </row>
-    <row r="75" spans="1:11">
+      <c r="L74" s="15">
+        <v>4.7946621010000001</v>
+      </c>
+    </row>
+    <row r="75" spans="1:12">
       <c r="A75" s="8" t="s">
         <v>73</v>
       </c>
@@ -3454,8 +3675,11 @@
       <c r="K75" s="15">
         <v>594.56080156402697</v>
       </c>
-    </row>
-    <row r="76" spans="1:11">
+      <c r="L75" s="15">
+        <v>1.6208092970000001</v>
+      </c>
+    </row>
+    <row r="76" spans="1:12">
       <c r="A76" s="8" t="s">
         <v>74</v>
       </c>
@@ -3483,8 +3707,11 @@
       <c r="K76" s="15">
         <v>73.561890645586303</v>
       </c>
-    </row>
-    <row r="77" spans="1:11">
+      <c r="L76" s="15">
+        <v>2.270169144</v>
+      </c>
+    </row>
+    <row r="77" spans="1:12">
       <c r="A77" s="8" t="s">
         <v>75</v>
       </c>
@@ -3515,8 +3742,11 @@
       <c r="K77" s="15">
         <v>49.126931063122903</v>
       </c>
-    </row>
-    <row r="78" spans="1:11">
+      <c r="L77" s="15">
+        <v>1.612780331</v>
+      </c>
+    </row>
+    <row r="78" spans="1:12">
       <c r="A78" s="8" t="s">
         <v>76</v>
       </c>
@@ -3542,8 +3772,11 @@
       <c r="K78" s="15">
         <v>3.6228878002205098</v>
       </c>
-    </row>
-    <row r="79" spans="1:11">
+      <c r="L78" s="15">
+        <v>1.546907963</v>
+      </c>
+    </row>
+    <row r="79" spans="1:12">
       <c r="A79" s="8" t="s">
         <v>77</v>
       </c>
@@ -3578,8 +3811,11 @@
       <c r="K79" s="15">
         <v>45.1352114924182</v>
       </c>
-    </row>
-    <row r="80" spans="1:11">
+      <c r="L79" s="15">
+        <v>4.5945722770000001</v>
+      </c>
+    </row>
+    <row r="80" spans="1:12">
       <c r="A80" s="8" t="s">
         <v>78</v>
       </c>
@@ -3614,8 +3850,11 @@
       <c r="K80" s="15">
         <v>231.44749034749</v>
       </c>
-    </row>
-    <row r="81" spans="1:11">
+      <c r="L80" s="15">
+        <v>2.3455869890000001</v>
+      </c>
+    </row>
+    <row r="81" spans="1:12">
       <c r="A81" s="8" t="s">
         <v>79</v>
       </c>
@@ -3644,8 +3883,11 @@
       <c r="K81" s="15">
         <v>82.599524187153094</v>
       </c>
-    </row>
-    <row r="82" spans="1:11">
+      <c r="L81" s="15">
+        <v>2.269450236</v>
+      </c>
+    </row>
+    <row r="82" spans="1:12">
       <c r="A82" s="8" t="s">
         <v>80</v>
       </c>
@@ -3674,8 +3916,11 @@
       <c r="K82" s="15">
         <v>43.951349260914398</v>
       </c>
-    </row>
-    <row r="83" spans="1:11">
+      <c r="L82" s="15">
+        <v>1.9295615370000001</v>
+      </c>
+    </row>
+    <row r="83" spans="1:12">
       <c r="A83" s="8" t="s">
         <v>81</v>
       </c>
@@ -3706,8 +3951,11 @@
       <c r="K83" s="15">
         <v>197.519134493</v>
       </c>
-    </row>
-    <row r="84" spans="1:11">
+      <c r="L83" s="15">
+        <v>2.0067722699999999</v>
+      </c>
+    </row>
+    <row r="84" spans="1:12">
       <c r="A84" s="8" t="s">
         <v>82</v>
       </c>
@@ -3738,8 +3986,11 @@
       <c r="K84" s="15">
         <v>15.195977675607899</v>
       </c>
-    </row>
-    <row r="85" spans="1:11">
+      <c r="L84" s="15">
+        <v>1.5667934619999999</v>
+      </c>
+    </row>
+    <row r="85" spans="1:12">
       <c r="A85" s="8" t="s">
         <v>83</v>
       </c>
@@ -3774,8 +4025,11 @@
       <c r="K85" s="15">
         <v>1454.0374999999999</v>
       </c>
-    </row>
-    <row r="86" spans="1:11">
+      <c r="L85" s="15">
+        <v>1.9806688539999999</v>
+      </c>
+    </row>
+    <row r="86" spans="1:12">
       <c r="A86" s="8" t="s">
         <v>84</v>
       </c>
@@ -3804,8 +4058,11 @@
       <c r="K86" s="15">
         <v>4.2885262442999901</v>
       </c>
-    </row>
-    <row r="87" spans="1:11">
+      <c r="L86" s="15">
+        <v>1.6035010940000001</v>
+      </c>
+    </row>
+    <row r="87" spans="1:12">
       <c r="A87" s="8" t="s">
         <v>85</v>
       </c>
@@ -3837,8 +4094,11 @@
       <c r="K87" s="15">
         <v>622.96206896551701</v>
       </c>
-    </row>
-    <row r="88" spans="1:11">
+      <c r="L87" s="15">
+        <v>1.831791645</v>
+      </c>
+    </row>
+    <row r="88" spans="1:12">
       <c r="A88" s="8" t="s">
         <v>86</v>
       </c>
@@ -3873,8 +4133,11 @@
       <c r="K88" s="15">
         <v>66.443723346793902</v>
       </c>
-    </row>
-    <row r="89" spans="1:11">
+      <c r="L88" s="15">
+        <v>2.1725092840000002</v>
+      </c>
+    </row>
+    <row r="89" spans="1:12">
       <c r="A89" s="8" t="s">
         <v>87</v>
       </c>
@@ -3909,8 +4172,11 @@
       <c r="K89" s="15">
         <v>123.654509353119</v>
       </c>
-    </row>
-    <row r="90" spans="1:11">
+      <c r="L89" s="15">
+        <v>4.3550731010000003</v>
+      </c>
+    </row>
+    <row r="90" spans="1:12">
       <c r="A90" s="8" t="s">
         <v>88</v>
       </c>
@@ -3938,8 +4204,11 @@
       <c r="K90" s="15">
         <v>1.9797413682123599</v>
       </c>
-    </row>
-    <row r="91" spans="1:11">
+      <c r="L90" s="15">
+        <v>4.1221787049999996</v>
+      </c>
+    </row>
+    <row r="91" spans="1:12">
       <c r="A91" s="8" t="s">
         <v>89</v>
       </c>
@@ -3974,8 +4243,11 @@
       <c r="K91" s="15">
         <v>46.280371747211902</v>
       </c>
-    </row>
-    <row r="92" spans="1:11">
+      <c r="L91" s="15">
+        <v>2.471931482</v>
+      </c>
+    </row>
+    <row r="92" spans="1:12">
       <c r="A92" s="8" t="s">
         <v>90</v>
       </c>
@@ -4006,8 +4278,11 @@
       <c r="K92" s="15">
         <v>80.079722159982097</v>
       </c>
-    </row>
-    <row r="93" spans="1:11">
+      <c r="L92" s="15">
+        <v>1.3015604540000001</v>
+      </c>
+    </row>
+    <row r="93" spans="1:12">
       <c r="A93" s="8" t="s">
         <v>91</v>
       </c>
@@ -4038,8 +4313,11 @@
       <c r="K93" s="15">
         <v>37.728367964597297</v>
       </c>
-    </row>
-    <row r="94" spans="1:11">
+      <c r="L93" s="15">
+        <v>1.960396129</v>
+      </c>
+    </row>
+    <row r="94" spans="1:12">
       <c r="A94" s="8" t="s">
         <v>92</v>
       </c>
@@ -4070,8 +4348,11 @@
       <c r="K94" s="15">
         <v>81.721395541128203</v>
       </c>
-    </row>
-    <row r="95" spans="1:11">
+      <c r="L94" s="15">
+        <v>1.503220129</v>
+      </c>
+    </row>
+    <row r="95" spans="1:12">
       <c r="A95" s="8" t="s">
         <v>93</v>
       </c>
@@ -4102,8 +4383,11 @@
       <c r="K95" s="15">
         <v>3.0776445723863999</v>
       </c>
-    </row>
-    <row r="96" spans="1:11">
+      <c r="L95" s="15">
+        <v>2.2975601029999999</v>
+      </c>
+    </row>
+    <row r="96" spans="1:12">
       <c r="A96" s="8" t="s">
         <v>94</v>
       </c>
@@ -4134,8 +4418,11 @@
       <c r="K96" s="15">
         <v>204.42970352284601</v>
       </c>
-    </row>
-    <row r="97" spans="1:11">
+      <c r="L96" s="15">
+        <v>2.0671706080000001</v>
+      </c>
+    </row>
+    <row r="97" spans="1:12">
       <c r="A97" s="8" t="s">
         <v>95</v>
       </c>
@@ -4166,8 +4453,11 @@
       <c r="K97" s="15">
         <v>508.544197091125</v>
       </c>
-    </row>
-    <row r="98" spans="1:11">
+      <c r="L97" s="15">
+        <v>1.8695020659999999</v>
+      </c>
+    </row>
+    <row r="98" spans="1:12">
       <c r="A98" s="8" t="s">
         <v>96</v>
       </c>
@@ -4202,8 +4492,11 @@
       <c r="K98" s="15">
         <v>18.206296760472402</v>
       </c>
-    </row>
-    <row r="99" spans="1:11">
+      <c r="L98" s="15">
+        <v>3.7186145019999999</v>
+      </c>
+    </row>
+    <row r="99" spans="1:12">
       <c r="A99" s="8" t="s">
         <v>97</v>
       </c>
@@ -4230,8 +4523,11 @@
       <c r="K99" s="15">
         <v>51.666785773641401</v>
       </c>
-    </row>
-    <row r="100" spans="1:11">
+      <c r="L99" s="15">
+        <v>2.3588229690000002</v>
+      </c>
+    </row>
+    <row r="100" spans="1:12">
       <c r="A100" s="8" t="s">
         <v>98</v>
       </c>
@@ -4262,8 +4558,11 @@
       <c r="K100" s="15">
         <v>16.9553548590827</v>
       </c>
-    </row>
-    <row r="101" spans="1:11">
+      <c r="L100" s="15">
+        <v>1.559410481</v>
+      </c>
+    </row>
+    <row r="101" spans="1:12">
       <c r="A101" s="8" t="s">
         <v>99</v>
       </c>
@@ -4294,8 +4593,11 @@
       <c r="K101" s="15">
         <v>209.587833371762</v>
       </c>
-    </row>
-    <row r="102" spans="1:11">
+      <c r="L101" s="15">
+        <v>1.6105036260000001</v>
+      </c>
+    </row>
+    <row r="102" spans="1:12">
       <c r="A102" s="8" t="s">
         <v>100</v>
       </c>
@@ -4330,8 +4632,11 @@
       <c r="K102" s="15">
         <v>14.4621363742146</v>
       </c>
-    </row>
-    <row r="103" spans="1:11">
+      <c r="L102" s="15">
+        <v>2.8172961070000002</v>
+      </c>
+    </row>
+    <row r="103" spans="1:12">
       <c r="A103" s="8" t="s">
         <v>101</v>
       </c>
@@ -4362,8 +4667,11 @@
       <c r="K103" s="15">
         <v>255.57279343088399</v>
       </c>
-    </row>
-    <row r="104" spans="1:11">
+      <c r="L103" s="15">
+        <v>2.3859996830000001</v>
+      </c>
+    </row>
+    <row r="104" spans="1:12">
       <c r="A104" s="8" t="s">
         <v>102</v>
       </c>
@@ -4390,8 +4698,11 @@
       <c r="K104" s="15">
         <v>778.20215946843905</v>
       </c>
-    </row>
-    <row r="105" spans="1:11">
+      <c r="L104" s="15">
+        <v>1.651153146</v>
+      </c>
+    </row>
+    <row r="105" spans="1:12">
       <c r="A105" s="8" t="s">
         <v>103</v>
       </c>
@@ -4422,8 +4733,11 @@
       <c r="K105" s="15">
         <v>55.132997040624197</v>
       </c>
-    </row>
-    <row r="106" spans="1:11">
+      <c r="L105" s="15">
+        <v>1.9408513249999999</v>
+      </c>
+    </row>
+    <row r="106" spans="1:12">
       <c r="A106" s="8" t="s">
         <v>104</v>
       </c>
@@ -4454,8 +4768,11 @@
       <c r="K106" s="15">
         <v>17.1439642587465</v>
       </c>
-    </row>
-    <row r="107" spans="1:11">
+      <c r="L106" s="15">
+        <v>2.919371215</v>
+      </c>
+    </row>
+    <row r="107" spans="1:12">
       <c r="A107" s="8" t="s">
         <v>105</v>
       </c>
@@ -4486,8 +4803,11 @@
       <c r="K107" s="15">
         <v>25.129285156249999</v>
       </c>
-    </row>
-    <row r="108" spans="1:11">
+      <c r="L107" s="15">
+        <v>1.979901752</v>
+      </c>
+    </row>
+    <row r="108" spans="1:12">
       <c r="A108" s="8" t="s">
         <v>106</v>
       </c>
@@ -4518,8 +4838,11 @@
       <c r="K108" s="15">
         <v>351.873394372338</v>
       </c>
-    </row>
-    <row r="109" spans="1:11">
+      <c r="L108" s="15">
+        <v>1.566442484</v>
+      </c>
+    </row>
+    <row r="109" spans="1:12">
       <c r="A109" s="8" t="s">
         <v>107</v>
       </c>
@@ -4554,8 +4877,11 @@
       <c r="K109" s="15">
         <v>124.027045298671</v>
       </c>
-    </row>
-    <row r="110" spans="1:11">
+      <c r="L109" s="15">
+        <v>2.7536132470000001</v>
+      </c>
+    </row>
+    <row r="110" spans="1:12">
       <c r="A110" s="8" t="s">
         <v>108</v>
       </c>
@@ -4590,8 +4916,11 @@
       <c r="K110" s="15">
         <v>112.37070028928601</v>
       </c>
-    </row>
-    <row r="111" spans="1:11">
+      <c r="L110" s="15">
+        <v>1.9087955809999999</v>
+      </c>
+    </row>
+    <row r="111" spans="1:12">
       <c r="A111" s="8" t="s">
         <v>109</v>
       </c>
@@ -4626,8 +4955,11 @@
       <c r="K111" s="15">
         <v>85.129255041724605</v>
       </c>
-    </row>
-    <row r="112" spans="1:11">
+      <c r="L111" s="15">
+        <v>2.0628492619999999</v>
+      </c>
+    </row>
+    <row r="112" spans="1:12">
       <c r="A112" s="8" t="s">
         <v>110</v>
       </c>
@@ -4662,8 +4994,11 @@
       <c r="K112" s="15">
         <v>8.8231172379093206</v>
       </c>
-    </row>
-    <row r="113" spans="1:11">
+      <c r="L112" s="15">
+        <v>5.9328232779999999</v>
+      </c>
+    </row>
+    <row r="113" spans="1:12">
       <c r="A113" s="8" t="s">
         <v>111</v>
       </c>
@@ -4694,8 +5029,11 @@
       <c r="K113" s="15">
         <v>494.86854479124401</v>
       </c>
-    </row>
-    <row r="114" spans="1:11">
+      <c r="L113" s="15">
+        <v>2.7858125299999998</v>
+      </c>
+    </row>
+    <row r="114" spans="1:12">
       <c r="A114" s="8" t="s">
         <v>112</v>
       </c>
@@ -4726,8 +5064,11 @@
       <c r="K114" s="15">
         <v>15.322308332829399</v>
       </c>
-    </row>
-    <row r="115" spans="1:11">
+      <c r="L114" s="15">
+        <v>1.4580674179999999</v>
+      </c>
+    </row>
+    <row r="115" spans="1:12">
       <c r="A115" s="8" t="s">
         <v>113</v>
       </c>
@@ -4758,8 +5099,11 @@
       <c r="K115" s="15">
         <v>82.327777489222498</v>
       </c>
-    </row>
-    <row r="116" spans="1:11">
+      <c r="L115" s="15">
+        <v>1.6261849719999999</v>
+      </c>
+    </row>
+    <row r="116" spans="1:12">
       <c r="A116" s="8" t="s">
         <v>114</v>
       </c>
@@ -4794,8 +5138,11 @@
       <c r="K116" s="15">
         <v>80.291195975302998</v>
       </c>
-    </row>
-    <row r="117" spans="1:11">
+      <c r="L116" s="15">
+        <v>2.3197503199999998</v>
+      </c>
+    </row>
+    <row r="117" spans="1:12">
       <c r="A117" s="8" t="s">
         <v>115</v>
       </c>
@@ -4821,8 +5168,11 @@
       <c r="K117" s="15">
         <v>104.699528955389</v>
       </c>
-    </row>
-    <row r="118" spans="1:11">
+      <c r="L117" s="15">
+        <v>1.6294331559999999</v>
+      </c>
+    </row>
+    <row r="118" spans="1:12">
       <c r="A118" s="8" t="s">
         <v>116</v>
       </c>
@@ -4857,8 +5207,11 @@
       <c r="K118" s="15">
         <v>7915.7306064880104</v>
       </c>
-    </row>
-    <row r="119" spans="1:11">
+      <c r="L118" s="15">
+        <v>1.530099412</v>
+      </c>
+    </row>
+    <row r="119" spans="1:12">
       <c r="A119" s="8" t="s">
         <v>117</v>
       </c>
@@ -4893,8 +5246,11 @@
       <c r="K119" s="15">
         <v>113.12839495903199</v>
       </c>
-    </row>
-    <row r="120" spans="1:11">
+      <c r="L119" s="15">
+        <v>2.992271423</v>
+      </c>
+    </row>
+    <row r="120" spans="1:12">
       <c r="A120" s="8" t="s">
         <v>118</v>
       </c>
@@ -4929,8 +5285,11 @@
       <c r="K120" s="15">
         <v>102.61906653426</v>
       </c>
-    </row>
-    <row r="121" spans="1:11">
+      <c r="L120" s="15">
+        <v>2.8881774459999998</v>
+      </c>
+    </row>
+    <row r="121" spans="1:12">
       <c r="A121" s="8" t="s">
         <v>119</v>
       </c>
@@ -4965,8 +5324,11 @@
       <c r="K121" s="15">
         <v>46.754285337444003</v>
       </c>
-    </row>
-    <row r="122" spans="1:11">
+      <c r="L121" s="15">
+        <v>2.1691135539999999</v>
+      </c>
+    </row>
+    <row r="122" spans="1:12">
       <c r="A122" s="8" t="s">
         <v>120</v>
       </c>
@@ -5001,8 +5363,11 @@
       <c r="K122" s="15">
         <v>527.96677267131702</v>
       </c>
-    </row>
-    <row r="123" spans="1:11">
+      <c r="L122" s="15">
+        <v>3.1578342109999999</v>
+      </c>
+    </row>
+    <row r="123" spans="1:12">
       <c r="A123" s="8" t="s">
         <v>121</v>
       </c>
@@ -5026,8 +5391,11 @@
         <v>3.7</v>
       </c>
       <c r="K123" s="15"/>
-    </row>
-    <row r="124" spans="1:11">
+      <c r="L123" s="15">
+        <v>1.9170053039999999</v>
+      </c>
+    </row>
+    <row r="124" spans="1:12">
       <c r="A124" s="8" t="s">
         <v>122</v>
       </c>
@@ -5062,8 +5430,11 @@
       <c r="K124" s="15">
         <v>93.1049519201935</v>
       </c>
-    </row>
-    <row r="125" spans="1:11">
+      <c r="L124" s="15">
+        <v>2.2706885099999998</v>
+      </c>
+    </row>
+    <row r="125" spans="1:12">
       <c r="A125" s="8" t="s">
         <v>123</v>
       </c>
@@ -5094,8 +5465,11 @@
       <c r="K125" s="15">
         <v>341.95503109551902</v>
       </c>
-    </row>
-    <row r="126" spans="1:11">
+      <c r="L125" s="15">
+        <v>1.5497655269999999</v>
+      </c>
+    </row>
+    <row r="126" spans="1:12">
       <c r="A126" s="8" t="s">
         <v>124</v>
       </c>
@@ -5126,8 +5500,11 @@
       <c r="K126" s="15">
         <v>24.717645036949701</v>
       </c>
-    </row>
-    <row r="127" spans="1:11">
+      <c r="L126" s="15">
+        <v>2.4664065709999998</v>
+      </c>
+    </row>
+    <row r="127" spans="1:12">
       <c r="A127" s="8" t="s">
         <v>125</v>
       </c>
@@ -5162,8 +5539,11 @@
       <c r="K127" s="15">
         <v>214.242762425347</v>
       </c>
-    </row>
-    <row r="128" spans="1:11">
+      <c r="L127" s="15">
+        <v>2.396185547</v>
+      </c>
+    </row>
+    <row r="128" spans="1:12">
       <c r="A128" s="8" t="s">
         <v>126</v>
       </c>
@@ -5188,8 +5568,11 @@
       </c>
       <c r="J128" s="6"/>
       <c r="K128" s="15"/>
-    </row>
-    <row r="129" spans="1:11">
+      <c r="L128" s="15">
+        <v>1.979137336</v>
+      </c>
+    </row>
+    <row r="129" spans="1:12">
       <c r="A129" s="8" t="s">
         <v>127</v>
       </c>
@@ -5218,8 +5601,11 @@
       <c r="K129" s="15">
         <v>64.281289179023801</v>
       </c>
-    </row>
-    <row r="130" spans="1:11">
+      <c r="L129" s="15">
+        <v>2.5833153879999999</v>
+      </c>
+    </row>
+    <row r="130" spans="1:12">
       <c r="A130" s="8" t="s">
         <v>128</v>
       </c>
@@ -5250,8 +5636,11 @@
       <c r="K130" s="15">
         <v>64.698599006547795</v>
       </c>
-    </row>
-    <row r="131" spans="1:11">
+      <c r="L130" s="15">
+        <v>2.0172102519999999</v>
+      </c>
+    </row>
+    <row r="131" spans="1:12">
       <c r="A131" s="8" t="s">
         <v>129</v>
       </c>
@@ -5286,8 +5675,11 @@
       <c r="K131" s="15">
         <v>135.13185421519299</v>
       </c>
-    </row>
-    <row r="132" spans="1:11">
+      <c r="L131" s="15">
+        <v>1.7415079250000001</v>
+      </c>
+    </row>
+    <row r="132" spans="1:12">
       <c r="A132" s="8" t="s">
         <v>130</v>
       </c>
@@ -5318,8 +5710,11 @@
       <c r="K132" s="15">
         <v>143.36631733774601</v>
       </c>
-    </row>
-    <row r="133" spans="1:11">
+      <c r="L132" s="15">
+        <v>1.660319265</v>
+      </c>
+    </row>
+    <row r="133" spans="1:12">
       <c r="A133" s="8" t="s">
         <v>131</v>
       </c>
@@ -5348,8 +5743,11 @@
       <c r="K133" s="15">
         <v>266.885964912281</v>
       </c>
-    </row>
-    <row r="134" spans="1:11">
+      <c r="L133" s="15">
+        <v>2.3274293319999999</v>
+      </c>
+    </row>
+    <row r="134" spans="1:12">
       <c r="A134" s="8" t="s">
         <v>132</v>
       </c>
@@ -5380,8 +5778,11 @@
       <c r="K134" s="15">
         <v>74.228417868177104</v>
       </c>
-    </row>
-    <row r="135" spans="1:11">
+      <c r="L134" s="15">
+        <v>1.466407341</v>
+      </c>
+    </row>
+    <row r="135" spans="1:12">
       <c r="A135" s="8" t="s">
         <v>133</v>
       </c>
@@ -5412,8 +5813,11 @@
       <c r="K135" s="15">
         <v>104.914075594766</v>
       </c>
-    </row>
-    <row r="136" spans="1:11">
+      <c r="L135" s="15">
+        <v>1.7250975909999999</v>
+      </c>
+    </row>
+    <row r="136" spans="1:12">
       <c r="A136" s="8" t="s">
         <v>134</v>
       </c>
@@ -5442,8 +5846,11 @@
       <c r="K136" s="15">
         <v>12.2530483263465</v>
       </c>
-    </row>
-    <row r="137" spans="1:11">
+      <c r="L136" s="15">
+        <v>2.7327663169999998</v>
+      </c>
+    </row>
+    <row r="137" spans="1:12">
       <c r="A137" s="8" t="s">
         <v>135</v>
       </c>
@@ -5474,8 +5881,11 @@
       <c r="K137" s="15">
         <v>213.75901655695199</v>
       </c>
-    </row>
-    <row r="138" spans="1:11">
+      <c r="L137" s="15">
+        <v>1.7230074019999999</v>
+      </c>
+    </row>
+    <row r="138" spans="1:12">
       <c r="A138" s="8" t="s">
         <v>136</v>
       </c>
@@ -5506,8 +5916,11 @@
       <c r="K138" s="15">
         <v>77.389837559771493</v>
       </c>
-    </row>
-    <row r="139" spans="1:11">
+      <c r="L138" s="15">
+        <v>5.1017697169999998</v>
+      </c>
+    </row>
+    <row r="139" spans="1:12">
       <c r="A139" s="8" t="s">
         <v>137</v>
       </c>
@@ -5538,8 +5951,11 @@
       <c r="K139" s="15">
         <v>112.44192583732099</v>
       </c>
-    </row>
-    <row r="140" spans="1:11">
+      <c r="L139" s="15">
+        <v>1.751084868</v>
+      </c>
+    </row>
+    <row r="140" spans="1:12">
       <c r="A140" s="8" t="s">
         <v>138</v>
       </c>
@@ -5574,8 +5990,11 @@
       <c r="K140" s="15">
         <v>272.89824742694202</v>
       </c>
-    </row>
-    <row r="141" spans="1:11">
+      <c r="L140" s="15">
+        <v>2.8989730470000001</v>
+      </c>
+    </row>
+    <row r="141" spans="1:12">
       <c r="A141" s="8" t="s">
         <v>139</v>
       </c>
@@ -5606,8 +6025,11 @@
       <c r="K141" s="15">
         <v>35.607764593732398</v>
       </c>
-    </row>
-    <row r="142" spans="1:11">
+      <c r="L141" s="15">
+        <v>5.4680782109999999</v>
+      </c>
+    </row>
+    <row r="142" spans="1:12">
       <c r="A142" s="8" t="s">
         <v>140</v>
       </c>
@@ -5642,8 +6064,11 @@
       <c r="K142" s="15">
         <v>19.750599931436401</v>
       </c>
-    </row>
-    <row r="143" spans="1:11">
+      <c r="L142" s="15">
+        <v>2.0612895770000002</v>
+      </c>
+    </row>
+    <row r="143" spans="1:12">
       <c r="A143" s="8" t="s">
         <v>141</v>
       </c>
@@ -5674,8 +6099,11 @@
       <c r="K143" s="15">
         <v>76.133521391631405</v>
       </c>
-    </row>
-    <row r="144" spans="1:11">
+      <c r="L143" s="15">
+        <v>2.3188884989999998</v>
+      </c>
+    </row>
+    <row r="144" spans="1:12">
       <c r="A144" s="8" t="s">
         <v>142</v>
       </c>
@@ -5704,8 +6132,11 @@
       <c r="K144" s="15">
         <v>36.253120571396202</v>
       </c>
-    </row>
-    <row r="145" spans="1:11">
+      <c r="L144" s="15">
+        <v>1.878402629</v>
+      </c>
+    </row>
+    <row r="145" spans="1:12">
       <c r="A145" s="8" t="s">
         <v>143</v>
       </c>
@@ -5736,8 +6167,11 @@
       <c r="K145" s="15">
         <v>308.12655206888797</v>
       </c>
-    </row>
-    <row r="146" spans="1:11">
+      <c r="L145" s="15">
+        <v>2.3690779389999999</v>
+      </c>
+    </row>
+    <row r="146" spans="1:12">
       <c r="A146" s="8" t="s">
         <v>144</v>
       </c>
@@ -5766,8 +6200,11 @@
       <c r="K146" s="15">
         <v>53.507623539216198</v>
       </c>
-    </row>
-    <row r="147" spans="1:11">
+      <c r="L146" s="15">
+        <v>1.404976709</v>
+      </c>
+    </row>
+    <row r="147" spans="1:12">
       <c r="A147" s="8" t="s">
         <v>145</v>
       </c>
@@ -5796,8 +6233,11 @@
       <c r="K147" s="15">
         <v>22.9948344745019</v>
       </c>
-    </row>
-    <row r="148" spans="1:11">
+      <c r="L147" s="15">
+        <v>2.1439141730000002</v>
+      </c>
+    </row>
+    <row r="148" spans="1:12">
       <c r="A148" s="8" t="s">
         <v>146</v>
       </c>
@@ -5828,6 +6268,9 @@
       <c r="K148" s="15">
         <v>42.729492051182604</v>
       </c>
+      <c r="L148" s="15">
+        <v>2.3203841710000002</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
added tax gdp data
</commit_message>
<xml_diff>
--- a/data_tables/Total_data_cleaned.xlsx
+++ b/data_tables/Total_data_cleaned.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ulrikaeriksson/Documents/Data_Mining/DataMining-Group23/data_tables/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8C4AE9E6-1175-B548-8A4C-4A95053398D3}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9B0F17D3-C707-FC40-BC31-8DA5D132607E}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="22200" windowHeight="12560" xr2:uid="{196242FC-4F62-234C-ABAE-90D7B6224D3F}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="159" uniqueCount="159">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="160" uniqueCount="160">
   <si>
     <t>Afghanistan</t>
   </si>
@@ -502,6 +502,9 @@
   </si>
   <si>
     <t>Alcohol or drug use disorder</t>
+  </si>
+  <si>
+    <t>Total Taxes (% GDP)</t>
   </si>
 </sst>
 </file>
@@ -970,10 +973,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{67CF83BE-F021-5E44-A4B8-2C5D9BB127DA}">
-  <dimension ref="A1:L148"/>
+  <dimension ref="A1:M148"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A24" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="H16" sqref="H16"/>
+    <sheetView tabSelected="1" topLeftCell="A124" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="F144" sqref="F144"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="16"/>
@@ -989,7 +992,7 @@
     <col min="9" max="9" width="14.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" ht="17">
+    <row r="1" spans="1:13" ht="17">
       <c r="A1" s="1" t="s">
         <v>147</v>
       </c>
@@ -1026,8 +1029,11 @@
       <c r="L1" s="16" t="s">
         <v>158</v>
       </c>
-    </row>
-    <row r="2" spans="1:12">
+      <c r="M1" s="16" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13">
       <c r="A2" s="8" t="s">
         <v>0</v>
       </c>
@@ -1058,8 +1064,11 @@
       <c r="L2" s="15">
         <v>1.809624516</v>
       </c>
-    </row>
-    <row r="3" spans="1:12">
+      <c r="M2" s="15">
+        <v>9.1248640000000005</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13">
       <c r="A3" s="8" t="s">
         <v>1</v>
       </c>
@@ -1093,8 +1102,11 @@
       <c r="L3" s="15">
         <v>2.3255375310000002</v>
       </c>
-    </row>
-    <row r="4" spans="1:12">
+      <c r="M3" s="15">
+        <v>23.52533</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13">
       <c r="A4" s="8" t="s">
         <v>2</v>
       </c>
@@ -1128,8 +1140,11 @@
       <c r="L4" s="15">
         <v>1.485914602</v>
       </c>
-    </row>
-    <row r="5" spans="1:12">
+      <c r="M4" s="15">
+        <v>14.162544</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13">
       <c r="A5" s="8" t="s">
         <v>3</v>
       </c>
@@ -1167,8 +1182,11 @@
       <c r="L5" s="15">
         <v>3.1186833850000002</v>
       </c>
-    </row>
-    <row r="6" spans="1:12">
+      <c r="M5" s="15">
+        <v>30.661214999999999</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13">
       <c r="A6" s="8" t="s">
         <v>4</v>
       </c>
@@ -1202,8 +1220,11 @@
       <c r="L6" s="15">
         <v>2.3654491160000002</v>
       </c>
-    </row>
-    <row r="7" spans="1:12">
+      <c r="M6" s="15">
+        <v>21.761512</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13">
       <c r="A7" s="8" t="s">
         <v>5</v>
       </c>
@@ -1241,8 +1262,11 @@
       <c r="L7" s="15">
         <v>3.8037627660000002</v>
       </c>
-    </row>
-    <row r="8" spans="1:12">
+      <c r="M7" s="15">
+        <v>28.578520000000001</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13">
       <c r="A8" s="8" t="s">
         <v>6</v>
       </c>
@@ -1280,8 +1304,11 @@
       <c r="L8" s="15">
         <v>2.8291145819999999</v>
       </c>
-    </row>
-    <row r="9" spans="1:12">
+      <c r="M8" s="15">
+        <v>41.884256999999998</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13">
       <c r="A9" s="8" t="s">
         <v>7</v>
       </c>
@@ -1319,8 +1346,11 @@
       <c r="L9" s="15">
         <v>3.2560069280000001</v>
       </c>
-    </row>
-    <row r="10" spans="1:12">
+      <c r="M9" s="15">
+        <v>16.506067999999999</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13">
       <c r="A10" s="8" t="s">
         <v>8</v>
       </c>
@@ -1352,8 +1382,11 @@
       <c r="L10" s="15">
         <v>1.615647681</v>
       </c>
-    </row>
-    <row r="11" spans="1:12">
+      <c r="M10" s="15">
+        <v>1.0698810000000001</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13">
       <c r="A11" s="8" t="s">
         <v>9</v>
       </c>
@@ -1387,8 +1420,11 @@
       <c r="L11" s="15">
         <v>2.031842132</v>
       </c>
-    </row>
-    <row r="12" spans="1:12">
+      <c r="M11" s="15">
+        <v>8.1908390000000004</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13">
       <c r="A12" s="8" t="s">
         <v>10</v>
       </c>
@@ -1426,8 +1462,11 @@
       <c r="L12" s="15">
         <v>5.1028469349999996</v>
       </c>
-    </row>
-    <row r="13" spans="1:12">
+      <c r="M12" s="15">
+        <v>35.748614000000003</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13">
       <c r="A13" s="8" t="s">
         <v>11</v>
       </c>
@@ -1465,8 +1504,11 @@
       <c r="L13" s="15">
         <v>2.2844173109999999</v>
       </c>
-    </row>
-    <row r="14" spans="1:12">
+      <c r="M13" s="15">
+        <v>43.875816</v>
+      </c>
+    </row>
+    <row r="14" spans="1:13">
       <c r="A14" s="8" t="s">
         <v>12</v>
       </c>
@@ -1500,8 +1542,11 @@
       <c r="L14" s="15">
         <v>1.6706470899999999</v>
       </c>
-    </row>
-    <row r="15" spans="1:12">
+      <c r="M14" s="15">
+        <v>15.888945</v>
+      </c>
+    </row>
+    <row r="15" spans="1:13">
       <c r="A15" s="8" t="s">
         <v>13</v>
       </c>
@@ -1537,8 +1582,11 @@
       <c r="L15" s="15">
         <v>2.434164628</v>
       </c>
-    </row>
-    <row r="16" spans="1:12">
+      <c r="M15" s="15">
+        <v>26.203921000000001</v>
+      </c>
+    </row>
+    <row r="16" spans="1:13">
       <c r="A16" s="8" t="s">
         <v>14</v>
       </c>
@@ -1572,8 +1620,11 @@
       <c r="L16" s="15">
         <v>3.526306038</v>
       </c>
-    </row>
-    <row r="17" spans="1:12">
+      <c r="M16" s="15">
+        <v>37.572918999999999</v>
+      </c>
+    </row>
+    <row r="17" spans="1:13">
       <c r="A17" s="8" t="s">
         <v>15</v>
       </c>
@@ -1607,8 +1658,11 @@
       <c r="L17" s="15">
         <v>2.3786810370000002</v>
       </c>
-    </row>
-    <row r="18" spans="1:12">
+      <c r="M17" s="15">
+        <v>20.871931</v>
+      </c>
+    </row>
+    <row r="18" spans="1:13">
       <c r="A18" s="8" t="s">
         <v>16</v>
       </c>
@@ -1646,8 +1700,11 @@
       <c r="L18" s="15">
         <v>3.730609555</v>
       </c>
-    </row>
-    <row r="19" spans="1:12">
+      <c r="M18" s="15">
+        <v>33.713017999999998</v>
+      </c>
+    </row>
+    <row r="19" spans="1:13">
       <c r="A19" s="8" t="s">
         <v>17</v>
       </c>
@@ -1685,8 +1742,11 @@
       <c r="L19" s="15">
         <v>2.3871194039999999</v>
       </c>
-    </row>
-    <row r="20" spans="1:12">
+      <c r="M19" s="15">
+        <v>28.800666</v>
+      </c>
+    </row>
+    <row r="20" spans="1:13">
       <c r="A20" s="8" t="s">
         <v>18</v>
       </c>
@@ -1724,8 +1784,11 @@
       <c r="L20" s="15">
         <v>1.6203995840000001</v>
       </c>
-    </row>
-    <row r="21" spans="1:12">
+      <c r="M20" s="15">
+        <v>16.652574000000001</v>
+      </c>
+    </row>
+    <row r="21" spans="1:13">
       <c r="A21" s="8" t="s">
         <v>19</v>
       </c>
@@ -1759,8 +1822,11 @@
       <c r="L21" s="15">
         <v>1.5939582269999999</v>
       </c>
-    </row>
-    <row r="22" spans="1:12">
+      <c r="M21" s="15">
+        <v>14.825889999999999</v>
+      </c>
+    </row>
+    <row r="22" spans="1:13">
       <c r="A22" s="8" t="s">
         <v>20</v>
       </c>
@@ -1792,8 +1858,11 @@
       <c r="L22" s="15">
         <v>1.8031018350000001</v>
       </c>
-    </row>
-    <row r="23" spans="1:12">
+      <c r="M22" s="15">
+        <v>13.376192</v>
+      </c>
+    </row>
+    <row r="23" spans="1:13">
       <c r="A23" s="8" t="s">
         <v>21</v>
       </c>
@@ -1831,8 +1900,11 @@
       <c r="L23" s="15">
         <v>3.7945346299999998</v>
       </c>
-    </row>
-    <row r="24" spans="1:12">
+      <c r="M23" s="15">
+        <v>32.830274000000003</v>
+      </c>
+    </row>
+    <row r="24" spans="1:13">
       <c r="A24" s="8" t="s">
         <v>22</v>
       </c>
@@ -1864,8 +1936,11 @@
       <c r="L24" s="15">
         <v>1.8895983300000001</v>
       </c>
-    </row>
-    <row r="25" spans="1:12">
+      <c r="M24" s="15">
+        <v>9.6534659999999999</v>
+      </c>
+    </row>
+    <row r="25" spans="1:13">
       <c r="A25" s="8" t="s">
         <v>23</v>
       </c>
@@ -1897,8 +1972,11 @@
       <c r="L25" s="15">
         <v>1.612914776</v>
       </c>
-    </row>
-    <row r="26" spans="1:12">
+      <c r="M25" s="15">
+        <v>5.6650309999999999</v>
+      </c>
+    </row>
+    <row r="26" spans="1:13">
       <c r="A26" s="8" t="s">
         <v>24</v>
       </c>
@@ -1932,8 +2010,11 @@
       <c r="L26" s="15">
         <v>3.461463626</v>
       </c>
-    </row>
-    <row r="27" spans="1:12">
+      <c r="M26" s="15">
+        <v>17.409112</v>
+      </c>
+    </row>
+    <row r="27" spans="1:13">
       <c r="A27" s="8" t="s">
         <v>25</v>
       </c>
@@ -1968,8 +2049,11 @@
       <c r="L27" s="15">
         <v>1.9578983599999999</v>
       </c>
-    </row>
-    <row r="28" spans="1:12">
+      <c r="M27" s="15">
+        <v>23.790354000000001</v>
+      </c>
+    </row>
+    <row r="28" spans="1:13">
       <c r="A28" s="8" t="s">
         <v>26</v>
       </c>
@@ -2007,8 +2091,11 @@
       <c r="L28" s="15">
         <v>2.3728377520000001</v>
       </c>
-    </row>
-    <row r="29" spans="1:12">
+      <c r="M28" s="15">
+        <v>19.211746000000002</v>
+      </c>
+    </row>
+    <row r="29" spans="1:13">
       <c r="A29" s="8" t="s">
         <v>27</v>
       </c>
@@ -2039,8 +2126,11 @@
       <c r="L29" s="15">
         <v>1.9430276660000001</v>
       </c>
-    </row>
-    <row r="30" spans="1:12">
+      <c r="M29" s="15">
+        <v>17.503682999999999</v>
+      </c>
+    </row>
+    <row r="30" spans="1:13">
       <c r="A30" s="8" t="s">
         <v>28</v>
       </c>
@@ -2072,8 +2162,11 @@
       <c r="L30" s="15">
         <v>1.8587189340000001</v>
       </c>
-    </row>
-    <row r="31" spans="1:12">
+      <c r="M30" s="15">
+        <v>7.1134009999999996</v>
+      </c>
+    </row>
+    <row r="31" spans="1:13">
       <c r="A31" s="8" t="s">
         <v>29</v>
       </c>
@@ -2111,8 +2204,11 @@
       <c r="L31" s="15">
         <v>1.9148140069999999</v>
       </c>
-    </row>
-    <row r="32" spans="1:12">
+      <c r="M31" s="15">
+        <v>13.854123</v>
+      </c>
+    </row>
+    <row r="32" spans="1:13">
       <c r="A32" s="8" t="s">
         <v>30</v>
       </c>
@@ -2150,8 +2246,11 @@
       <c r="L32" s="15">
         <v>2.7405460929999998</v>
       </c>
-    </row>
-    <row r="33" spans="1:12">
+      <c r="M32" s="15">
+        <v>35.163044999999997</v>
+      </c>
+    </row>
+    <row r="33" spans="1:13">
       <c r="A33" s="8" t="s">
         <v>31</v>
       </c>
@@ -2189,8 +2288,11 @@
       <c r="L33" s="15">
         <v>1.7680723469999999</v>
       </c>
-    </row>
-    <row r="34" spans="1:12">
+      <c r="M33" s="15">
+        <v>23.997837000000001</v>
+      </c>
+    </row>
+    <row r="34" spans="1:13">
       <c r="A34" s="8" t="s">
         <v>32</v>
       </c>
@@ -2224,8 +2326,11 @@
       <c r="L34" s="15">
         <v>2.7127169690000001</v>
       </c>
-    </row>
-    <row r="35" spans="1:12">
+      <c r="M34" s="15">
+        <v>34.068710000000003</v>
+      </c>
+    </row>
+    <row r="35" spans="1:13">
       <c r="A35" s="8" t="s">
         <v>33</v>
       </c>
@@ -2259,8 +2364,11 @@
       <c r="L35" s="15">
         <v>2.8271041879999999</v>
       </c>
-    </row>
-    <row r="36" spans="1:12">
+      <c r="M35" s="15">
+        <v>45.43515</v>
+      </c>
+    </row>
+    <row r="36" spans="1:13">
       <c r="A36" s="8" t="s">
         <v>34</v>
       </c>
@@ -2298,8 +2406,11 @@
       <c r="L36" s="15">
         <v>2.1777191999999999</v>
       </c>
-    </row>
-    <row r="37" spans="1:12">
+      <c r="M36" s="15">
+        <v>13.509418</v>
+      </c>
+    </row>
+    <row r="37" spans="1:13">
       <c r="A37" s="8" t="s">
         <v>35</v>
       </c>
@@ -2333,8 +2444,11 @@
       <c r="L37" s="15">
         <v>2.31497332</v>
       </c>
-    </row>
-    <row r="38" spans="1:12">
+      <c r="M37" s="15">
+        <v>14.671663000000001</v>
+      </c>
+    </row>
+    <row r="38" spans="1:13">
       <c r="A38" s="8" t="s">
         <v>36</v>
       </c>
@@ -2368,8 +2482,9 @@
       <c r="L38" s="15">
         <v>1.446643887</v>
       </c>
-    </row>
-    <row r="39" spans="1:12">
+      <c r="M38" s="15"/>
+    </row>
+    <row r="39" spans="1:13">
       <c r="A39" s="8" t="s">
         <v>37</v>
       </c>
@@ -2403,8 +2518,11 @@
       <c r="L39" s="15">
         <v>3.0883517739999999</v>
       </c>
-    </row>
-    <row r="40" spans="1:12">
+      <c r="M39" s="15">
+        <v>17.381668999999999</v>
+      </c>
+    </row>
+    <row r="40" spans="1:13">
       <c r="A40" s="8" t="s">
         <v>38</v>
       </c>
@@ -2442,8 +2560,11 @@
       <c r="L40" s="15">
         <v>5.4835234560000004</v>
       </c>
-    </row>
-    <row r="41" spans="1:12">
+      <c r="M40" s="15">
+        <v>33.730350999999999</v>
+      </c>
+    </row>
+    <row r="41" spans="1:13">
       <c r="A41" s="8" t="s">
         <v>39</v>
       </c>
@@ -2477,8 +2598,9 @@
       <c r="L41" s="15">
         <v>2.616682548</v>
       </c>
-    </row>
-    <row r="42" spans="1:12">
+      <c r="M41" s="15"/>
+    </row>
+    <row r="42" spans="1:13">
       <c r="A42" s="8" t="s">
         <v>40</v>
       </c>
@@ -2516,8 +2638,11 @@
       <c r="L42" s="15">
         <v>4.0242325509999999</v>
       </c>
-    </row>
-    <row r="43" spans="1:12">
+      <c r="M42" s="15">
+        <v>44.017195000000001</v>
+      </c>
+    </row>
+    <row r="43" spans="1:13">
       <c r="A43" s="8" t="s">
         <v>41</v>
       </c>
@@ -2555,8 +2680,11 @@
       <c r="L43" s="15">
         <v>2.7333169019999999</v>
       </c>
-    </row>
-    <row r="44" spans="1:12">
+      <c r="M43" s="15">
+        <v>45.277869000000003</v>
+      </c>
+    </row>
+    <row r="44" spans="1:13">
       <c r="A44" s="8" t="s">
         <v>42</v>
       </c>
@@ -2585,8 +2713,11 @@
       <c r="L44" s="15">
         <v>2.0146800420000002</v>
       </c>
-    </row>
-    <row r="45" spans="1:12">
+      <c r="M44" s="15">
+        <v>20.494221</v>
+      </c>
+    </row>
+    <row r="45" spans="1:13">
       <c r="A45" s="8" t="s">
         <v>43</v>
       </c>
@@ -2617,8 +2748,11 @@
       <c r="L45" s="15">
         <v>1.576080782</v>
       </c>
-    </row>
-    <row r="46" spans="1:12">
+      <c r="M45" s="15">
+        <v>11.14148</v>
+      </c>
+    </row>
+    <row r="46" spans="1:13">
       <c r="A46" s="8" t="s">
         <v>44</v>
       </c>
@@ -2656,8 +2790,11 @@
       <c r="L46" s="15">
         <v>2.4086422789999999</v>
       </c>
-    </row>
-    <row r="47" spans="1:12">
+      <c r="M46" s="15">
+        <v>25.819448000000001</v>
+      </c>
+    </row>
+    <row r="47" spans="1:13">
       <c r="A47" s="8" t="s">
         <v>45</v>
       </c>
@@ -2695,8 +2832,11 @@
       <c r="L47" s="15">
         <v>2.827630079</v>
       </c>
-    </row>
-    <row r="48" spans="1:12">
+      <c r="M47" s="15">
+        <v>37.430619999999998</v>
+      </c>
+    </row>
+    <row r="48" spans="1:13">
       <c r="A48" s="8" t="s">
         <v>46</v>
       </c>
@@ -2734,8 +2874,11 @@
       <c r="L48" s="15">
         <v>1.6884604519999999</v>
       </c>
-    </row>
-    <row r="49" spans="1:12">
+      <c r="M48" s="15">
+        <v>12.377316</v>
+      </c>
+    </row>
+    <row r="49" spans="1:13">
       <c r="A49" s="8" t="s">
         <v>47</v>
       </c>
@@ -2773,8 +2916,11 @@
       <c r="L49" s="15">
         <v>1.8782843119999999</v>
       </c>
-    </row>
-    <row r="50" spans="1:12">
+      <c r="M49" s="15">
+        <v>38.338583999999997</v>
+      </c>
+    </row>
+    <row r="50" spans="1:13">
       <c r="A50" s="8" t="s">
         <v>48</v>
       </c>
@@ -2806,8 +2952,11 @@
       <c r="L50" s="15">
         <v>3.162466411</v>
       </c>
-    </row>
-    <row r="51" spans="1:12">
+      <c r="M50" s="15">
+        <v>10.78232</v>
+      </c>
+    </row>
+    <row r="51" spans="1:13">
       <c r="A51" s="8" t="s">
         <v>49</v>
       </c>
@@ -2839,8 +2988,11 @@
       <c r="L51" s="15">
         <v>1.590701079</v>
       </c>
-    </row>
-    <row r="52" spans="1:12">
+      <c r="M51" s="15">
+        <v>14.030989</v>
+      </c>
+    </row>
+    <row r="52" spans="1:13">
       <c r="A52" s="8" t="s">
         <v>50</v>
       </c>
@@ -2872,8 +3024,11 @@
       <c r="L52" s="15">
         <v>2.334270047</v>
       </c>
-    </row>
-    <row r="53" spans="1:12">
+      <c r="M52" s="15">
+        <v>13.731528000000001</v>
+      </c>
+    </row>
+    <row r="53" spans="1:13">
       <c r="A53" s="8" t="s">
         <v>51</v>
       </c>
@@ -2907,8 +3062,11 @@
       <c r="L53" s="15">
         <v>2.1300707230000002</v>
       </c>
-    </row>
-    <row r="54" spans="1:12">
+      <c r="M53" s="15">
+        <v>22.421873000000001</v>
+      </c>
+    </row>
+    <row r="54" spans="1:13">
       <c r="A54" s="8" t="s">
         <v>52</v>
       </c>
@@ -2932,8 +3090,11 @@
         <v>7039.7142857142899</v>
       </c>
       <c r="L54" s="15"/>
-    </row>
-    <row r="55" spans="1:12">
+      <c r="M54" s="15">
+        <v>13.574933</v>
+      </c>
+    </row>
+    <row r="55" spans="1:13">
       <c r="A55" s="8" t="s">
         <v>53</v>
       </c>
@@ -2971,8 +3132,11 @@
       <c r="L55" s="15">
         <v>2.6101259950000002</v>
       </c>
-    </row>
-    <row r="56" spans="1:12">
+      <c r="M55" s="15">
+        <v>39.148890999999999</v>
+      </c>
+    </row>
+    <row r="56" spans="1:13">
       <c r="A56" s="8" t="s">
         <v>54</v>
       </c>
@@ -3003,8 +3167,11 @@
       <c r="L56" s="15">
         <v>2.1393359009999999</v>
       </c>
-    </row>
-    <row r="57" spans="1:12">
+      <c r="M56" s="15">
+        <v>36.789971000000001</v>
+      </c>
+    </row>
+    <row r="57" spans="1:13">
       <c r="A57" s="8" t="s">
         <v>55</v>
       </c>
@@ -3038,8 +3205,11 @@
       <c r="L57" s="15">
         <v>1.7448725620000001</v>
       </c>
-    </row>
-    <row r="58" spans="1:12">
+      <c r="M57" s="15">
+        <v>17.577255000000001</v>
+      </c>
+    </row>
+    <row r="58" spans="1:13">
       <c r="A58" s="8" t="s">
         <v>56</v>
       </c>
@@ -3073,8 +3243,11 @@
       <c r="L58" s="15">
         <v>1.2969102939999999</v>
       </c>
-    </row>
-    <row r="59" spans="1:12">
+      <c r="M58" s="15">
+        <v>10.361459</v>
+      </c>
+    </row>
+    <row r="59" spans="1:13">
       <c r="A59" s="8" t="s">
         <v>57</v>
       </c>
@@ -3108,8 +3281,11 @@
       <c r="L59" s="15">
         <v>1.7879851849999999</v>
       </c>
-    </row>
-    <row r="60" spans="1:12">
+      <c r="M59" s="15">
+        <v>7.9746290000000002</v>
+      </c>
+    </row>
+    <row r="60" spans="1:13">
       <c r="A60" s="8" t="s">
         <v>58</v>
       </c>
@@ -3141,8 +3317,11 @@
       <c r="L60" s="15">
         <v>2.1814031009999999</v>
       </c>
-    </row>
-    <row r="61" spans="1:12">
+      <c r="M60" s="15">
+        <v>1.3778090000000001</v>
+      </c>
+    </row>
+    <row r="61" spans="1:13">
       <c r="A61" s="8" t="s">
         <v>59</v>
       </c>
@@ -3180,8 +3359,11 @@
       <c r="L61" s="15">
         <v>3.2364014619999999</v>
       </c>
-    </row>
-    <row r="62" spans="1:12">
+      <c r="M61" s="15">
+        <v>23.358557999999999</v>
+      </c>
+    </row>
+    <row r="62" spans="1:13">
       <c r="A62" s="8" t="s">
         <v>60</v>
       </c>
@@ -3219,8 +3401,11 @@
       <c r="L62" s="15">
         <v>1.3260031560000001</v>
       </c>
-    </row>
-    <row r="63" spans="1:12">
+      <c r="M62" s="15">
+        <v>31.128926</v>
+      </c>
+    </row>
+    <row r="63" spans="1:13">
       <c r="A63" s="8" t="s">
         <v>61</v>
       </c>
@@ -3258,8 +3443,11 @@
       <c r="L63" s="15">
         <v>1.683797108</v>
       </c>
-    </row>
-    <row r="64" spans="1:12">
+      <c r="M63" s="15">
+        <v>42.385586000000004</v>
+      </c>
+    </row>
+    <row r="64" spans="1:13">
       <c r="A64" s="8" t="s">
         <v>62</v>
       </c>
@@ -3291,8 +3479,11 @@
       <c r="L64" s="15">
         <v>1.720200808</v>
       </c>
-    </row>
-    <row r="65" spans="1:12">
+      <c r="M64" s="15">
+        <v>16.017084000000001</v>
+      </c>
+    </row>
+    <row r="65" spans="1:13">
       <c r="A65" s="8" t="s">
         <v>63</v>
       </c>
@@ -3330,8 +3521,11 @@
       <c r="L65" s="15">
         <v>2.3290716069999999</v>
       </c>
-    </row>
-    <row r="66" spans="1:12">
+      <c r="M65" s="15">
+        <v>25.114878999999998</v>
+      </c>
+    </row>
+    <row r="66" spans="1:13">
       <c r="A66" s="8" t="s">
         <v>64</v>
       </c>
@@ -3369,8 +3563,11 @@
       <c r="L66" s="15">
         <v>1.5638960449999999</v>
       </c>
-    </row>
-    <row r="67" spans="1:12">
+      <c r="M66" s="15">
+        <v>30.777436000000002</v>
+      </c>
+    </row>
+    <row r="67" spans="1:13">
       <c r="A67" s="8" t="s">
         <v>65</v>
       </c>
@@ -3402,8 +3599,11 @@
       <c r="L67" s="15">
         <v>1.61326719</v>
       </c>
-    </row>
-    <row r="68" spans="1:12">
+      <c r="M67" s="15">
+        <v>15.341718</v>
+      </c>
+    </row>
+    <row r="68" spans="1:13">
       <c r="A68" s="8" t="s">
         <v>66</v>
       </c>
@@ -3437,8 +3637,11 @@
       <c r="L68" s="15">
         <v>3.3750323070000001</v>
       </c>
-    </row>
-    <row r="69" spans="1:12">
+      <c r="M68" s="15">
+        <v>15.228497000000001</v>
+      </c>
+    </row>
+    <row r="69" spans="1:13">
       <c r="A69" s="8" t="s">
         <v>67</v>
       </c>
@@ -3472,8 +3675,11 @@
       <c r="L69" s="15">
         <v>1.5311732680000001</v>
       </c>
-    </row>
-    <row r="70" spans="1:12">
+      <c r="M69" s="15">
+        <v>15.800242000000001</v>
+      </c>
+    </row>
+    <row r="70" spans="1:13">
       <c r="A70" s="8" t="s">
         <v>68</v>
       </c>
@@ -3499,8 +3705,11 @@
         <v>168.154679893451</v>
       </c>
       <c r="L70" s="15"/>
-    </row>
-    <row r="71" spans="1:12">
+      <c r="M70" s="15">
+        <v>23.459638000000002</v>
+      </c>
+    </row>
+    <row r="71" spans="1:13">
       <c r="A71" s="8" t="s">
         <v>69</v>
       </c>
@@ -3534,8 +3743,11 @@
       <c r="L71" s="15">
         <v>1.5134735370000001</v>
       </c>
-    </row>
-    <row r="72" spans="1:12">
+      <c r="M71" s="15">
+        <v>1.5125850000000001</v>
+      </c>
+    </row>
+    <row r="72" spans="1:13">
       <c r="A72" s="8" t="s">
         <v>70</v>
       </c>
@@ -3569,8 +3781,11 @@
       <c r="L72" s="15">
         <v>3.336949615</v>
       </c>
-    </row>
-    <row r="73" spans="1:12">
+      <c r="M72" s="15">
+        <v>25.102250000000002</v>
+      </c>
+    </row>
+    <row r="73" spans="1:13">
       <c r="A73" s="8" t="s">
         <v>71</v>
       </c>
@@ -3604,8 +3819,11 @@
       <c r="L73" s="15">
         <v>1.6259996080000001</v>
       </c>
-    </row>
-    <row r="74" spans="1:12">
+      <c r="M73" s="15">
+        <v>12.428921000000001</v>
+      </c>
+    </row>
+    <row r="74" spans="1:13">
       <c r="A74" s="8" t="s">
         <v>72</v>
       </c>
@@ -3643,8 +3861,11 @@
       <c r="L74" s="15">
         <v>4.7946621010000001</v>
       </c>
-    </row>
-    <row r="75" spans="1:12">
+      <c r="M74" s="15">
+        <v>30.234611000000001</v>
+      </c>
+    </row>
+    <row r="75" spans="1:13">
       <c r="A75" s="8" t="s">
         <v>73</v>
       </c>
@@ -3678,8 +3899,11 @@
       <c r="L75" s="15">
         <v>1.6208092970000001</v>
       </c>
-    </row>
-    <row r="76" spans="1:12">
+      <c r="M75" s="15">
+        <v>13.693778999999999</v>
+      </c>
+    </row>
+    <row r="76" spans="1:13">
       <c r="A76" s="8" t="s">
         <v>74</v>
       </c>
@@ -3710,8 +3934,11 @@
       <c r="L76" s="15">
         <v>2.270169144</v>
       </c>
-    </row>
-    <row r="77" spans="1:12">
+      <c r="M76" s="15">
+        <v>26.536635</v>
+      </c>
+    </row>
+    <row r="77" spans="1:13">
       <c r="A77" s="8" t="s">
         <v>75</v>
       </c>
@@ -3745,8 +3972,9 @@
       <c r="L77" s="15">
         <v>1.612780331</v>
       </c>
-    </row>
-    <row r="78" spans="1:12">
+      <c r="M77" s="15"/>
+    </row>
+    <row r="78" spans="1:13">
       <c r="A78" s="8" t="s">
         <v>76</v>
       </c>
@@ -3775,8 +4003,11 @@
       <c r="L78" s="15">
         <v>1.546907963</v>
       </c>
-    </row>
-    <row r="79" spans="1:12">
+      <c r="M78" s="15">
+        <v>1.192523</v>
+      </c>
+    </row>
+    <row r="79" spans="1:13">
       <c r="A79" s="8" t="s">
         <v>77</v>
       </c>
@@ -3814,8 +4045,11 @@
       <c r="L79" s="15">
         <v>4.5945722770000001</v>
       </c>
-    </row>
-    <row r="80" spans="1:12">
+      <c r="M79" s="15">
+        <v>29.684875000000002</v>
+      </c>
+    </row>
+    <row r="80" spans="1:13">
       <c r="A80" s="8" t="s">
         <v>78</v>
       </c>
@@ -3853,8 +4087,11 @@
       <c r="L80" s="15">
         <v>2.3455869890000001</v>
       </c>
-    </row>
-    <row r="81" spans="1:12">
+      <c r="M80" s="15">
+        <v>37.932749000000001</v>
+      </c>
+    </row>
+    <row r="81" spans="1:13">
       <c r="A81" s="8" t="s">
         <v>79</v>
       </c>
@@ -3886,8 +4123,11 @@
       <c r="L81" s="15">
         <v>2.269450236</v>
       </c>
-    </row>
-    <row r="82" spans="1:12">
+      <c r="M81" s="15">
+        <v>25.286065000000001</v>
+      </c>
+    </row>
+    <row r="82" spans="1:13">
       <c r="A82" s="8" t="s">
         <v>80</v>
       </c>
@@ -3919,8 +4159,11 @@
       <c r="L82" s="15">
         <v>1.9295615370000001</v>
       </c>
-    </row>
-    <row r="83" spans="1:12">
+      <c r="M82" s="15">
+        <v>10.999344000000001</v>
+      </c>
+    </row>
+    <row r="83" spans="1:13">
       <c r="A83" s="8" t="s">
         <v>81</v>
       </c>
@@ -3954,8 +4197,11 @@
       <c r="L83" s="15">
         <v>2.0067722699999999</v>
       </c>
-    </row>
-    <row r="84" spans="1:12">
+      <c r="M83" s="15">
+        <v>15.323005</v>
+      </c>
+    </row>
+    <row r="84" spans="1:13">
       <c r="A84" s="8" t="s">
         <v>82</v>
       </c>
@@ -3989,8 +4235,11 @@
       <c r="L84" s="15">
         <v>1.5667934619999999</v>
       </c>
-    </row>
-    <row r="85" spans="1:12">
+      <c r="M84" s="15">
+        <v>14.916247</v>
+      </c>
+    </row>
+    <row r="85" spans="1:13">
       <c r="A85" s="8" t="s">
         <v>83</v>
       </c>
@@ -4028,8 +4277,11 @@
       <c r="L85" s="15">
         <v>1.9806688539999999</v>
       </c>
-    </row>
-    <row r="86" spans="1:12">
+      <c r="M85" s="15">
+        <v>31.893222000000002</v>
+      </c>
+    </row>
+    <row r="86" spans="1:13">
       <c r="A86" s="8" t="s">
         <v>84</v>
       </c>
@@ -4061,8 +4313,11 @@
       <c r="L86" s="15">
         <v>1.6035010940000001</v>
       </c>
-    </row>
-    <row r="87" spans="1:12">
+      <c r="M86" s="15">
+        <v>16.519642999999999</v>
+      </c>
+    </row>
+    <row r="87" spans="1:13">
       <c r="A87" s="8" t="s">
         <v>85</v>
       </c>
@@ -4097,8 +4352,11 @@
       <c r="L87" s="15">
         <v>1.831791645</v>
       </c>
-    </row>
-    <row r="88" spans="1:12">
+      <c r="M87" s="15">
+        <v>18.213287999999999</v>
+      </c>
+    </row>
+    <row r="88" spans="1:13">
       <c r="A88" s="8" t="s">
         <v>86</v>
       </c>
@@ -4136,8 +4394,11 @@
       <c r="L88" s="15">
         <v>2.1725092840000002</v>
       </c>
-    </row>
-    <row r="89" spans="1:12">
+      <c r="M88" s="15">
+        <v>13.701247</v>
+      </c>
+    </row>
+    <row r="89" spans="1:13">
       <c r="A89" s="8" t="s">
         <v>87</v>
       </c>
@@ -4175,8 +4436,11 @@
       <c r="L89" s="15">
         <v>4.3550731010000003</v>
       </c>
-    </row>
-    <row r="90" spans="1:12">
+      <c r="M89" s="15">
+        <v>26.432732999999999</v>
+      </c>
+    </row>
+    <row r="90" spans="1:13">
       <c r="A90" s="8" t="s">
         <v>88</v>
       </c>
@@ -4207,8 +4471,11 @@
       <c r="L90" s="15">
         <v>4.1221787049999996</v>
       </c>
-    </row>
-    <row r="91" spans="1:12">
+      <c r="M90" s="15">
+        <v>20.360968</v>
+      </c>
+    </row>
+    <row r="91" spans="1:13">
       <c r="A91" s="8" t="s">
         <v>89</v>
       </c>
@@ -4246,8 +4513,11 @@
       <c r="L91" s="15">
         <v>2.471931482</v>
       </c>
-    </row>
-    <row r="92" spans="1:12">
+      <c r="M91" s="15">
+        <v>36.090035</v>
+      </c>
+    </row>
+    <row r="92" spans="1:13">
       <c r="A92" s="8" t="s">
         <v>90</v>
       </c>
@@ -4281,8 +4551,11 @@
       <c r="L92" s="15">
         <v>1.3015604540000001</v>
       </c>
-    </row>
-    <row r="93" spans="1:12">
+      <c r="M92" s="15">
+        <v>21.448879999999999</v>
+      </c>
+    </row>
+    <row r="93" spans="1:13">
       <c r="A93" s="8" t="s">
         <v>91</v>
       </c>
@@ -4316,8 +4589,11 @@
       <c r="L93" s="15">
         <v>1.960396129</v>
       </c>
-    </row>
-    <row r="94" spans="1:12">
+      <c r="M93" s="15">
+        <v>20.156713</v>
+      </c>
+    </row>
+    <row r="94" spans="1:13">
       <c r="A94" s="8" t="s">
         <v>92</v>
       </c>
@@ -4351,8 +4627,11 @@
       <c r="L94" s="15">
         <v>1.503220129</v>
       </c>
-    </row>
-    <row r="95" spans="1:12">
+      <c r="M94" s="15">
+        <v>8.3322769999999995</v>
+      </c>
+    </row>
+    <row r="95" spans="1:13">
       <c r="A95" s="8" t="s">
         <v>93</v>
       </c>
@@ -4386,8 +4665,11 @@
       <c r="L95" s="15">
         <v>2.2975601029999999</v>
       </c>
-    </row>
-    <row r="96" spans="1:12">
+      <c r="M95" s="15">
+        <v>28.710813000000002</v>
+      </c>
+    </row>
+    <row r="96" spans="1:13">
       <c r="A96" s="8" t="s">
         <v>94</v>
       </c>
@@ -4421,8 +4703,11 @@
       <c r="L96" s="15">
         <v>2.0671706080000001</v>
       </c>
-    </row>
-    <row r="97" spans="1:12">
+      <c r="M96" s="15">
+        <v>18.687477999999999</v>
+      </c>
+    </row>
+    <row r="97" spans="1:13">
       <c r="A97" s="8" t="s">
         <v>95</v>
       </c>
@@ -4456,8 +4741,11 @@
       <c r="L97" s="15">
         <v>1.8695020659999999</v>
       </c>
-    </row>
-    <row r="98" spans="1:12">
+      <c r="M97" s="15">
+        <v>38.400931</v>
+      </c>
+    </row>
+    <row r="98" spans="1:13">
       <c r="A98" s="8" t="s">
         <v>96</v>
       </c>
@@ -4495,8 +4783,11 @@
       <c r="L98" s="15">
         <v>3.7186145019999999</v>
       </c>
-    </row>
-    <row r="99" spans="1:12">
+      <c r="M98" s="15">
+        <v>32.613869999999999</v>
+      </c>
+    </row>
+    <row r="99" spans="1:13">
       <c r="A99" s="8" t="s">
         <v>97</v>
       </c>
@@ -4526,8 +4817,11 @@
       <c r="L99" s="15">
         <v>2.3588229690000002</v>
       </c>
-    </row>
-    <row r="100" spans="1:12">
+      <c r="M99" s="15">
+        <v>23.448450000000001</v>
+      </c>
+    </row>
+    <row r="100" spans="1:13">
       <c r="A100" s="8" t="s">
         <v>98</v>
       </c>
@@ -4561,8 +4855,11 @@
       <c r="L100" s="15">
         <v>1.559410481</v>
       </c>
-    </row>
-    <row r="101" spans="1:12">
+      <c r="M100" s="15">
+        <v>13.454078000000001</v>
+      </c>
+    </row>
+    <row r="101" spans="1:13">
       <c r="A101" s="8" t="s">
         <v>99</v>
       </c>
@@ -4596,8 +4893,11 @@
       <c r="L101" s="15">
         <v>1.6105036260000001</v>
       </c>
-    </row>
-    <row r="102" spans="1:12">
+      <c r="M101" s="15">
+        <v>7.1707000000000001</v>
+      </c>
+    </row>
+    <row r="102" spans="1:13">
       <c r="A102" s="8" t="s">
         <v>100</v>
       </c>
@@ -4635,8 +4935,11 @@
       <c r="L102" s="15">
         <v>2.8172961070000002</v>
       </c>
-    </row>
-    <row r="103" spans="1:12">
+      <c r="M102" s="15">
+        <v>38.709806999999998</v>
+      </c>
+    </row>
+    <row r="103" spans="1:13">
       <c r="A103" s="8" t="s">
         <v>101</v>
       </c>
@@ -4670,8 +4973,11 @@
       <c r="L103" s="15">
         <v>2.3859996830000001</v>
       </c>
-    </row>
-    <row r="104" spans="1:12">
+      <c r="M103" s="15">
+        <v>9.9883570000000006</v>
+      </c>
+    </row>
+    <row r="104" spans="1:13">
       <c r="A104" s="8" t="s">
         <v>102</v>
       </c>
@@ -4701,8 +5007,11 @@
       <c r="L104" s="15">
         <v>1.651153146</v>
       </c>
-    </row>
-    <row r="105" spans="1:12">
+      <c r="M104" s="15">
+        <v>5.5946610000000003</v>
+      </c>
+    </row>
+    <row r="105" spans="1:13">
       <c r="A105" s="8" t="s">
         <v>103</v>
       </c>
@@ -4736,8 +5045,11 @@
       <c r="L105" s="15">
         <v>1.9408513249999999</v>
       </c>
-    </row>
-    <row r="106" spans="1:12">
+      <c r="M105" s="15">
+        <v>15.463361000000001</v>
+      </c>
+    </row>
+    <row r="106" spans="1:13">
       <c r="A106" s="8" t="s">
         <v>104</v>
       </c>
@@ -4771,8 +5083,11 @@
       <c r="L106" s="15">
         <v>2.919371215</v>
       </c>
-    </row>
-    <row r="107" spans="1:12">
+      <c r="M106" s="15">
+        <v>10.489746</v>
+      </c>
+    </row>
+    <row r="107" spans="1:13">
       <c r="A107" s="8" t="s">
         <v>105</v>
       </c>
@@ -4806,8 +5121,11 @@
       <c r="L107" s="15">
         <v>1.979901752</v>
       </c>
-    </row>
-    <row r="108" spans="1:12">
+      <c r="M107" s="15">
+        <v>13.614037</v>
+      </c>
+    </row>
+    <row r="108" spans="1:13">
       <c r="A108" s="8" t="s">
         <v>106</v>
       </c>
@@ -4841,8 +5159,11 @@
       <c r="L108" s="15">
         <v>1.566442484</v>
       </c>
-    </row>
-    <row r="109" spans="1:12">
+      <c r="M108" s="15">
+        <v>13.676774</v>
+      </c>
+    </row>
+    <row r="109" spans="1:13">
       <c r="A109" s="8" t="s">
         <v>107</v>
       </c>
@@ -4880,8 +5201,11 @@
       <c r="L109" s="15">
         <v>2.7536132470000001</v>
       </c>
-    </row>
-    <row r="110" spans="1:12">
+      <c r="M109" s="15">
+        <v>33.346711999999997</v>
+      </c>
+    </row>
+    <row r="110" spans="1:13">
       <c r="A110" s="8" t="s">
         <v>108</v>
       </c>
@@ -4919,8 +5243,11 @@
       <c r="L110" s="15">
         <v>1.9087955809999999</v>
       </c>
-    </row>
-    <row r="111" spans="1:12">
+      <c r="M110" s="15">
+        <v>34.141741000000003</v>
+      </c>
+    </row>
+    <row r="111" spans="1:13">
       <c r="A111" s="8" t="s">
         <v>109</v>
       </c>
@@ -4958,8 +5285,11 @@
       <c r="L111" s="15">
         <v>2.0628492619999999</v>
       </c>
-    </row>
-    <row r="112" spans="1:12">
+      <c r="M111" s="15">
+        <v>26.441125</v>
+      </c>
+    </row>
+    <row r="112" spans="1:13">
       <c r="A112" s="8" t="s">
         <v>110</v>
       </c>
@@ -4997,8 +5327,11 @@
       <c r="L112" s="15">
         <v>5.9328232779999999</v>
       </c>
-    </row>
-    <row r="113" spans="1:12">
+      <c r="M112" s="15">
+        <v>29.046813</v>
+      </c>
+    </row>
+    <row r="113" spans="1:13">
       <c r="A113" s="8" t="s">
         <v>111</v>
       </c>
@@ -5032,8 +5365,11 @@
       <c r="L113" s="15">
         <v>2.7858125299999998</v>
       </c>
-    </row>
-    <row r="114" spans="1:12">
+      <c r="M113" s="15">
+        <v>15.459153000000001</v>
+      </c>
+    </row>
+    <row r="114" spans="1:13">
       <c r="A114" s="8" t="s">
         <v>112</v>
       </c>
@@ -5067,8 +5403,11 @@
       <c r="L114" s="15">
         <v>1.4580674179999999</v>
       </c>
-    </row>
-    <row r="115" spans="1:12">
+      <c r="M114" s="15">
+        <v>2.23278</v>
+      </c>
+    </row>
+    <row r="115" spans="1:13">
       <c r="A115" s="8" t="s">
         <v>113</v>
       </c>
@@ -5102,8 +5441,11 @@
       <c r="L115" s="15">
         <v>1.6261849719999999</v>
       </c>
-    </row>
-    <row r="116" spans="1:12">
+      <c r="M115" s="15">
+        <v>15.920230999999999</v>
+      </c>
+    </row>
+    <row r="116" spans="1:13">
       <c r="A116" s="8" t="s">
         <v>114</v>
       </c>
@@ -5141,8 +5483,11 @@
       <c r="L116" s="15">
         <v>2.3197503199999998</v>
       </c>
-    </row>
-    <row r="117" spans="1:12">
+      <c r="M116" s="15">
+        <v>35.078639000000003</v>
+      </c>
+    </row>
+    <row r="117" spans="1:13">
       <c r="A117" s="8" t="s">
         <v>115</v>
       </c>
@@ -5171,8 +5516,11 @@
       <c r="L117" s="15">
         <v>1.6294331559999999</v>
       </c>
-    </row>
-    <row r="118" spans="1:12">
+      <c r="M117" s="15">
+        <v>11.178661</v>
+      </c>
+    </row>
+    <row r="118" spans="1:13">
       <c r="A118" s="8" t="s">
         <v>116</v>
       </c>
@@ -5210,8 +5558,11 @@
       <c r="L118" s="15">
         <v>1.530099412</v>
       </c>
-    </row>
-    <row r="119" spans="1:12">
+      <c r="M118" s="15">
+        <v>13.421915</v>
+      </c>
+    </row>
+    <row r="119" spans="1:13">
       <c r="A119" s="8" t="s">
         <v>117</v>
       </c>
@@ -5249,8 +5600,11 @@
       <c r="L119" s="15">
         <v>2.992271423</v>
       </c>
-    </row>
-    <row r="120" spans="1:12">
+      <c r="M119" s="15">
+        <v>32.356543000000002</v>
+      </c>
+    </row>
+    <row r="120" spans="1:13">
       <c r="A120" s="8" t="s">
         <v>118</v>
       </c>
@@ -5288,8 +5642,11 @@
       <c r="L120" s="15">
         <v>2.8881774459999998</v>
       </c>
-    </row>
-    <row r="121" spans="1:12">
+      <c r="M120" s="15">
+        <v>36.505336999999997</v>
+      </c>
+    </row>
+    <row r="121" spans="1:13">
       <c r="A121" s="8" t="s">
         <v>119</v>
       </c>
@@ -5327,8 +5684,11 @@
       <c r="L121" s="15">
         <v>2.1691135539999999</v>
       </c>
-    </row>
-    <row r="122" spans="1:12">
+      <c r="M121" s="15">
+        <v>29.305698</v>
+      </c>
+    </row>
+    <row r="122" spans="1:13">
       <c r="A122" s="8" t="s">
         <v>120</v>
       </c>
@@ -5366,8 +5726,11 @@
       <c r="L122" s="15">
         <v>3.1578342109999999</v>
       </c>
-    </row>
-    <row r="123" spans="1:12">
+      <c r="M122" s="15">
+        <v>26.236792000000001</v>
+      </c>
+    </row>
+    <row r="123" spans="1:13">
       <c r="A123" s="8" t="s">
         <v>121</v>
       </c>
@@ -5394,8 +5757,9 @@
       <c r="L123" s="15">
         <v>1.9170053039999999</v>
       </c>
-    </row>
-    <row r="124" spans="1:12">
+      <c r="M123" s="15"/>
+    </row>
+    <row r="124" spans="1:13">
       <c r="A124" s="8" t="s">
         <v>122</v>
       </c>
@@ -5433,8 +5797,11 @@
       <c r="L124" s="15">
         <v>2.2706885099999998</v>
       </c>
-    </row>
-    <row r="125" spans="1:12">
+      <c r="M124" s="15">
+        <v>33.180988999999997</v>
+      </c>
+    </row>
+    <row r="125" spans="1:13">
       <c r="A125" s="8" t="s">
         <v>123</v>
       </c>
@@ -5468,8 +5835,11 @@
       <c r="L125" s="15">
         <v>1.5497655269999999</v>
       </c>
-    </row>
-    <row r="126" spans="1:12">
+      <c r="M125" s="15">
+        <v>12.444495999999999</v>
+      </c>
+    </row>
+    <row r="126" spans="1:13">
       <c r="A126" s="8" t="s">
         <v>124</v>
       </c>
@@ -5503,8 +5873,11 @@
       <c r="L126" s="15">
         <v>2.4664065709999998</v>
       </c>
-    </row>
-    <row r="127" spans="1:12">
+      <c r="M126" s="15">
+        <v>44.237478000000003</v>
+      </c>
+    </row>
+    <row r="127" spans="1:13">
       <c r="A127" s="8" t="s">
         <v>125</v>
       </c>
@@ -5542,8 +5915,11 @@
       <c r="L127" s="15">
         <v>2.396185547</v>
       </c>
-    </row>
-    <row r="128" spans="1:12">
+      <c r="M127" s="15">
+        <v>27.700901999999999</v>
+      </c>
+    </row>
+    <row r="128" spans="1:13">
       <c r="A128" s="8" t="s">
         <v>126</v>
       </c>
@@ -5571,8 +5947,9 @@
       <c r="L128" s="15">
         <v>1.979137336</v>
       </c>
-    </row>
-    <row r="129" spans="1:12">
+      <c r="M128" s="15"/>
+    </row>
+    <row r="129" spans="1:13">
       <c r="A129" s="8" t="s">
         <v>127</v>
       </c>
@@ -5604,8 +5981,11 @@
       <c r="L129" s="15">
         <v>2.5833153879999999</v>
       </c>
-    </row>
-    <row r="130" spans="1:12">
+      <c r="M129" s="15">
+        <v>20.6</v>
+      </c>
+    </row>
+    <row r="130" spans="1:13">
       <c r="A130" s="8" t="s">
         <v>128</v>
       </c>
@@ -5639,8 +6019,11 @@
       <c r="L130" s="15">
         <v>2.0172102519999999</v>
       </c>
-    </row>
-    <row r="131" spans="1:12">
+      <c r="M130" s="15">
+        <v>11.390269</v>
+      </c>
+    </row>
+    <row r="131" spans="1:13">
       <c r="A131" s="8" t="s">
         <v>129</v>
       </c>
@@ -5678,8 +6061,11 @@
       <c r="L131" s="15">
         <v>1.7415079250000001</v>
       </c>
-    </row>
-    <row r="132" spans="1:12">
+      <c r="M131" s="15">
+        <v>17.834917999999998</v>
+      </c>
+    </row>
+    <row r="132" spans="1:13">
       <c r="A132" s="8" t="s">
         <v>130</v>
       </c>
@@ -5713,8 +6099,11 @@
       <c r="L132" s="15">
         <v>1.660319265</v>
       </c>
-    </row>
-    <row r="133" spans="1:12">
+      <c r="M132" s="15">
+        <v>18.763441</v>
+      </c>
+    </row>
+    <row r="133" spans="1:13">
       <c r="A133" s="8" t="s">
         <v>131</v>
       </c>
@@ -5746,8 +6135,11 @@
       <c r="L133" s="15">
         <v>2.3274293319999999</v>
       </c>
-    </row>
-    <row r="134" spans="1:12">
+      <c r="M133" s="15">
+        <v>26.147864999999999</v>
+      </c>
+    </row>
+    <row r="134" spans="1:13">
       <c r="A134" s="8" t="s">
         <v>132</v>
       </c>
@@ -5781,8 +6173,11 @@
       <c r="L134" s="15">
         <v>1.466407341</v>
       </c>
-    </row>
-    <row r="135" spans="1:12">
+      <c r="M134" s="15">
+        <v>29.614932</v>
+      </c>
+    </row>
+    <row r="135" spans="1:13">
       <c r="A135" s="8" t="s">
         <v>133</v>
       </c>
@@ -5816,8 +6211,11 @@
       <c r="L135" s="15">
         <v>1.7250975909999999</v>
       </c>
-    </row>
-    <row r="136" spans="1:12">
+      <c r="M135" s="15">
+        <v>25.301887000000001</v>
+      </c>
+    </row>
+    <row r="136" spans="1:13">
       <c r="A136" s="8" t="s">
         <v>134</v>
       </c>
@@ -5849,8 +6247,11 @@
       <c r="L136" s="15">
         <v>2.7327663169999998</v>
       </c>
-    </row>
-    <row r="137" spans="1:12">
+      <c r="M136" s="15">
+        <v>20.373964000000001</v>
+      </c>
+    </row>
+    <row r="137" spans="1:13">
       <c r="A137" s="8" t="s">
         <v>135</v>
       </c>
@@ -5884,8 +6285,11 @@
       <c r="L137" s="15">
         <v>1.7230074019999999</v>
       </c>
-    </row>
-    <row r="138" spans="1:12">
+      <c r="M137" s="15">
+        <v>12.676283</v>
+      </c>
+    </row>
+    <row r="138" spans="1:13">
       <c r="A138" s="8" t="s">
         <v>136</v>
       </c>
@@ -5919,8 +6323,11 @@
       <c r="L138" s="15">
         <v>5.1017697169999998</v>
       </c>
-    </row>
-    <row r="139" spans="1:12">
+      <c r="M138" s="15">
+        <v>30.859074</v>
+      </c>
+    </row>
+    <row r="139" spans="1:13">
       <c r="A139" s="8" t="s">
         <v>137</v>
       </c>
@@ -5954,8 +6361,11 @@
       <c r="L139" s="15">
         <v>1.751084868</v>
       </c>
-    </row>
-    <row r="140" spans="1:12">
+      <c r="M139" s="15">
+        <v>9.2430889999999994</v>
+      </c>
+    </row>
+    <row r="140" spans="1:13">
       <c r="A140" s="8" t="s">
         <v>138</v>
       </c>
@@ -5993,8 +6403,11 @@
       <c r="L140" s="15">
         <v>2.8989730470000001</v>
       </c>
-    </row>
-    <row r="141" spans="1:12">
+      <c r="M140" s="15">
+        <v>32.734135000000002</v>
+      </c>
+    </row>
+    <row r="141" spans="1:13">
       <c r="A141" s="8" t="s">
         <v>139</v>
       </c>
@@ -6028,8 +6441,11 @@
       <c r="L141" s="15">
         <v>5.4680782109999999</v>
       </c>
-    </row>
-    <row r="142" spans="1:12">
+      <c r="M141" s="15">
+        <v>25.773724000000001</v>
+      </c>
+    </row>
+    <row r="142" spans="1:13">
       <c r="A142" s="8" t="s">
         <v>140</v>
       </c>
@@ -6067,8 +6483,11 @@
       <c r="L142" s="15">
         <v>2.0612895770000002</v>
       </c>
-    </row>
-    <row r="143" spans="1:12">
+      <c r="M142" s="15">
+        <v>34.229075999999999</v>
+      </c>
+    </row>
+    <row r="143" spans="1:13">
       <c r="A143" s="8" t="s">
         <v>141</v>
       </c>
@@ -6102,8 +6521,11 @@
       <c r="L143" s="15">
         <v>2.3188884989999998</v>
       </c>
-    </row>
-    <row r="144" spans="1:12">
+      <c r="M143" s="15">
+        <v>26.204868999999999</v>
+      </c>
+    </row>
+    <row r="144" spans="1:13">
       <c r="A144" s="8" t="s">
         <v>142</v>
       </c>
@@ -6135,8 +6557,11 @@
       <c r="L144" s="15">
         <v>1.878402629</v>
       </c>
-    </row>
-    <row r="145" spans="1:12">
+      <c r="M144" s="15">
+        <v>20.279105000000001</v>
+      </c>
+    </row>
+    <row r="145" spans="1:13">
       <c r="A145" s="8" t="s">
         <v>143</v>
       </c>
@@ -6170,8 +6595,11 @@
       <c r="L145" s="15">
         <v>2.3690779389999999</v>
       </c>
-    </row>
-    <row r="146" spans="1:12">
+      <c r="M145" s="15">
+        <v>17.944656999999999</v>
+      </c>
+    </row>
+    <row r="146" spans="1:13">
       <c r="A146" s="8" t="s">
         <v>144</v>
       </c>
@@ -6203,8 +6631,11 @@
       <c r="L146" s="15">
         <v>1.404976709</v>
       </c>
-    </row>
-    <row r="147" spans="1:12">
+      <c r="M146" s="15">
+        <v>7.0387729999999999</v>
+      </c>
+    </row>
+    <row r="147" spans="1:13">
       <c r="A147" s="8" t="s">
         <v>145</v>
       </c>
@@ -6236,8 +6667,11 @@
       <c r="L147" s="15">
         <v>2.1439141730000002</v>
       </c>
-    </row>
-    <row r="148" spans="1:12">
+      <c r="M147" s="15">
+        <v>12.970041</v>
+      </c>
+    </row>
+    <row r="148" spans="1:13">
       <c r="A148" s="8" t="s">
         <v>146</v>
       </c>
@@ -6271,6 +6705,9 @@
       <c r="L148" s="15">
         <v>2.3203841710000002</v>
       </c>
+      <c r="M148" s="15">
+        <v>27.182075999999999</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
added data about internet usage and export
</commit_message>
<xml_diff>
--- a/data_tables/Total_data_cleaned.xlsx
+++ b/data_tables/Total_data_cleaned.xlsx
@@ -1,37 +1,31 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10312"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Simon\Documents\projects\datamining\DataMining-Group23\data_tables\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ulrikaeriksson/Documents/Data_Mining/DataMining-Group23/data_tables/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{17818FF5-08B4-4AED-B436-C5F4BB978910}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3F0785A5-EFD7-FC49-9C3C-06175E1673C0}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{196242FC-4F62-234C-ABAE-90D7B6224D3F}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="19420" windowHeight="13380" xr2:uid="{196242FC-4F62-234C-ABAE-90D7B6224D3F}"/>
   </bookViews>
   <sheets>
     <sheet name="Blad1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="181029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="294" uniqueCount="263">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="163" uniqueCount="163">
   <si>
     <t>Afghanistan</t>
   </si>
@@ -516,317 +510,17 @@
     <t>Economic inequality</t>
   </si>
   <si>
-    <t>27.8</t>
-  </si>
-  <si>
-    <t>29.0</t>
-  </si>
-  <si>
-    <t>27.6</t>
-  </si>
-  <si>
-    <t>42.4</t>
-  </si>
-  <si>
-    <t>32.4</t>
-  </si>
-  <si>
-    <t>34.7</t>
-  </si>
-  <si>
-    <t>30.5</t>
-  </si>
-  <si>
-    <t>31.8</t>
-  </si>
-  <si>
-    <t>32.0</t>
-  </si>
-  <si>
-    <t>26.7</t>
-  </si>
-  <si>
-    <t>28.1</t>
-  </si>
-  <si>
-    <t>47.8</t>
-  </si>
-  <si>
-    <t>45.8</t>
-  </si>
-  <si>
-    <t>33.1</t>
-  </si>
-  <si>
-    <t>60.5</t>
-  </si>
-  <si>
-    <t>46.9</t>
-  </si>
-  <si>
-    <t>37.4</t>
-  </si>
-  <si>
-    <t>35.3</t>
-  </si>
-  <si>
-    <t>30.8</t>
-  </si>
-  <si>
-    <t>46.5</t>
-  </si>
-  <si>
-    <t>34.0</t>
-  </si>
-  <si>
-    <t>56.2</t>
-  </si>
-  <si>
-    <t>43.3</t>
-  </si>
-  <si>
-    <t>47.7</t>
-  </si>
-  <si>
-    <t>38.6</t>
-  </si>
-  <si>
-    <t>50.8</t>
-  </si>
-  <si>
-    <t>42.1</t>
-  </si>
-  <si>
-    <t>40.2</t>
-  </si>
-  <si>
-    <t>48.7</t>
-  </si>
-  <si>
-    <t>32.2</t>
-  </si>
-  <si>
-    <t>35.6</t>
-  </si>
-  <si>
-    <t>25.9</t>
-  </si>
-  <si>
-    <t>28.5</t>
-  </si>
-  <si>
-    <t>45.3</t>
-  </si>
-  <si>
-    <t>34.6</t>
-  </si>
-  <si>
-    <t>33.2</t>
-  </si>
-  <si>
-    <t>26.8</t>
-  </si>
-  <si>
-    <t>32.3</t>
-  </si>
-  <si>
-    <t>47.3</t>
-  </si>
-  <si>
-    <t>36.5</t>
-  </si>
-  <si>
-    <t>31.4</t>
-  </si>
-  <si>
-    <t>42.8</t>
-  </si>
-  <si>
-    <t>35.8</t>
-  </si>
-  <si>
-    <t>33.7</t>
-  </si>
-  <si>
-    <t>60.8</t>
-  </si>
-  <si>
-    <t>30.9</t>
-  </si>
-  <si>
-    <t>25.6</t>
-  </si>
-  <si>
-    <t>35.7</t>
-  </si>
-  <si>
-    <t>38.1</t>
-  </si>
-  <si>
-    <t>38.8</t>
-  </si>
-  <si>
-    <t>29.5</t>
-  </si>
-  <si>
-    <t>31.9</t>
-  </si>
-  <si>
-    <t>41.4</t>
-  </si>
-  <si>
-    <t>41.7</t>
-  </si>
-  <si>
-    <t>45.5</t>
-  </si>
-  <si>
-    <t>32.1</t>
-  </si>
-  <si>
-    <t>35.4</t>
-  </si>
-  <si>
-    <t>26.5</t>
-  </si>
-  <si>
-    <t>37.9</t>
-  </si>
-  <si>
-    <t>35.1</t>
-  </si>
-  <si>
-    <t>54.2</t>
-  </si>
-  <si>
-    <t>37.7</t>
-  </si>
-  <si>
-    <t>31.2</t>
-  </si>
-  <si>
-    <t>40.6</t>
-  </si>
-  <si>
-    <t>46.1</t>
-  </si>
-  <si>
-    <t>33.0</t>
-  </si>
-  <si>
-    <t>43.4</t>
-  </si>
-  <si>
-    <t>26.3</t>
-  </si>
-  <si>
-    <t>40.7</t>
-  </si>
-  <si>
-    <t>45.6</t>
-  </si>
-  <si>
-    <t>59.1</t>
-  </si>
-  <si>
-    <t>32.8</t>
-  </si>
-  <si>
-    <t>28.6</t>
-  </si>
-  <si>
-    <t>46.6</t>
-  </si>
-  <si>
-    <t>43.0</t>
-  </si>
-  <si>
-    <t>30.7</t>
-  </si>
-  <si>
-    <t>35.5</t>
-  </si>
-  <si>
-    <t>50.4</t>
-  </si>
-  <si>
-    <t>47.9</t>
-  </si>
-  <si>
-    <t>43.8</t>
-  </si>
-  <si>
-    <t>40.1</t>
-  </si>
-  <si>
-    <t>27.5</t>
-  </si>
-  <si>
-    <t>45.9</t>
-  </si>
-  <si>
-    <t>40.3</t>
-  </si>
-  <si>
-    <t>29.1</t>
-  </si>
-  <si>
-    <t>26.1</t>
-  </si>
-  <si>
-    <t>25.7</t>
-  </si>
-  <si>
-    <t>63.0</t>
-  </si>
-  <si>
-    <t>31.6</t>
-  </si>
-  <si>
-    <t>36.0</t>
-  </si>
-  <si>
-    <t>39.8</t>
-  </si>
-  <si>
-    <t>27.2</t>
-  </si>
-  <si>
-    <t>32.5</t>
-  </si>
-  <si>
-    <t>37.8</t>
-  </si>
-  <si>
-    <t>41.9</t>
-  </si>
-  <si>
-    <t>43.2</t>
-  </si>
-  <si>
-    <t>25.5</t>
-  </si>
-  <si>
-    <t>34.1</t>
-  </si>
-  <si>
-    <t>41.5</t>
-  </si>
-  <si>
-    <t>39.7</t>
-  </si>
-  <si>
-    <t>36.7</t>
-  </si>
-  <si>
-    <t>57.1</t>
+    <t>Indivduals using internet %</t>
+  </si>
+  <si>
+    <t>Total value of export (% of GDP)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="6">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -870,7 +564,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -893,14 +587,8 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF8F9FA"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
   </fills>
-  <borders count="4">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -936,28 +624,13 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="medium">
-        <color rgb="FFA2A9B1"/>
-      </left>
-      <right style="medium">
-        <color rgb="FFA2A9B1"/>
-      </right>
-      <top style="medium">
-        <color rgb="FFA2A9B1"/>
-      </top>
-      <bottom style="medium">
-        <color rgb="FFA2A9B1"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1000,7 +673,8 @@
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="2" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Dålig" xfId="1" builtinId="27"/>
@@ -1317,13 +991,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{67CF83BE-F021-5E44-A4B8-2C5D9BB127DA}">
-  <dimension ref="A1:N148"/>
+  <dimension ref="A1:P148"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="O3" sqref="O3"/>
+    <sheetView tabSelected="1" topLeftCell="I1" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="O7" sqref="O7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="16"/>
   <cols>
     <col min="1" max="1" width="12.1640625" style="8" customWidth="1"/>
     <col min="2" max="2" width="17.1640625" style="9" customWidth="1"/>
@@ -1331,13 +1005,14 @@
     <col min="4" max="4" width="21.33203125" style="9" customWidth="1"/>
     <col min="5" max="5" width="10.83203125" style="6" customWidth="1"/>
     <col min="6" max="6" width="18.5" style="6" customWidth="1"/>
-    <col min="7" max="7" width="19.6640625" style="6" customWidth="1"/>
-    <col min="8" max="8" width="20.6640625" style="6" customWidth="1"/>
+    <col min="7" max="7" width="16" style="6" customWidth="1"/>
+    <col min="8" max="8" width="13.83203125" style="6" customWidth="1"/>
     <col min="9" max="9" width="14.6640625" customWidth="1"/>
-    <col min="13" max="13" width="21.58203125" customWidth="1"/>
+    <col min="13" max="13" width="21.5" customWidth="1"/>
+    <col min="14" max="14" width="10.6640625" style="19"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:16" ht="34">
       <c r="A1" s="1" t="s">
         <v>147</v>
       </c>
@@ -1377,11 +1052,17 @@
       <c r="M1" s="16" t="s">
         <v>159</v>
       </c>
-      <c r="N1" s="17" t="s">
+      <c r="N1" s="1" t="s">
         <v>160</v>
       </c>
-    </row>
-    <row r="2" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="O1" s="13" t="s">
+        <v>161</v>
+      </c>
+      <c r="P1" s="17" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="2" spans="1:16">
       <c r="A2" s="8" t="s">
         <v>0</v>
       </c>
@@ -1415,11 +1096,17 @@
       <c r="M2" s="15">
         <v>9.1248640000000005</v>
       </c>
-      <c r="N2" s="18" t="s">
-        <v>161</v>
-      </c>
-    </row>
-    <row r="3" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="N2" s="18">
+        <v>27.8</v>
+      </c>
+      <c r="O2">
+        <v>6.39</v>
+      </c>
+      <c r="P2">
+        <v>3.66</v>
+      </c>
+    </row>
+    <row r="3" spans="1:16">
       <c r="A3" s="8" t="s">
         <v>1</v>
       </c>
@@ -1456,11 +1143,17 @@
       <c r="M3" s="15">
         <v>23.52533</v>
       </c>
-      <c r="N3" s="18" t="s">
-        <v>162</v>
-      </c>
-    </row>
-    <row r="4" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="N3" s="18">
+        <v>29</v>
+      </c>
+      <c r="O3">
+        <v>60.1</v>
+      </c>
+      <c r="P3">
+        <v>17.61</v>
+      </c>
+    </row>
+    <row r="4" spans="1:16">
       <c r="A4" s="8" t="s">
         <v>2</v>
       </c>
@@ -1497,11 +1190,17 @@
       <c r="M4" s="15">
         <v>14.162544</v>
       </c>
-      <c r="N4" s="18" t="s">
-        <v>163</v>
-      </c>
-    </row>
-    <row r="5" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="N4" s="18">
+        <v>27.6</v>
+      </c>
+      <c r="O4">
+        <v>18.09</v>
+      </c>
+      <c r="P4">
+        <v>29.5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:16">
       <c r="A5" s="8" t="s">
         <v>3</v>
       </c>
@@ -1542,11 +1241,17 @@
       <c r="M5" s="15">
         <v>30.661214999999999</v>
       </c>
-      <c r="N5" s="18" t="s">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="6" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="N5" s="18">
+        <v>42.4</v>
+      </c>
+      <c r="O5">
+        <v>64.7</v>
+      </c>
+      <c r="P5">
+        <v>13.49</v>
+      </c>
+    </row>
+    <row r="6" spans="1:16">
       <c r="A6" s="8" t="s">
         <v>4</v>
       </c>
@@ -1583,11 +1288,17 @@
       <c r="M6" s="15">
         <v>21.761512</v>
       </c>
-      <c r="N6" s="18" t="s">
-        <v>165</v>
-      </c>
-    </row>
-    <row r="7" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="N6" s="18">
+        <v>32.4</v>
+      </c>
+      <c r="O6">
+        <v>46.3</v>
+      </c>
+      <c r="P6">
+        <v>13.47</v>
+      </c>
+    </row>
+    <row r="7" spans="1:16">
       <c r="A7" s="8" t="s">
         <v>5</v>
       </c>
@@ -1628,11 +1339,17 @@
       <c r="M7" s="15">
         <v>28.578520000000001</v>
       </c>
-      <c r="N7" s="18" t="s">
-        <v>166</v>
-      </c>
-    </row>
-    <row r="8" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="N7" s="18">
+        <v>34.700000000000003</v>
+      </c>
+      <c r="O7">
+        <v>84.56</v>
+      </c>
+      <c r="P7">
+        <v>16.88</v>
+      </c>
+    </row>
+    <row r="8" spans="1:16">
       <c r="A8" s="8" t="s">
         <v>6</v>
       </c>
@@ -1673,11 +1390,17 @@
       <c r="M8" s="15">
         <v>41.884256999999998</v>
       </c>
-      <c r="N8" s="18" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="9" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="N8" s="18">
+        <v>30.5</v>
+      </c>
+      <c r="O8">
+        <v>81</v>
+      </c>
+      <c r="P8">
+        <v>41.32</v>
+      </c>
+    </row>
+    <row r="9" spans="1:16">
       <c r="A9" s="8" t="s">
         <v>7</v>
       </c>
@@ -1718,11 +1441,17 @@
       <c r="M9" s="15">
         <v>16.506067999999999</v>
       </c>
-      <c r="N9" s="18" t="s">
-        <v>168</v>
-      </c>
-    </row>
-    <row r="10" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="N9" s="18">
+        <v>31.8</v>
+      </c>
+      <c r="O9">
+        <v>61</v>
+      </c>
+      <c r="P9">
+        <v>39.1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:16">
       <c r="A10" s="8" t="s">
         <v>8</v>
       </c>
@@ -1758,8 +1487,14 @@
         <v>1.0698810000000001</v>
       </c>
       <c r="N10" s="18"/>
-    </row>
-    <row r="11" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="O10">
+        <v>91</v>
+      </c>
+      <c r="P10">
+        <v>109.52</v>
+      </c>
+    </row>
+    <row r="11" spans="1:16">
       <c r="A11" s="8" t="s">
         <v>9</v>
       </c>
@@ -1796,11 +1531,17 @@
       <c r="M11" s="15">
         <v>8.1908390000000004</v>
       </c>
-      <c r="N11" s="18" t="s">
-        <v>169</v>
-      </c>
-    </row>
-    <row r="12" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="N11" s="18">
+        <v>32</v>
+      </c>
+      <c r="O11">
+        <v>9.6</v>
+      </c>
+      <c r="P11">
+        <v>17.649999999999999</v>
+      </c>
+    </row>
+    <row r="12" spans="1:16">
       <c r="A12" s="8" t="s">
         <v>10</v>
       </c>
@@ -1841,11 +1582,17 @@
       <c r="M12" s="15">
         <v>35.748614000000003</v>
       </c>
-      <c r="N12" s="18" t="s">
-        <v>170</v>
-      </c>
-    </row>
-    <row r="13" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="N12" s="18">
+        <v>26.7</v>
+      </c>
+      <c r="O12">
+        <v>59.02</v>
+      </c>
+      <c r="P12">
+        <v>47.36</v>
+      </c>
+    </row>
+    <row r="13" spans="1:16">
       <c r="A13" s="8" t="s">
         <v>11</v>
       </c>
@@ -1886,11 +1633,17 @@
       <c r="M13" s="15">
         <v>43.875816</v>
       </c>
-      <c r="N13" s="18" t="s">
-        <v>171</v>
-      </c>
-    </row>
-    <row r="14" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="N13" s="18">
+        <v>28.1</v>
+      </c>
+      <c r="O13">
+        <v>85</v>
+      </c>
+      <c r="P13">
+        <v>86.17</v>
+      </c>
+    </row>
+    <row r="14" spans="1:16">
       <c r="A14" s="8" t="s">
         <v>12</v>
       </c>
@@ -1927,11 +1680,17 @@
       <c r="M14" s="15">
         <v>15.888945</v>
       </c>
-      <c r="N14" s="18" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="15" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="N14" s="18">
+        <v>47.8</v>
+      </c>
+      <c r="O14">
+        <v>5.3</v>
+      </c>
+      <c r="P14">
+        <v>20.99</v>
+      </c>
+    </row>
+    <row r="15" spans="1:16">
       <c r="A15" s="8" t="s">
         <v>13</v>
       </c>
@@ -1970,11 +1729,17 @@
       <c r="M15" s="15">
         <v>26.203921000000001</v>
       </c>
-      <c r="N15" s="18" t="s">
-        <v>173</v>
-      </c>
-    </row>
-    <row r="16" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="N15" s="18">
+        <v>45.8</v>
+      </c>
+      <c r="O15">
+        <v>39.020000000000003</v>
+      </c>
+      <c r="P15">
+        <v>39.04</v>
+      </c>
+    </row>
+    <row r="16" spans="1:16">
       <c r="A16" s="8" t="s">
         <v>14</v>
       </c>
@@ -2011,11 +1776,17 @@
       <c r="M16" s="15">
         <v>37.572918999999999</v>
       </c>
-      <c r="N16" s="18" t="s">
-        <v>174</v>
-      </c>
-    </row>
-    <row r="17" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="N16" s="18">
+        <v>33.1</v>
+      </c>
+      <c r="O16">
+        <v>60.8</v>
+      </c>
+      <c r="P16">
+        <v>31.81</v>
+      </c>
+    </row>
+    <row r="17" spans="1:16">
       <c r="A17" s="8" t="s">
         <v>15</v>
       </c>
@@ -2052,11 +1823,17 @@
       <c r="M17" s="15">
         <v>20.871931</v>
       </c>
-      <c r="N17" s="18" t="s">
-        <v>175</v>
-      </c>
-    </row>
-    <row r="18" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="N17" s="18">
+        <v>60.5</v>
+      </c>
+      <c r="O17">
+        <v>18.5</v>
+      </c>
+      <c r="P17">
+        <v>49.12</v>
+      </c>
+    </row>
+    <row r="18" spans="1:16">
       <c r="A18" s="8" t="s">
         <v>16</v>
       </c>
@@ -2097,11 +1874,17 @@
       <c r="M18" s="15">
         <v>33.713017999999998</v>
       </c>
-      <c r="N18" s="18" t="s">
-        <v>176</v>
-      </c>
-    </row>
-    <row r="19" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="N18" s="18">
+        <v>46.9</v>
+      </c>
+      <c r="O18">
+        <v>57.6</v>
+      </c>
+      <c r="P18">
+        <v>9.98</v>
+      </c>
+    </row>
+    <row r="19" spans="1:16">
       <c r="A19" s="8" t="s">
         <v>17</v>
       </c>
@@ -2142,11 +1925,17 @@
       <c r="M19" s="15">
         <v>28.800666</v>
       </c>
-      <c r="N19" s="18" t="s">
-        <v>177</v>
-      </c>
-    </row>
-    <row r="20" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="N19" s="18">
+        <v>37.4</v>
+      </c>
+      <c r="O19">
+        <v>55.49</v>
+      </c>
+      <c r="P19">
+        <v>50.77</v>
+      </c>
+    </row>
+    <row r="20" spans="1:16">
       <c r="A20" s="8" t="s">
         <v>18</v>
       </c>
@@ -2187,11 +1976,17 @@
       <c r="M20" s="15">
         <v>16.652574000000001</v>
       </c>
-      <c r="N20" s="18" t="s">
-        <v>178</v>
-      </c>
-    </row>
-    <row r="21" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="N20" s="18">
+        <v>35.299999999999997</v>
+      </c>
+      <c r="O20">
+        <v>9.4</v>
+      </c>
+      <c r="P20">
+        <v>19.41</v>
+      </c>
+    </row>
+    <row r="21" spans="1:16">
       <c r="A21" s="8" t="s">
         <v>19</v>
       </c>
@@ -2228,11 +2023,17 @@
       <c r="M21" s="15">
         <v>14.825889999999999</v>
       </c>
-      <c r="N21" s="18" t="s">
-        <v>179</v>
-      </c>
-    </row>
-    <row r="22" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="N21" s="18">
+        <v>30.8</v>
+      </c>
+      <c r="O21">
+        <v>9</v>
+      </c>
+      <c r="P21">
+        <v>69.849999999999994</v>
+      </c>
+    </row>
+    <row r="22" spans="1:16">
       <c r="A22" s="8" t="s">
         <v>20</v>
       </c>
@@ -2267,11 +2068,17 @@
       <c r="M22" s="15">
         <v>13.376192</v>
       </c>
-      <c r="N22" s="18" t="s">
-        <v>180</v>
-      </c>
-    </row>
-    <row r="23" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="N22" s="18">
+        <v>46.5</v>
+      </c>
+      <c r="O22">
+        <v>11</v>
+      </c>
+      <c r="P22">
+        <v>17.920000000000002</v>
+      </c>
+    </row>
+    <row r="23" spans="1:16">
       <c r="A23" s="8" t="s">
         <v>21</v>
       </c>
@@ -2312,11 +2119,17 @@
       <c r="M23" s="15">
         <v>32.830274000000003</v>
       </c>
-      <c r="N23" s="18" t="s">
-        <v>181</v>
-      </c>
-    </row>
-    <row r="24" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="N23" s="18">
+        <v>34</v>
+      </c>
+      <c r="O23">
+        <v>87.12</v>
+      </c>
+      <c r="P23">
+        <v>26.61</v>
+      </c>
+    </row>
+    <row r="24" spans="1:16">
       <c r="A24" s="8" t="s">
         <v>22</v>
       </c>
@@ -2351,16 +2164,19 @@
       <c r="M24" s="15">
         <v>9.6534659999999999</v>
       </c>
-      <c r="N24" s="18" t="s">
-        <v>182</v>
-      </c>
-    </row>
-    <row r="25" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="N24" s="18">
+        <v>56.2</v>
+      </c>
+      <c r="P24">
+        <v>5.92</v>
+      </c>
+    </row>
+    <row r="25" spans="1:16">
       <c r="A25" s="8" t="s">
         <v>23</v>
       </c>
       <c r="B25" s="9">
-        <v>4.5589370727539063</v>
+        <v>4.5589370727539062</v>
       </c>
       <c r="C25" s="9">
         <f t="shared" si="0"/>
@@ -2390,11 +2206,17 @@
       <c r="M25" s="15">
         <v>5.6650309999999999</v>
       </c>
-      <c r="N25" s="18" t="s">
-        <v>183</v>
-      </c>
-    </row>
-    <row r="26" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="N25" s="18">
+        <v>43.3</v>
+      </c>
+      <c r="O25">
+        <v>2.5</v>
+      </c>
+      <c r="P25">
+        <v>30.17</v>
+      </c>
+    </row>
+    <row r="26" spans="1:16">
       <c r="A26" s="8" t="s">
         <v>24</v>
       </c>
@@ -2431,11 +2253,17 @@
       <c r="M26" s="15">
         <v>17.409112</v>
       </c>
-      <c r="N26" s="18" t="s">
-        <v>184</v>
-      </c>
-    </row>
-    <row r="27" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="N26" s="18">
+        <v>47.7</v>
+      </c>
+      <c r="O26">
+        <v>72.349999999999994</v>
+      </c>
+      <c r="P26">
+        <v>29.85</v>
+      </c>
+    </row>
+    <row r="27" spans="1:16">
       <c r="A27" s="8" t="s">
         <v>25</v>
       </c>
@@ -2473,11 +2301,17 @@
       <c r="M27" s="15">
         <v>23.790354000000001</v>
       </c>
-      <c r="N27" s="18" t="s">
-        <v>185</v>
-      </c>
-    </row>
-    <row r="28" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="N27" s="18">
+        <v>38.6</v>
+      </c>
+      <c r="O27">
+        <v>49.3</v>
+      </c>
+      <c r="P27">
+        <v>22.89</v>
+      </c>
+    </row>
+    <row r="28" spans="1:16">
       <c r="A28" s="8" t="s">
         <v>26</v>
       </c>
@@ -2518,11 +2352,17 @@
       <c r="M28" s="15">
         <v>19.211746000000002</v>
       </c>
-      <c r="N28" s="18" t="s">
-        <v>186</v>
-      </c>
-    </row>
-    <row r="29" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="N28" s="18">
+        <v>50.8</v>
+      </c>
+      <c r="O28">
+        <v>52.57</v>
+      </c>
+      <c r="P28">
+        <v>15.76</v>
+      </c>
+    </row>
+    <row r="29" spans="1:16">
       <c r="A29" s="8" t="s">
         <v>27</v>
       </c>
@@ -2556,11 +2396,17 @@
       <c r="M29" s="15">
         <v>17.503682999999999</v>
       </c>
-      <c r="N29" s="18" t="s">
-        <v>187</v>
-      </c>
-    </row>
-    <row r="30" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="N29" s="18">
+        <v>42.1</v>
+      </c>
+      <c r="O29">
+        <v>7.11</v>
+      </c>
+      <c r="P29">
+        <v>73.41</v>
+      </c>
+    </row>
+    <row r="30" spans="1:16">
       <c r="A30" s="8" t="s">
         <v>28</v>
       </c>
@@ -2595,11 +2441,17 @@
       <c r="M30" s="15">
         <v>7.1134009999999996</v>
       </c>
-      <c r="N30" s="18" t="s">
-        <v>188</v>
-      </c>
-    </row>
-    <row r="31" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="N30" s="18">
+        <v>40.200000000000003</v>
+      </c>
+      <c r="O30">
+        <v>3</v>
+      </c>
+      <c r="P30">
+        <v>20.83</v>
+      </c>
+    </row>
+    <row r="31" spans="1:16">
       <c r="A31" s="8" t="s">
         <v>29</v>
       </c>
@@ -2640,11 +2492,17 @@
       <c r="M31" s="15">
         <v>13.854123</v>
       </c>
-      <c r="N31" s="18" t="s">
-        <v>189</v>
-      </c>
-    </row>
-    <row r="32" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="N31" s="18">
+        <v>48.7</v>
+      </c>
+      <c r="O31">
+        <v>49.41</v>
+      </c>
+      <c r="P31">
+        <v>65.84</v>
+      </c>
+    </row>
+    <row r="32" spans="1:16">
       <c r="A32" s="8" t="s">
         <v>30</v>
       </c>
@@ -2685,11 +2543,17 @@
       <c r="M32" s="15">
         <v>35.163044999999997</v>
       </c>
-      <c r="N32" s="18" t="s">
-        <v>190</v>
-      </c>
-    </row>
-    <row r="33" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="N32" s="18">
+        <v>32.200000000000003</v>
+      </c>
+      <c r="O32">
+        <v>68.569999999999993</v>
+      </c>
+      <c r="P32">
+        <v>23.94</v>
+      </c>
+    </row>
+    <row r="33" spans="1:16">
       <c r="A33" s="8" t="s">
         <v>31</v>
       </c>
@@ -2730,11 +2594,17 @@
       <c r="M33" s="15">
         <v>23.997837000000001</v>
       </c>
-      <c r="N33" s="18" t="s">
-        <v>191</v>
-      </c>
-    </row>
-    <row r="34" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="N33" s="18">
+        <v>35.6</v>
+      </c>
+      <c r="O33">
+        <v>69.33</v>
+      </c>
+      <c r="P33">
+        <v>16.059999999999999</v>
+      </c>
+    </row>
+    <row r="34" spans="1:16">
       <c r="A34" s="8" t="s">
         <v>32</v>
       </c>
@@ -2771,11 +2641,17 @@
       <c r="M34" s="15">
         <v>34.068710000000003</v>
       </c>
-      <c r="N34" s="18" t="s">
-        <v>192</v>
-      </c>
-    </row>
-    <row r="35" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="N34" s="18">
+        <v>25.9</v>
+      </c>
+      <c r="O34">
+        <v>79.709999999999994</v>
+      </c>
+      <c r="P34">
+        <v>83.7</v>
+      </c>
+    </row>
+    <row r="35" spans="1:16">
       <c r="A35" s="8" t="s">
         <v>33</v>
       </c>
@@ -2812,11 +2688,17 @@
       <c r="M35" s="15">
         <v>45.43515</v>
       </c>
-      <c r="N35" s="18" t="s">
-        <v>193</v>
-      </c>
-    </row>
-    <row r="36" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="N35" s="18">
+        <v>28.5</v>
+      </c>
+      <c r="O35">
+        <v>95.99</v>
+      </c>
+      <c r="P35">
+        <v>31.23</v>
+      </c>
+    </row>
+    <row r="36" spans="1:16">
       <c r="A36" s="8" t="s">
         <v>34</v>
       </c>
@@ -2857,11 +2739,17 @@
       <c r="M36" s="15">
         <v>13.509418</v>
       </c>
-      <c r="N36" s="18" t="s">
-        <v>194</v>
-      </c>
-    </row>
-    <row r="37" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="N36" s="18">
+        <v>45.3</v>
+      </c>
+      <c r="O36">
+        <v>49.58</v>
+      </c>
+      <c r="P36">
+        <v>16.440000000000001</v>
+      </c>
+    </row>
+    <row r="37" spans="1:16">
       <c r="A37" s="8" t="s">
         <v>35</v>
       </c>
@@ -2901,8 +2789,14 @@
       <c r="N37" s="18">
         <v>45</v>
       </c>
-    </row>
-    <row r="38" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="O37">
+        <v>43</v>
+      </c>
+      <c r="P37">
+        <v>27.59</v>
+      </c>
+    </row>
+    <row r="38" spans="1:16">
       <c r="A38" s="8" t="s">
         <v>36</v>
       </c>
@@ -2937,11 +2831,17 @@
         <v>1.446643887</v>
       </c>
       <c r="M38" s="15"/>
-      <c r="N38" s="18" t="s">
-        <v>168</v>
-      </c>
-    </row>
-    <row r="39" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="N38" s="18">
+        <v>31.8</v>
+      </c>
+      <c r="O38">
+        <v>31.7</v>
+      </c>
+      <c r="P38">
+        <v>10.57</v>
+      </c>
+    </row>
+    <row r="39" spans="1:16">
       <c r="A39" s="8" t="s">
         <v>37</v>
       </c>
@@ -2981,8 +2881,14 @@
       <c r="N39" s="18">
         <v>40</v>
       </c>
-    </row>
-    <row r="40" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="O39">
+        <v>29.7</v>
+      </c>
+      <c r="P39">
+        <v>21.38</v>
+      </c>
+    </row>
+    <row r="40" spans="1:16">
       <c r="A40" s="8" t="s">
         <v>38</v>
       </c>
@@ -3023,11 +2929,17 @@
       <c r="M40" s="15">
         <v>33.730350999999999</v>
       </c>
-      <c r="N40" s="18" t="s">
-        <v>195</v>
-      </c>
-    </row>
-    <row r="41" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="N40" s="18">
+        <v>34.6</v>
+      </c>
+      <c r="O40">
+        <v>84.24</v>
+      </c>
+      <c r="P40">
+        <v>61.46</v>
+      </c>
+    </row>
+    <row r="41" spans="1:16">
       <c r="A41" s="8" t="s">
         <v>39</v>
       </c>
@@ -3062,11 +2974,17 @@
         <v>2.616682548</v>
       </c>
       <c r="M41" s="15"/>
-      <c r="N41" s="18" t="s">
-        <v>196</v>
-      </c>
-    </row>
-    <row r="42" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="N41" s="18">
+        <v>33.200000000000003</v>
+      </c>
+      <c r="O41">
+        <v>2.9</v>
+      </c>
+      <c r="P41">
+        <v>4.68</v>
+      </c>
+    </row>
+    <row r="42" spans="1:16">
       <c r="A42" s="8" t="s">
         <v>40</v>
       </c>
@@ -3107,11 +3025,17 @@
       <c r="M42" s="15">
         <v>44.017195000000001</v>
       </c>
-      <c r="N42" s="18" t="s">
-        <v>197</v>
-      </c>
-    </row>
-    <row r="43" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="N42" s="18">
+        <v>26.8</v>
+      </c>
+      <c r="O42">
+        <v>92.38</v>
+      </c>
+      <c r="P42">
+        <v>28.35</v>
+      </c>
+    </row>
+    <row r="43" spans="1:16">
       <c r="A43" s="8" t="s">
         <v>41</v>
       </c>
@@ -3152,11 +3076,17 @@
       <c r="M43" s="15">
         <v>45.277869000000003</v>
       </c>
-      <c r="N43" s="18" t="s">
-        <v>198</v>
-      </c>
-    </row>
-    <row r="44" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="N43" s="18">
+        <v>32.299999999999997</v>
+      </c>
+      <c r="O43">
+        <v>83.75</v>
+      </c>
+      <c r="P43">
+        <v>21.14</v>
+      </c>
+    </row>
+    <row r="44" spans="1:16">
       <c r="A44" s="8" t="s">
         <v>42</v>
       </c>
@@ -3191,8 +3121,14 @@
       <c r="N44" s="18">
         <v>38</v>
       </c>
-    </row>
-    <row r="45" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="O44">
+        <v>9.81</v>
+      </c>
+      <c r="P44">
+        <v>51.19</v>
+      </c>
+    </row>
+    <row r="45" spans="1:16">
       <c r="A45" s="8" t="s">
         <v>43</v>
       </c>
@@ -3226,11 +3162,17 @@
       <c r="M45" s="15">
         <v>11.14148</v>
       </c>
-      <c r="N45" s="18" t="s">
-        <v>199</v>
-      </c>
-    </row>
-    <row r="46" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="N45" s="18">
+        <v>47.3</v>
+      </c>
+      <c r="O45">
+        <v>15.56</v>
+      </c>
+      <c r="P45">
+        <v>13.04</v>
+      </c>
+    </row>
+    <row r="46" spans="1:16">
       <c r="A46" s="8" t="s">
         <v>44</v>
       </c>
@@ -3271,11 +3213,17 @@
       <c r="M46" s="15">
         <v>25.819448000000001</v>
       </c>
-      <c r="N46" s="18" t="s">
-        <v>200</v>
-      </c>
-    </row>
-    <row r="47" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="N46" s="18">
+        <v>36.5</v>
+      </c>
+      <c r="O46">
+        <v>48.9</v>
+      </c>
+      <c r="P46">
+        <v>17.329999999999998</v>
+      </c>
+    </row>
+    <row r="47" spans="1:16">
       <c r="A47" s="8" t="s">
         <v>45</v>
       </c>
@@ -3316,11 +3264,17 @@
       <c r="M47" s="15">
         <v>37.430619999999998</v>
       </c>
-      <c r="N47" s="18" t="s">
-        <v>201</v>
-      </c>
-    </row>
-    <row r="48" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="N47" s="18">
+        <v>31.4</v>
+      </c>
+      <c r="O47">
+        <v>86.19</v>
+      </c>
+      <c r="P47">
+        <v>37.61</v>
+      </c>
+    </row>
+    <row r="48" spans="1:16">
       <c r="A48" s="8" t="s">
         <v>46</v>
       </c>
@@ -3361,11 +3315,17 @@
       <c r="M48" s="15">
         <v>12.377316</v>
       </c>
-      <c r="N48" s="18" t="s">
-        <v>202</v>
-      </c>
-    </row>
-    <row r="49" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="N48" s="18">
+        <v>42.8</v>
+      </c>
+      <c r="O48">
+        <v>18.899999999999999</v>
+      </c>
+      <c r="P48">
+        <v>25.55</v>
+      </c>
+    </row>
+    <row r="49" spans="1:16">
       <c r="A49" s="8" t="s">
         <v>47</v>
       </c>
@@ -3406,11 +3366,17 @@
       <c r="M49" s="15">
         <v>38.338583999999997</v>
       </c>
-      <c r="N49" s="18" t="s">
-        <v>203</v>
-      </c>
-    </row>
-    <row r="50" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="N49" s="18">
+        <v>35.799999999999997</v>
+      </c>
+      <c r="O49">
+        <v>63.21</v>
+      </c>
+      <c r="P49">
+        <v>14.93</v>
+      </c>
+    </row>
+    <row r="50" spans="1:16">
       <c r="A50" s="8" t="s">
         <v>48</v>
       </c>
@@ -3445,11 +3411,17 @@
       <c r="M50" s="15">
         <v>10.78232</v>
       </c>
-      <c r="N50" s="18" t="s">
-        <v>189</v>
-      </c>
-    </row>
-    <row r="51" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="N50" s="18">
+        <v>48.7</v>
+      </c>
+      <c r="O50">
+        <v>23.4</v>
+      </c>
+      <c r="P50">
+        <v>19.440000000000001</v>
+      </c>
+    </row>
+    <row r="51" spans="1:16">
       <c r="A51" s="8" t="s">
         <v>49</v>
       </c>
@@ -3484,11 +3456,17 @@
       <c r="M51" s="15">
         <v>14.030989</v>
       </c>
-      <c r="N51" s="18" t="s">
-        <v>204</v>
-      </c>
-    </row>
-    <row r="52" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="N51" s="18">
+        <v>33.700000000000003</v>
+      </c>
+      <c r="O51">
+        <v>1.72</v>
+      </c>
+      <c r="P51">
+        <v>37.67</v>
+      </c>
+    </row>
+    <row r="52" spans="1:16">
       <c r="A52" s="8" t="s">
         <v>50</v>
       </c>
@@ -3523,11 +3501,17 @@
       <c r="M52" s="15">
         <v>13.731528000000001</v>
       </c>
-      <c r="N52" s="18" t="s">
-        <v>205</v>
-      </c>
-    </row>
-    <row r="53" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="N52" s="18">
+        <v>60.8</v>
+      </c>
+      <c r="O52">
+        <v>11.4</v>
+      </c>
+      <c r="P52">
+        <v>12.38</v>
+      </c>
+    </row>
+    <row r="53" spans="1:16">
       <c r="A53" s="8" t="s">
         <v>51</v>
       </c>
@@ -3567,8 +3551,14 @@
       <c r="N53" s="18">
         <v>50</v>
       </c>
-    </row>
-    <row r="54" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="O53">
+        <v>19.079999999999998</v>
+      </c>
+      <c r="P53">
+        <v>44.73</v>
+      </c>
+    </row>
+    <row r="54" spans="1:16">
       <c r="A54" s="8" t="s">
         <v>52</v>
       </c>
@@ -3596,8 +3586,14 @@
         <v>13.574933</v>
       </c>
       <c r="N54" s="18"/>
-    </row>
-    <row r="55" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="O54">
+        <v>74.56</v>
+      </c>
+      <c r="P54">
+        <v>162.75</v>
+      </c>
+    </row>
+    <row r="55" spans="1:16">
       <c r="A55" s="8" t="s">
         <v>53</v>
       </c>
@@ -3638,11 +3634,17 @@
       <c r="M55" s="15">
         <v>39.148890999999999</v>
       </c>
-      <c r="N55" s="18" t="s">
-        <v>206</v>
-      </c>
-    </row>
-    <row r="56" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="N55" s="18">
+        <v>30.9</v>
+      </c>
+      <c r="O55">
+        <v>76.13</v>
+      </c>
+      <c r="P55">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="56" spans="1:16">
       <c r="A56" s="8" t="s">
         <v>54</v>
       </c>
@@ -3676,11 +3678,17 @@
       <c r="M56" s="15">
         <v>36.789971000000001</v>
       </c>
-      <c r="N56" s="18" t="s">
-        <v>207</v>
-      </c>
-    </row>
-    <row r="57" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="N56" s="18">
+        <v>25.6</v>
+      </c>
+      <c r="O56">
+        <v>98.16</v>
+      </c>
+      <c r="P56">
+        <v>31.55</v>
+      </c>
+    </row>
+    <row r="57" spans="1:16">
       <c r="A57" s="8" t="s">
         <v>55</v>
       </c>
@@ -3717,11 +3725,17 @@
       <c r="M57" s="15">
         <v>17.577255000000001</v>
       </c>
-      <c r="N57" s="18" t="s">
-        <v>208</v>
-      </c>
-    </row>
-    <row r="58" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="N57" s="18">
+        <v>35.700000000000003</v>
+      </c>
+      <c r="O57">
+        <v>18</v>
+      </c>
+      <c r="P57">
+        <v>15.36</v>
+      </c>
+    </row>
+    <row r="58" spans="1:16">
       <c r="A58" s="8" t="s">
         <v>56</v>
       </c>
@@ -3758,11 +3772,17 @@
       <c r="M58" s="15">
         <v>10.361459</v>
       </c>
-      <c r="N58" s="18" t="s">
-        <v>209</v>
-      </c>
-    </row>
-    <row r="59" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="N58" s="18">
+        <v>38.1</v>
+      </c>
+      <c r="O58">
+        <v>17.14</v>
+      </c>
+      <c r="P58">
+        <v>21.86</v>
+      </c>
+    </row>
+    <row r="59" spans="1:16">
       <c r="A59" s="8" t="s">
         <v>57</v>
       </c>
@@ -3799,11 +3819,17 @@
       <c r="M59" s="15">
         <v>7.9746290000000002</v>
       </c>
-      <c r="N59" s="18" t="s">
-        <v>210</v>
-      </c>
-    </row>
-    <row r="60" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="N59" s="18">
+        <v>38.799999999999997</v>
+      </c>
+      <c r="O59">
+        <v>39.35</v>
+      </c>
+      <c r="P59">
+        <v>20.25</v>
+      </c>
+    </row>
+    <row r="60" spans="1:16">
       <c r="A60" s="8" t="s">
         <v>58</v>
       </c>
@@ -3838,11 +3864,17 @@
       <c r="M60" s="15">
         <v>1.3778090000000001</v>
       </c>
-      <c r="N60" s="18" t="s">
-        <v>211</v>
-      </c>
-    </row>
-    <row r="61" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="N60" s="18">
+        <v>29.5</v>
+      </c>
+      <c r="O60">
+        <v>11.3</v>
+      </c>
+      <c r="P60">
+        <v>37.549999999999997</v>
+      </c>
+    </row>
+    <row r="61" spans="1:16">
       <c r="A61" s="8" t="s">
         <v>59</v>
       </c>
@@ -3883,11 +3915,17 @@
       <c r="M61" s="15">
         <v>23.358557999999999</v>
       </c>
-      <c r="N61" s="18" t="s">
-        <v>212</v>
-      </c>
-    </row>
-    <row r="62" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="N61" s="18">
+        <v>31.9</v>
+      </c>
+      <c r="O61">
+        <v>79.69</v>
+      </c>
+      <c r="P61">
+        <v>57.73</v>
+      </c>
+    </row>
+    <row r="62" spans="1:16">
       <c r="A62" s="8" t="s">
         <v>60</v>
       </c>
@@ -3928,11 +3966,17 @@
       <c r="M62" s="15">
         <v>31.128926</v>
       </c>
-      <c r="N62" s="18" t="s">
-        <v>213</v>
-      </c>
-    </row>
-    <row r="63" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="N62" s="18">
+        <v>41.4</v>
+      </c>
+      <c r="O62">
+        <v>71.45</v>
+      </c>
+      <c r="P62">
+        <v>22.56</v>
+      </c>
+    </row>
+    <row r="63" spans="1:16">
       <c r="A63" s="8" t="s">
         <v>61</v>
       </c>
@@ -3973,11 +4017,17 @@
       <c r="M63" s="15">
         <v>42.385586000000004</v>
       </c>
-      <c r="N63" s="18" t="s">
-        <v>166</v>
-      </c>
-    </row>
-    <row r="64" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="N63" s="18">
+        <v>34.700000000000003</v>
+      </c>
+      <c r="O63">
+        <v>61.96</v>
+      </c>
+      <c r="P63">
+        <v>24.39</v>
+      </c>
+    </row>
+    <row r="64" spans="1:16">
       <c r="A64" s="8" t="s">
         <v>62</v>
       </c>
@@ -4012,11 +4062,17 @@
       <c r="M64" s="15">
         <v>16.017084000000001</v>
       </c>
-      <c r="N64" s="18" t="s">
-        <v>214</v>
-      </c>
-    </row>
-    <row r="65" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="N64" s="18">
+        <v>41.7</v>
+      </c>
+      <c r="O64">
+        <v>14.6</v>
+      </c>
+      <c r="P64">
+        <v>37.4</v>
+      </c>
+    </row>
+    <row r="65" spans="1:16">
       <c r="A65" s="8" t="s">
         <v>63</v>
       </c>
@@ -4057,11 +4113,17 @@
       <c r="M65" s="15">
         <v>25.114878999999998</v>
       </c>
-      <c r="N65" s="18" t="s">
-        <v>215</v>
-      </c>
-    </row>
-    <row r="66" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="N65" s="18">
+        <v>45.5</v>
+      </c>
+      <c r="O65">
+        <v>40.5</v>
+      </c>
+      <c r="P65">
+        <v>10.43</v>
+      </c>
+    </row>
+    <row r="66" spans="1:16">
       <c r="A66" s="8" t="s">
         <v>64</v>
       </c>
@@ -4102,16 +4164,22 @@
       <c r="M66" s="15">
         <v>30.777436000000002</v>
       </c>
-      <c r="N66" s="18" t="s">
-        <v>216</v>
-      </c>
-    </row>
-    <row r="67" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="N66" s="18">
+        <v>32.1</v>
+      </c>
+      <c r="O66">
+        <v>90.58</v>
+      </c>
+      <c r="P66">
+        <v>15.6</v>
+      </c>
+    </row>
+    <row r="67" spans="1:16">
       <c r="A67" s="8" t="s">
         <v>65</v>
       </c>
       <c r="B67" s="9">
-        <v>4.8080825805664063</v>
+        <v>4.8080825805664062</v>
       </c>
       <c r="C67" s="9">
         <f t="shared" ref="C67:C130" si="1">ROUND(B67,0)</f>
@@ -4141,11 +4209,17 @@
       <c r="M67" s="15">
         <v>15.341718</v>
       </c>
-      <c r="N67" s="18" t="s">
-        <v>217</v>
-      </c>
-    </row>
-    <row r="68" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="N67" s="18">
+        <v>35.4</v>
+      </c>
+      <c r="O67">
+        <v>44</v>
+      </c>
+      <c r="P67">
+        <v>23.71</v>
+      </c>
+    </row>
+    <row r="68" spans="1:16">
       <c r="A68" s="8" t="s">
         <v>66</v>
       </c>
@@ -4182,11 +4256,17 @@
       <c r="M68" s="15">
         <v>15.228497000000001</v>
       </c>
-      <c r="N68" s="18" t="s">
-        <v>218</v>
-      </c>
-    </row>
-    <row r="69" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="N68" s="18">
+        <v>26.5</v>
+      </c>
+      <c r="O68">
+        <v>54.89</v>
+      </c>
+      <c r="P68">
+        <v>32.090000000000003</v>
+      </c>
+    </row>
+    <row r="69" spans="1:16">
       <c r="A69" s="8" t="s">
         <v>67</v>
       </c>
@@ -4223,11 +4303,17 @@
       <c r="M69" s="15">
         <v>15.800242000000001</v>
       </c>
-      <c r="N69" s="18" t="s">
-        <v>184</v>
-      </c>
-    </row>
-    <row r="70" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="N69" s="18">
+        <v>47.7</v>
+      </c>
+      <c r="O69">
+        <v>43.4</v>
+      </c>
+      <c r="P69">
+        <v>11.93</v>
+      </c>
+    </row>
+    <row r="70" spans="1:16">
       <c r="A70" s="8" t="s">
         <v>68</v>
       </c>
@@ -4256,11 +4342,11 @@
       <c r="M70" s="15">
         <v>23.459638000000002</v>
       </c>
-      <c r="N70" s="18" t="s">
-        <v>218</v>
-      </c>
-    </row>
-    <row r="71" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="N70" s="18">
+        <v>26.5</v>
+      </c>
+    </row>
+    <row r="71" spans="1:16">
       <c r="A71" s="8" t="s">
         <v>69</v>
       </c>
@@ -4298,8 +4384,14 @@
         <v>1.5125850000000001</v>
       </c>
       <c r="N71" s="18"/>
-    </row>
-    <row r="72" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="O71">
+        <v>78.7</v>
+      </c>
+      <c r="P71">
+        <v>57.49</v>
+      </c>
+    </row>
+    <row r="72" spans="1:16">
       <c r="A72" s="8" t="s">
         <v>70</v>
       </c>
@@ -4336,11 +4428,17 @@
       <c r="M72" s="15">
         <v>25.102250000000002</v>
       </c>
-      <c r="N72" s="18" t="s">
-        <v>197</v>
-      </c>
-    </row>
-    <row r="73" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="N72" s="18">
+        <v>26.8</v>
+      </c>
+      <c r="O72">
+        <v>28.3</v>
+      </c>
+      <c r="P72">
+        <v>16.59</v>
+      </c>
+    </row>
+    <row r="73" spans="1:16">
       <c r="A73" s="8" t="s">
         <v>71</v>
       </c>
@@ -4377,11 +4475,17 @@
       <c r="M73" s="15">
         <v>12.428921000000001</v>
       </c>
-      <c r="N73" s="18" t="s">
-        <v>219</v>
-      </c>
-    </row>
-    <row r="74" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="N73" s="18">
+        <v>37.9</v>
+      </c>
+      <c r="O73">
+        <v>14.26</v>
+      </c>
+      <c r="P73">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="74" spans="1:16">
       <c r="A74" s="8" t="s">
         <v>72</v>
       </c>
@@ -4422,11 +4526,17 @@
       <c r="M74" s="15">
         <v>30.234611000000001</v>
       </c>
-      <c r="N74" s="18" t="s">
-        <v>220</v>
-      </c>
-    </row>
-    <row r="75" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="N74" s="18">
+        <v>35.1</v>
+      </c>
+      <c r="O74">
+        <v>75.83</v>
+      </c>
+      <c r="P74">
+        <v>45.97</v>
+      </c>
+    </row>
+    <row r="75" spans="1:16">
       <c r="A75" s="8" t="s">
         <v>73</v>
       </c>
@@ -4464,8 +4574,14 @@
         <v>13.693778999999999</v>
       </c>
       <c r="N75" s="18"/>
-    </row>
-    <row r="76" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="O75">
+        <v>74.7</v>
+      </c>
+      <c r="P75">
+        <v>7.61</v>
+      </c>
+    </row>
+    <row r="76" spans="1:16">
       <c r="A76" s="8" t="s">
         <v>74</v>
       </c>
@@ -4499,11 +4615,17 @@
       <c r="M76" s="15">
         <v>26.536635</v>
       </c>
-      <c r="N76" s="18" t="s">
-        <v>221</v>
-      </c>
-    </row>
-    <row r="77" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="N76" s="18">
+        <v>54.2</v>
+      </c>
+      <c r="O76">
+        <v>11</v>
+      </c>
+      <c r="P76">
+        <v>42.4</v>
+      </c>
+    </row>
+    <row r="77" spans="1:16">
       <c r="A77" s="8" t="s">
         <v>75</v>
       </c>
@@ -4538,11 +4660,17 @@
         <v>1.612780331</v>
       </c>
       <c r="M77" s="15"/>
-      <c r="N77" s="18" t="s">
-        <v>196</v>
-      </c>
-    </row>
-    <row r="78" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="N77" s="18">
+        <v>33.200000000000003</v>
+      </c>
+      <c r="O77">
+        <v>5.41</v>
+      </c>
+      <c r="P77">
+        <v>48.32</v>
+      </c>
+    </row>
+    <row r="78" spans="1:16">
       <c r="A78" s="8" t="s">
         <v>76</v>
       </c>
@@ -4575,8 +4703,14 @@
         <v>1.192523</v>
       </c>
       <c r="N78" s="18"/>
-    </row>
-    <row r="79" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="O78">
+        <v>17.760000000000002</v>
+      </c>
+      <c r="P78">
+        <v>45.54</v>
+      </c>
+    </row>
+    <row r="79" spans="1:16">
       <c r="A79" s="8" t="s">
         <v>77</v>
       </c>
@@ -4617,11 +4751,17 @@
       <c r="M79" s="15">
         <v>29.684875000000002</v>
       </c>
-      <c r="N79" s="18" t="s">
-        <v>222</v>
-      </c>
-    </row>
-    <row r="80" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="N79" s="18">
+        <v>37.700000000000003</v>
+      </c>
+      <c r="O79">
+        <v>72.13</v>
+      </c>
+      <c r="P79">
+        <v>66.94</v>
+      </c>
+    </row>
+    <row r="80" spans="1:16">
       <c r="A80" s="8" t="s">
         <v>78</v>
       </c>
@@ -4662,11 +4802,17 @@
       <c r="M80" s="15">
         <v>37.932749000000001</v>
       </c>
-      <c r="N80" s="18" t="s">
-        <v>223</v>
-      </c>
-    </row>
-    <row r="81" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="N80" s="18">
+        <v>31.2</v>
+      </c>
+      <c r="O80">
+        <v>94.67</v>
+      </c>
+      <c r="P80">
+        <v>42.35</v>
+      </c>
+    </row>
+    <row r="81" spans="1:16">
       <c r="A81" s="8" t="s">
         <v>79</v>
       </c>
@@ -4701,11 +4847,14 @@
       <c r="M81" s="15">
         <v>25.286065000000001</v>
       </c>
-      <c r="N81" s="18" t="s">
-        <v>191</v>
-      </c>
-    </row>
-    <row r="82" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="N81" s="18">
+        <v>35.6</v>
+      </c>
+      <c r="P81">
+        <v>45.19</v>
+      </c>
+    </row>
+    <row r="82" spans="1:16">
       <c r="A82" s="8" t="s">
         <v>80</v>
       </c>
@@ -4740,11 +4889,17 @@
       <c r="M82" s="15">
         <v>10.999344000000001</v>
       </c>
-      <c r="N82" s="18" t="s">
-        <v>224</v>
-      </c>
-    </row>
-    <row r="83" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="N82" s="18">
+        <v>40.6</v>
+      </c>
+      <c r="O82">
+        <v>3.7</v>
+      </c>
+      <c r="P82">
+        <v>20.59</v>
+      </c>
+    </row>
+    <row r="83" spans="1:16">
       <c r="A83" s="8" t="s">
         <v>81</v>
       </c>
@@ -4781,11 +4936,17 @@
       <c r="M83" s="15">
         <v>15.323005</v>
       </c>
-      <c r="N83" s="18" t="s">
-        <v>225</v>
-      </c>
-    </row>
-    <row r="84" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="N83" s="18">
+        <v>46.1</v>
+      </c>
+      <c r="O83">
+        <v>5.83</v>
+      </c>
+      <c r="P83">
+        <v>18.329999999999998</v>
+      </c>
+    </row>
+    <row r="84" spans="1:16">
       <c r="A84" s="8" t="s">
         <v>82</v>
       </c>
@@ -4822,11 +4983,17 @@
       <c r="M84" s="15">
         <v>14.916247</v>
       </c>
-      <c r="N84" s="18" t="s">
-        <v>226</v>
-      </c>
-    </row>
-    <row r="85" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="N84" s="18">
+        <v>33</v>
+      </c>
+      <c r="O84">
+        <v>7</v>
+      </c>
+      <c r="P84">
+        <v>14.6</v>
+      </c>
+    </row>
+    <row r="85" spans="1:16">
       <c r="A85" s="8" t="s">
         <v>83</v>
       </c>
@@ -4868,8 +5035,14 @@
         <v>31.893222000000002</v>
       </c>
       <c r="N85" s="18"/>
-    </row>
-    <row r="86" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="O85">
+        <v>73.17</v>
+      </c>
+      <c r="P85">
+        <v>66.489999999999995</v>
+      </c>
+    </row>
+    <row r="86" spans="1:16">
       <c r="A86" s="8" t="s">
         <v>84</v>
       </c>
@@ -4904,11 +5077,17 @@
       <c r="M86" s="15">
         <v>16.519642999999999</v>
       </c>
-      <c r="N86" s="18" t="s">
-        <v>165</v>
-      </c>
-    </row>
-    <row r="87" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="N86" s="18">
+        <v>32.4</v>
+      </c>
+      <c r="O86">
+        <v>10.7</v>
+      </c>
+      <c r="P86">
+        <v>48.86</v>
+      </c>
+    </row>
+    <row r="87" spans="1:16">
       <c r="A87" s="8" t="s">
         <v>85</v>
       </c>
@@ -4946,11 +5125,17 @@
       <c r="M87" s="15">
         <v>18.213287999999999</v>
       </c>
-      <c r="N87" s="18" t="s">
-        <v>203</v>
-      </c>
-    </row>
-    <row r="88" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="N87" s="18">
+        <v>35.799999999999997</v>
+      </c>
+      <c r="O87">
+        <v>41.44</v>
+      </c>
+      <c r="P87">
+        <v>22.48</v>
+      </c>
+    </row>
+    <row r="88" spans="1:16">
       <c r="A88" s="8" t="s">
         <v>86</v>
       </c>
@@ -4991,11 +5176,17 @@
       <c r="M88" s="15">
         <v>13.701247</v>
       </c>
-      <c r="N88" s="18" t="s">
-        <v>227</v>
-      </c>
-    </row>
-    <row r="89" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="N88" s="18">
+        <v>43.4</v>
+      </c>
+      <c r="O88">
+        <v>44.39</v>
+      </c>
+      <c r="P88">
+        <v>31.54</v>
+      </c>
+    </row>
+    <row r="89" spans="1:16">
       <c r="A89" s="8" t="s">
         <v>87</v>
       </c>
@@ -5036,11 +5227,17 @@
       <c r="M89" s="15">
         <v>26.432732999999999</v>
       </c>
-      <c r="N89" s="18" t="s">
-        <v>228</v>
-      </c>
-    </row>
-    <row r="90" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="N89" s="18">
+        <v>26.3</v>
+      </c>
+      <c r="O89">
+        <v>46.6</v>
+      </c>
+      <c r="P89">
+        <v>33.090000000000003</v>
+      </c>
+    </row>
+    <row r="90" spans="1:16">
       <c r="A90" s="8" t="s">
         <v>88</v>
       </c>
@@ -5074,11 +5271,17 @@
       <c r="M90" s="15">
         <v>20.360968</v>
       </c>
-      <c r="N90" s="18" t="s">
-        <v>198</v>
-      </c>
-    </row>
-    <row r="91" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="N90" s="18">
+        <v>32.299999999999997</v>
+      </c>
+      <c r="O90">
+        <v>27</v>
+      </c>
+      <c r="P90">
+        <v>43.44</v>
+      </c>
+    </row>
+    <row r="91" spans="1:16">
       <c r="A91" s="8" t="s">
         <v>89</v>
       </c>
@@ -5119,11 +5322,17 @@
       <c r="M91" s="15">
         <v>36.090035</v>
       </c>
-      <c r="N91" s="18" t="s">
-        <v>212</v>
-      </c>
-    </row>
-    <row r="92" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="N91" s="18">
+        <v>31.9</v>
+      </c>
+      <c r="O91">
+        <v>61</v>
+      </c>
+      <c r="P91">
+        <v>9.36</v>
+      </c>
+    </row>
+    <row r="92" spans="1:16">
       <c r="A92" s="8" t="s">
         <v>90</v>
       </c>
@@ -5160,11 +5369,17 @@
       <c r="M92" s="15">
         <v>21.448879999999999</v>
       </c>
-      <c r="N92" s="18" t="s">
-        <v>229</v>
-      </c>
-    </row>
-    <row r="93" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="N92" s="18">
+        <v>40.700000000000003</v>
+      </c>
+      <c r="O92">
+        <v>56.8</v>
+      </c>
+      <c r="P92">
+        <v>22.71</v>
+      </c>
+    </row>
+    <row r="93" spans="1:16">
       <c r="A93" s="8" t="s">
         <v>91</v>
       </c>
@@ -5201,11 +5416,17 @@
       <c r="M93" s="15">
         <v>20.156713</v>
       </c>
-      <c r="N93" s="18" t="s">
-        <v>230</v>
-      </c>
-    </row>
-    <row r="94" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="N93" s="18">
+        <v>45.6</v>
+      </c>
+      <c r="O93">
+        <v>5.94</v>
+      </c>
+      <c r="P93">
+        <v>33.17</v>
+      </c>
+    </row>
+    <row r="94" spans="1:16">
       <c r="A94" s="8" t="s">
         <v>92</v>
       </c>
@@ -5242,11 +5463,17 @@
       <c r="M94" s="15">
         <v>8.3322769999999995</v>
       </c>
-      <c r="N94" s="18" t="s">
-        <v>209</v>
-      </c>
-    </row>
-    <row r="95" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="N94" s="18">
+        <v>38.1</v>
+      </c>
+      <c r="O94">
+        <v>2.1</v>
+      </c>
+      <c r="P94">
+        <v>37.46</v>
+      </c>
+    </row>
+    <row r="95" spans="1:16">
       <c r="A95" s="8" t="s">
         <v>93</v>
       </c>
@@ -5283,11 +5510,17 @@
       <c r="M95" s="15">
         <v>28.710813000000002</v>
       </c>
-      <c r="N95" s="18" t="s">
-        <v>231</v>
-      </c>
-    </row>
-    <row r="96" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="N95" s="18">
+        <v>59.1</v>
+      </c>
+      <c r="O95">
+        <v>14.84</v>
+      </c>
+      <c r="P95">
+        <v>37.090000000000003</v>
+      </c>
+    </row>
+    <row r="96" spans="1:16">
       <c r="A96" s="8" t="s">
         <v>94</v>
       </c>
@@ -5324,11 +5557,17 @@
       <c r="M96" s="15">
         <v>18.687477999999999</v>
       </c>
-      <c r="N96" s="18" t="s">
-        <v>232</v>
-      </c>
-    </row>
-    <row r="97" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="N96" s="18">
+        <v>32.799999999999997</v>
+      </c>
+      <c r="O96">
+        <v>15.44</v>
+      </c>
+      <c r="P96">
+        <v>4.93</v>
+      </c>
+    </row>
+    <row r="97" spans="1:16">
       <c r="A97" s="8" t="s">
         <v>95</v>
       </c>
@@ -5365,11 +5604,17 @@
       <c r="M97" s="15">
         <v>38.400931</v>
       </c>
-      <c r="N97" s="18" t="s">
-        <v>233</v>
-      </c>
-    </row>
-    <row r="98" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="N97" s="18">
+        <v>28.6</v>
+      </c>
+      <c r="O97">
+        <v>93.17</v>
+      </c>
+      <c r="P97">
+        <v>74.739999999999995</v>
+      </c>
+    </row>
+    <row r="98" spans="1:16">
       <c r="A98" s="8" t="s">
         <v>96</v>
       </c>
@@ -5411,13 +5656,19 @@
         <v>32.613869999999999</v>
       </c>
       <c r="N98" s="18"/>
-    </row>
-    <row r="99" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="O98">
+        <v>85.5</v>
+      </c>
+      <c r="P98">
+        <v>21.54</v>
+      </c>
+    </row>
+    <row r="99" spans="1:16">
       <c r="A99" s="8" t="s">
         <v>97</v>
       </c>
       <c r="B99" s="9">
-        <v>6.4763565063476563</v>
+        <v>6.4763565063476562</v>
       </c>
       <c r="C99" s="9">
         <f t="shared" si="1"/>
@@ -5445,11 +5696,17 @@
       <c r="M99" s="15">
         <v>23.448450000000001</v>
       </c>
-      <c r="N99" s="18" t="s">
-        <v>234</v>
-      </c>
-    </row>
-    <row r="100" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="N99" s="18">
+        <v>46.6</v>
+      </c>
+      <c r="O99">
+        <v>17.600000000000001</v>
+      </c>
+      <c r="P99">
+        <v>48.12</v>
+      </c>
+    </row>
+    <row r="100" spans="1:16">
       <c r="A100" s="8" t="s">
         <v>98</v>
       </c>
@@ -5486,11 +5743,17 @@
       <c r="M100" s="15">
         <v>13.454078000000001</v>
       </c>
-      <c r="N100" s="18" t="s">
-        <v>181</v>
-      </c>
-    </row>
-    <row r="101" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="N100" s="18">
+        <v>34</v>
+      </c>
+      <c r="O100">
+        <v>1.95</v>
+      </c>
+      <c r="P100">
+        <v>18.190000000000001</v>
+      </c>
+    </row>
+    <row r="101" spans="1:16">
       <c r="A101" s="8" t="s">
         <v>99</v>
       </c>
@@ -5527,11 +5790,17 @@
       <c r="M101" s="15">
         <v>7.1707000000000001</v>
       </c>
-      <c r="N101" s="18" t="s">
-        <v>235</v>
-      </c>
-    </row>
-    <row r="102" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="N101" s="18">
+        <v>43</v>
+      </c>
+      <c r="O101">
+        <v>42.68</v>
+      </c>
+      <c r="P101">
+        <v>17.64</v>
+      </c>
+    </row>
+    <row r="102" spans="1:16">
       <c r="A102" s="8" t="s">
         <v>100</v>
       </c>
@@ -5572,11 +5841,17 @@
       <c r="M102" s="15">
         <v>38.709806999999998</v>
       </c>
-      <c r="N102" s="18" t="s">
-        <v>197</v>
-      </c>
-    </row>
-    <row r="103" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="N102" s="18">
+        <v>26.8</v>
+      </c>
+      <c r="O102">
+        <v>96.3</v>
+      </c>
+      <c r="P102">
+        <v>28.28</v>
+      </c>
+    </row>
+    <row r="103" spans="1:16">
       <c r="A103" s="8" t="s">
         <v>101</v>
       </c>
@@ -5613,11 +5888,17 @@
       <c r="M103" s="15">
         <v>9.9883570000000006</v>
       </c>
-      <c r="N103" s="18" t="s">
-        <v>236</v>
-      </c>
-    </row>
-    <row r="104" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="N103" s="18">
+        <v>30.7</v>
+      </c>
+      <c r="O103">
+        <v>13.8</v>
+      </c>
+      <c r="P103">
+        <v>11.68</v>
+      </c>
+    </row>
+    <row r="104" spans="1:16">
       <c r="A104" s="8" t="s">
         <v>102</v>
       </c>
@@ -5650,11 +5931,14 @@
       <c r="M104" s="15">
         <v>5.5946610000000003</v>
       </c>
-      <c r="N104" s="18" t="s">
-        <v>237</v>
-      </c>
-    </row>
-    <row r="105" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="N104" s="18">
+        <v>35.5</v>
+      </c>
+      <c r="O104">
+        <v>53.67</v>
+      </c>
+    </row>
+    <row r="105" spans="1:16">
       <c r="A105" s="8" t="s">
         <v>103</v>
       </c>
@@ -5691,11 +5975,17 @@
       <c r="M105" s="15">
         <v>15.463361000000001</v>
       </c>
-      <c r="N105" s="18" t="s">
-        <v>238</v>
-      </c>
-    </row>
-    <row r="106" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="N105" s="18">
+        <v>50.4</v>
+      </c>
+      <c r="O105">
+        <v>44.92</v>
+      </c>
+      <c r="P105">
+        <v>13.7</v>
+      </c>
+    </row>
+    <row r="106" spans="1:16">
       <c r="A106" s="8" t="s">
         <v>104</v>
       </c>
@@ -5732,11 +6022,17 @@
       <c r="M106" s="15">
         <v>10.489746</v>
       </c>
-      <c r="N106" s="18" t="s">
-        <v>239</v>
-      </c>
-    </row>
-    <row r="107" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="N106" s="18">
+        <v>47.9</v>
+      </c>
+      <c r="O106">
+        <v>43</v>
+      </c>
+      <c r="P106">
+        <v>31.25</v>
+      </c>
+    </row>
+    <row r="107" spans="1:16">
       <c r="A107" s="8" t="s">
         <v>105</v>
       </c>
@@ -5773,11 +6069,17 @@
       <c r="M107" s="15">
         <v>13.614037</v>
       </c>
-      <c r="N107" s="18" t="s">
-        <v>240</v>
-      </c>
-    </row>
-    <row r="108" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="N107" s="18">
+        <v>43.8</v>
+      </c>
+      <c r="O107">
+        <v>40.200000000000003</v>
+      </c>
+      <c r="P107">
+        <v>18.920000000000002</v>
+      </c>
+    </row>
+    <row r="108" spans="1:16">
       <c r="A108" s="8" t="s">
         <v>106</v>
       </c>
@@ -5814,11 +6116,17 @@
       <c r="M108" s="15">
         <v>13.676774</v>
       </c>
-      <c r="N108" s="18" t="s">
-        <v>241</v>
-      </c>
-    </row>
-    <row r="109" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="N108" s="18">
+        <v>40.1</v>
+      </c>
+      <c r="O108">
+        <v>39.69</v>
+      </c>
+      <c r="P108">
+        <v>27.24</v>
+      </c>
+    </row>
+    <row r="109" spans="1:16">
       <c r="A109" s="8" t="s">
         <v>107</v>
       </c>
@@ -5859,11 +6167,17 @@
       <c r="M109" s="15">
         <v>33.346711999999997</v>
       </c>
-      <c r="N109" s="18" t="s">
-        <v>216</v>
-      </c>
-    </row>
-    <row r="110" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="N109" s="18">
+        <v>32.1</v>
+      </c>
+      <c r="O109">
+        <v>66.599999999999994</v>
+      </c>
+      <c r="P109">
+        <v>38.31</v>
+      </c>
+    </row>
+    <row r="110" spans="1:16">
       <c r="A110" s="8" t="s">
         <v>108</v>
       </c>
@@ -5904,11 +6218,17 @@
       <c r="M110" s="15">
         <v>34.141741000000003</v>
       </c>
-      <c r="N110" s="18" t="s">
-        <v>191</v>
-      </c>
-    </row>
-    <row r="111" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="N110" s="18">
+        <v>35.6</v>
+      </c>
+      <c r="O110">
+        <v>64.59</v>
+      </c>
+      <c r="P110">
+        <v>27.61</v>
+      </c>
+    </row>
+    <row r="111" spans="1:16">
       <c r="A111" s="8" t="s">
         <v>109</v>
       </c>
@@ -5949,16 +6269,22 @@
       <c r="M111" s="15">
         <v>26.441125</v>
       </c>
-      <c r="N111" s="18" t="s">
-        <v>242</v>
-      </c>
-    </row>
-    <row r="112" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="N111" s="18">
+        <v>27.5</v>
+      </c>
+      <c r="O111">
+        <v>54.08</v>
+      </c>
+      <c r="P111">
+        <v>34.44</v>
+      </c>
+    </row>
+    <row r="112" spans="1:16">
       <c r="A112" s="8" t="s">
         <v>110</v>
       </c>
       <c r="B112" s="9">
-        <v>5.5787429809570313</v>
+        <v>5.5787429809570312</v>
       </c>
       <c r="C112" s="9">
         <f t="shared" si="1"/>
@@ -5994,11 +6320,17 @@
       <c r="M112" s="15">
         <v>29.046813</v>
       </c>
-      <c r="N112" s="18" t="s">
-        <v>222</v>
-      </c>
-    </row>
-    <row r="113" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="N112" s="18">
+        <v>37.700000000000003</v>
+      </c>
+      <c r="O112">
+        <v>70.52</v>
+      </c>
+      <c r="P112">
+        <v>24.5</v>
+      </c>
+    </row>
+    <row r="113" spans="1:16">
       <c r="A113" s="8" t="s">
         <v>111</v>
       </c>
@@ -6035,11 +6367,17 @@
       <c r="M113" s="15">
         <v>15.459153000000001</v>
       </c>
-      <c r="N113" s="18" t="s">
-        <v>238</v>
-      </c>
-    </row>
-    <row r="114" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="N113" s="18">
+        <v>50.4</v>
+      </c>
+      <c r="O113">
+        <v>10.6</v>
+      </c>
+      <c r="P113">
+        <v>5.57</v>
+      </c>
+    </row>
+    <row r="114" spans="1:16">
       <c r="A114" s="8" t="s">
         <v>112</v>
       </c>
@@ -6076,11 +6414,17 @@
       <c r="M114" s="15">
         <v>2.23278</v>
       </c>
-      <c r="N114" s="18" t="s">
-        <v>243</v>
-      </c>
-    </row>
-    <row r="115" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="N114" s="18">
+        <v>45.9</v>
+      </c>
+      <c r="O114">
+        <v>63.7</v>
+      </c>
+      <c r="P114">
+        <v>46.39</v>
+      </c>
+    </row>
+    <row r="115" spans="1:16">
       <c r="A115" s="8" t="s">
         <v>113</v>
       </c>
@@ -6117,11 +6461,17 @@
       <c r="M115" s="15">
         <v>15.920230999999999</v>
       </c>
-      <c r="N115" s="18" t="s">
-        <v>244</v>
-      </c>
-    </row>
-    <row r="116" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="N115" s="18">
+        <v>40.299999999999997</v>
+      </c>
+      <c r="O115">
+        <v>17.7</v>
+      </c>
+      <c r="P115">
+        <v>17.96</v>
+      </c>
+    </row>
+    <row r="116" spans="1:16">
       <c r="A116" s="8" t="s">
         <v>114</v>
       </c>
@@ -6162,11 +6512,14 @@
       <c r="M116" s="15">
         <v>35.078639000000003</v>
       </c>
-      <c r="N116" s="18" t="s">
-        <v>245</v>
-      </c>
-    </row>
-    <row r="117" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="N116" s="18">
+        <v>29.1</v>
+      </c>
+      <c r="O116">
+        <v>53.5</v>
+      </c>
+    </row>
+    <row r="117" spans="1:16">
       <c r="A117" s="8" t="s">
         <v>115</v>
       </c>
@@ -6198,11 +6551,17 @@
       <c r="M117" s="15">
         <v>11.178661</v>
       </c>
-      <c r="N117" s="18" t="s">
-        <v>181</v>
-      </c>
-    </row>
-    <row r="118" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="N117" s="18">
+        <v>34</v>
+      </c>
+      <c r="O117">
+        <v>2.1</v>
+      </c>
+      <c r="P117">
+        <v>43.42</v>
+      </c>
+    </row>
+    <row r="118" spans="1:16">
       <c r="A118" s="8" t="s">
         <v>116</v>
       </c>
@@ -6244,8 +6603,14 @@
         <v>13.421915</v>
       </c>
       <c r="N118" s="18"/>
-    </row>
-    <row r="119" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="O118">
+        <v>82</v>
+      </c>
+      <c r="P118">
+        <v>133.76</v>
+      </c>
+    </row>
+    <row r="119" spans="1:16">
       <c r="A119" s="8" t="s">
         <v>117</v>
       </c>
@@ -6286,11 +6651,17 @@
       <c r="M119" s="15">
         <v>32.356543000000002</v>
       </c>
-      <c r="N119" s="18" t="s">
-        <v>246</v>
-      </c>
-    </row>
-    <row r="120" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="N119" s="18">
+        <v>26.1</v>
+      </c>
+      <c r="O119">
+        <v>79.98</v>
+      </c>
+      <c r="P119">
+        <v>81.709999999999994</v>
+      </c>
+    </row>
+    <row r="120" spans="1:16">
       <c r="A120" s="8" t="s">
         <v>118</v>
       </c>
@@ -6331,11 +6702,17 @@
       <c r="M120" s="15">
         <v>36.505336999999997</v>
       </c>
-      <c r="N120" s="18" t="s">
-        <v>247</v>
-      </c>
-    </row>
-    <row r="121" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="N120" s="18">
+        <v>25.7</v>
+      </c>
+      <c r="O120">
+        <v>71.59</v>
+      </c>
+      <c r="P120">
+        <v>72.790000000000006</v>
+      </c>
+    </row>
+    <row r="121" spans="1:16">
       <c r="A121" s="8" t="s">
         <v>119</v>
       </c>
@@ -6376,11 +6753,17 @@
       <c r="M121" s="15">
         <v>29.305698</v>
       </c>
-      <c r="N121" s="18" t="s">
-        <v>248</v>
-      </c>
-    </row>
-    <row r="122" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="N121" s="18">
+        <v>63</v>
+      </c>
+      <c r="O121">
+        <v>49</v>
+      </c>
+      <c r="P121">
+        <v>34.75</v>
+      </c>
+    </row>
+    <row r="122" spans="1:16">
       <c r="A122" s="8" t="s">
         <v>120</v>
       </c>
@@ -6421,11 +6804,17 @@
       <c r="M122" s="15">
         <v>26.236792000000001</v>
       </c>
-      <c r="N122" s="18" t="s">
-        <v>249</v>
-      </c>
-    </row>
-    <row r="123" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="N122" s="18">
+        <v>31.6</v>
+      </c>
+      <c r="O122">
+        <v>84.33</v>
+      </c>
+      <c r="P122">
+        <v>41.87</v>
+      </c>
+    </row>
+    <row r="123" spans="1:16">
       <c r="A123" s="8" t="s">
         <v>121</v>
       </c>
@@ -6453,11 +6842,14 @@
         <v>1.9170053039999999</v>
       </c>
       <c r="M123" s="15"/>
-      <c r="N123" s="18" t="s">
-        <v>215</v>
-      </c>
-    </row>
-    <row r="124" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="N123" s="18">
+        <v>45.5</v>
+      </c>
+      <c r="O123">
+        <v>15.9</v>
+      </c>
+    </row>
+    <row r="124" spans="1:16">
       <c r="A124" s="8" t="s">
         <v>122</v>
       </c>
@@ -6498,11 +6890,17 @@
       <c r="M124" s="15">
         <v>33.180988999999997</v>
       </c>
-      <c r="N124" s="18" t="s">
-        <v>250</v>
-      </c>
-    </row>
-    <row r="125" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="N124" s="18">
+        <v>36</v>
+      </c>
+      <c r="O124">
+        <v>76.19</v>
+      </c>
+      <c r="P124">
+        <v>22.94</v>
+      </c>
+    </row>
+    <row r="125" spans="1:16">
       <c r="A125" s="8" t="s">
         <v>123</v>
       </c>
@@ -6539,11 +6937,17 @@
       <c r="M125" s="15">
         <v>12.444495999999999</v>
       </c>
-      <c r="N125" s="18" t="s">
-        <v>251</v>
-      </c>
-    </row>
-    <row r="126" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="N125" s="18">
+        <v>39.799999999999997</v>
+      </c>
+      <c r="O125">
+        <v>25.8</v>
+      </c>
+      <c r="P125">
+        <v>13.62</v>
+      </c>
+    </row>
+    <row r="126" spans="1:16">
       <c r="A126" s="8" t="s">
         <v>124</v>
       </c>
@@ -6580,11 +6984,17 @@
       <c r="M126" s="15">
         <v>44.237478000000003</v>
       </c>
-      <c r="N126" s="18" t="s">
-        <v>252</v>
-      </c>
-    </row>
-    <row r="127" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="N126" s="18">
+        <v>27.2</v>
+      </c>
+      <c r="O126">
+        <v>92.52</v>
+      </c>
+      <c r="P126">
+        <v>29.58</v>
+      </c>
+    </row>
+    <row r="127" spans="1:16">
       <c r="A127" s="8" t="s">
         <v>125</v>
       </c>
@@ -6625,11 +7035,17 @@
       <c r="M127" s="15">
         <v>27.700901999999999</v>
       </c>
-      <c r="N127" s="18" t="s">
-        <v>253</v>
-      </c>
-    </row>
-    <row r="128" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="N127" s="18">
+        <v>32.5</v>
+      </c>
+      <c r="O127">
+        <v>87</v>
+      </c>
+      <c r="P127">
+        <v>42.51</v>
+      </c>
+    </row>
+    <row r="128" spans="1:16">
       <c r="A128" s="8" t="s">
         <v>126</v>
       </c>
@@ -6659,8 +7075,11 @@
       </c>
       <c r="M128" s="15"/>
       <c r="N128" s="18"/>
-    </row>
-    <row r="129" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="O128">
+        <v>83.99</v>
+      </c>
+    </row>
+    <row r="129" spans="1:16">
       <c r="A129" s="8" t="s">
         <v>127</v>
       </c>
@@ -6695,11 +7114,17 @@
       <c r="M129" s="15">
         <v>20.6</v>
       </c>
-      <c r="N129" s="18" t="s">
-        <v>181</v>
-      </c>
-    </row>
-    <row r="130" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="N129" s="18">
+        <v>34</v>
+      </c>
+      <c r="O129">
+        <v>17.489999999999998</v>
+      </c>
+      <c r="P129">
+        <v>8.8000000000000007</v>
+      </c>
+    </row>
+    <row r="130" spans="1:16">
       <c r="A130" s="8" t="s">
         <v>128</v>
       </c>
@@ -6736,11 +7161,17 @@
       <c r="M130" s="15">
         <v>11.390269</v>
       </c>
-      <c r="N130" s="18" t="s">
-        <v>254</v>
-      </c>
-    </row>
-    <row r="131" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="N130" s="18">
+        <v>37.799999999999997</v>
+      </c>
+      <c r="O130">
+        <v>4.8600000000000003</v>
+      </c>
+      <c r="P130">
+        <v>8.51</v>
+      </c>
+    </row>
+    <row r="131" spans="1:16">
       <c r="A131" s="8" t="s">
         <v>129</v>
       </c>
@@ -6781,11 +7212,17 @@
       <c r="M131" s="15">
         <v>17.834917999999998</v>
       </c>
-      <c r="N131" s="18" t="s">
-        <v>200</v>
-      </c>
-    </row>
-    <row r="132" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="N131" s="18">
+        <v>36.5</v>
+      </c>
+      <c r="O131">
+        <v>34.89</v>
+      </c>
+      <c r="P131">
+        <v>60.39</v>
+      </c>
+    </row>
+    <row r="132" spans="1:16">
       <c r="A132" s="8" t="s">
         <v>130</v>
       </c>
@@ -6822,11 +7259,17 @@
       <c r="M132" s="15">
         <v>18.763441</v>
       </c>
-      <c r="N132" s="18" t="s">
-        <v>235</v>
-      </c>
-    </row>
-    <row r="133" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="N132" s="18">
+        <v>43</v>
+      </c>
+      <c r="O132">
+        <v>5.7</v>
+      </c>
+      <c r="P132">
+        <v>43.48</v>
+      </c>
+    </row>
+    <row r="133" spans="1:16">
       <c r="A133" s="8" t="s">
         <v>131</v>
       </c>
@@ -6861,11 +7304,17 @@
       <c r="M133" s="15">
         <v>26.147864999999999</v>
       </c>
-      <c r="N133" s="18" t="s">
-        <v>244</v>
-      </c>
-    </row>
-    <row r="134" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="N133" s="18">
+        <v>40.299999999999997</v>
+      </c>
+      <c r="O133">
+        <v>65.099999999999994</v>
+      </c>
+      <c r="P133">
+        <v>69.27</v>
+      </c>
+    </row>
+    <row r="134" spans="1:16">
       <c r="A134" s="8" t="s">
         <v>132</v>
       </c>
@@ -6902,11 +7351,17 @@
       <c r="M134" s="15">
         <v>29.614932</v>
       </c>
-      <c r="N134" s="18" t="s">
-        <v>203</v>
-      </c>
-    </row>
-    <row r="135" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="N134" s="18">
+        <v>35.799999999999997</v>
+      </c>
+      <c r="O134">
+        <v>46.16</v>
+      </c>
+      <c r="P134">
+        <v>35.43</v>
+      </c>
+    </row>
+    <row r="135" spans="1:16">
       <c r="A135" s="8" t="s">
         <v>133</v>
       </c>
@@ -6943,11 +7398,17 @@
       <c r="M135" s="15">
         <v>25.301887000000001</v>
       </c>
-      <c r="N135" s="18" t="s">
-        <v>255</v>
-      </c>
-    </row>
-    <row r="136" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="N135" s="18">
+        <v>41.9</v>
+      </c>
+      <c r="O135">
+        <v>51.04</v>
+      </c>
+      <c r="P135">
+        <v>20.3</v>
+      </c>
+    </row>
+    <row r="136" spans="1:16">
       <c r="A136" s="8" t="s">
         <v>134</v>
       </c>
@@ -6982,11 +7443,17 @@
       <c r="M136" s="15">
         <v>20.373964000000001</v>
       </c>
-      <c r="N136" s="18" t="s">
-        <v>256</v>
-      </c>
-    </row>
-    <row r="137" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="N136" s="18">
+        <v>43.2</v>
+      </c>
+      <c r="O136">
+        <v>12.2</v>
+      </c>
+      <c r="P136">
+        <v>30.72</v>
+      </c>
+    </row>
+    <row r="137" spans="1:16">
       <c r="A137" s="8" t="s">
         <v>135</v>
       </c>
@@ -7023,11 +7490,17 @@
       <c r="M137" s="15">
         <v>12.676283</v>
       </c>
-      <c r="N137" s="18" t="s">
-        <v>202</v>
-      </c>
-    </row>
-    <row r="138" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="N137" s="18">
+        <v>42.8</v>
+      </c>
+      <c r="O137">
+        <v>17.71</v>
+      </c>
+      <c r="P137">
+        <v>8.41</v>
+      </c>
+    </row>
+    <row r="138" spans="1:16">
       <c r="A138" s="8" t="s">
         <v>136</v>
       </c>
@@ -7064,11 +7537,17 @@
       <c r="M138" s="15">
         <v>30.859074</v>
       </c>
-      <c r="N138" s="18" t="s">
-        <v>257</v>
-      </c>
-    </row>
-    <row r="139" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="N138" s="18">
+        <v>25.5</v>
+      </c>
+      <c r="O138">
+        <v>43.4</v>
+      </c>
+      <c r="P138">
+        <v>44.92</v>
+      </c>
+    </row>
+    <row r="139" spans="1:16">
       <c r="A139" s="8" t="s">
         <v>137</v>
       </c>
@@ -7106,8 +7585,14 @@
         <v>9.2430889999999994</v>
       </c>
       <c r="N139" s="18"/>
-    </row>
-    <row r="140" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="O139">
+        <v>90.4</v>
+      </c>
+      <c r="P139">
+        <v>89.87</v>
+      </c>
+    </row>
+    <row r="140" spans="1:16">
       <c r="A140" s="8" t="s">
         <v>138</v>
       </c>
@@ -7148,11 +7633,17 @@
       <c r="M140" s="15">
         <v>32.734135000000002</v>
       </c>
-      <c r="N140" s="18" t="s">
-        <v>258</v>
-      </c>
-    </row>
-    <row r="141" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="N140" s="18">
+        <v>34.1</v>
+      </c>
+      <c r="O140">
+        <v>91.61</v>
+      </c>
+      <c r="P140">
+        <v>15.45</v>
+      </c>
+    </row>
+    <row r="141" spans="1:16">
       <c r="A141" s="8" t="s">
         <v>139</v>
       </c>
@@ -7189,11 +7680,17 @@
       <c r="M141" s="15">
         <v>25.773724000000001</v>
       </c>
-      <c r="N141" s="18" t="s">
-        <v>259</v>
-      </c>
-    </row>
-    <row r="142" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="N141" s="18">
+        <v>41.5</v>
+      </c>
+      <c r="O141">
+        <v>87.36</v>
+      </c>
+      <c r="P141">
+        <v>9.34</v>
+      </c>
+    </row>
+    <row r="142" spans="1:16">
       <c r="A142" s="8" t="s">
         <v>140</v>
       </c>
@@ -7234,11 +7731,17 @@
       <c r="M142" s="15">
         <v>34.229075999999999</v>
       </c>
-      <c r="N142" s="18" t="s">
-        <v>260</v>
-      </c>
-    </row>
-    <row r="143" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="N142" s="18">
+        <v>39.700000000000003</v>
+      </c>
+      <c r="O142">
+        <v>61.46</v>
+      </c>
+      <c r="P142">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="143" spans="1:16">
       <c r="A143" s="8" t="s">
         <v>141</v>
       </c>
@@ -7275,11 +7778,17 @@
       <c r="M143" s="15">
         <v>26.204868999999999</v>
       </c>
-      <c r="N143" s="18" t="s">
-        <v>261</v>
-      </c>
-    </row>
-    <row r="144" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="N143" s="18">
+        <v>36.700000000000003</v>
+      </c>
+      <c r="O143">
+        <v>43.55</v>
+      </c>
+      <c r="P143">
+        <v>21.07</v>
+      </c>
+    </row>
+    <row r="144" spans="1:16">
       <c r="A144" s="8" t="s">
         <v>142</v>
       </c>
@@ -7314,11 +7823,17 @@
       <c r="M144" s="15">
         <v>20.279105000000001</v>
       </c>
-      <c r="N144" s="18" t="s">
-        <v>176</v>
-      </c>
-    </row>
-    <row r="145" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="N144" s="18">
+        <v>46.9</v>
+      </c>
+      <c r="O144">
+        <v>57</v>
+      </c>
+      <c r="P144">
+        <v>23.96</v>
+      </c>
+    </row>
+    <row r="145" spans="1:16">
       <c r="A145" s="8" t="s">
         <v>143</v>
       </c>
@@ -7355,11 +7870,17 @@
       <c r="M145" s="15">
         <v>17.944656999999999</v>
       </c>
-      <c r="N145" s="18" t="s">
-        <v>178</v>
-      </c>
-    </row>
-    <row r="146" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="N145" s="18">
+        <v>35.299999999999997</v>
+      </c>
+      <c r="O145">
+        <v>48.31</v>
+      </c>
+      <c r="P145">
+        <v>85.95</v>
+      </c>
+    </row>
+    <row r="146" spans="1:16">
       <c r="A146" s="8" t="s">
         <v>144</v>
       </c>
@@ -7394,16 +7915,22 @@
       <c r="M146" s="15">
         <v>7.0387729999999999</v>
       </c>
-      <c r="N146" s="18" t="s">
-        <v>261</v>
-      </c>
-    </row>
-    <row r="147" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="N146" s="18">
+        <v>36.700000000000003</v>
+      </c>
+      <c r="O146">
+        <v>22.55</v>
+      </c>
+      <c r="P146">
+        <v>29.56</v>
+      </c>
+    </row>
+    <row r="147" spans="1:16">
       <c r="A147" s="8" t="s">
         <v>145</v>
       </c>
       <c r="B147" s="9">
-        <v>3.9327774047851563</v>
+        <v>3.9327774047851562</v>
       </c>
       <c r="C147" s="9">
         <f t="shared" si="2"/>
@@ -7433,11 +7960,17 @@
       <c r="M147" s="15">
         <v>12.970041</v>
       </c>
-      <c r="N147" s="18" t="s">
-        <v>262</v>
-      </c>
-    </row>
-    <row r="148" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="N147" s="18">
+        <v>57.1</v>
+      </c>
+      <c r="O147">
+        <v>17.34</v>
+      </c>
+      <c r="P147">
+        <v>35.72</v>
+      </c>
+    </row>
+    <row r="148" spans="1:16">
       <c r="A148" s="8" t="s">
         <v>146</v>
       </c>
@@ -7474,8 +8007,14 @@
       <c r="M148" s="15">
         <v>27.182075999999999</v>
       </c>
-      <c r="N148" s="18" t="s">
-        <v>256</v>
+      <c r="N148" s="18">
+        <v>43.2</v>
+      </c>
+      <c r="O148">
+        <v>19.89</v>
+      </c>
+      <c r="P148">
+        <v>24.22</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added arable land file and arable data in total data
</commit_message>
<xml_diff>
--- a/data_tables/Total_data_cleaned.xlsx
+++ b/data_tables/Total_data_cleaned.xlsx
@@ -1,31 +1,37 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10312"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22026"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ulrikaeriksson/Documents/Data_Mining/DataMining-Group23/data_tables/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Simon\Documents\projects\datamining\DataMining-Group23\data_tables\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3F0785A5-EFD7-FC49-9C3C-06175E1673C0}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{067DB9A7-5A9E-4E8E-8A63-5BC4C34CF2DB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="19420" windowHeight="13380" xr2:uid="{196242FC-4F62-234C-ABAE-90D7B6224D3F}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{196242FC-4F62-234C-ABAE-90D7B6224D3F}"/>
   </bookViews>
   <sheets>
     <sheet name="Blad1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="163" uniqueCount="163">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="164" uniqueCount="164">
   <si>
     <t>Afghanistan</t>
   </si>
@@ -514,13 +520,16 @@
   </si>
   <si>
     <t>Total value of export (% of GDP)</t>
+  </si>
+  <si>
+    <t>Arable land</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -991,13 +1000,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{67CF83BE-F021-5E44-A4B8-2C5D9BB127DA}">
-  <dimension ref="A1:P148"/>
+  <dimension ref="A1:Q148"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="I1" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="O7" sqref="O7"/>
+    <sheetView tabSelected="1" topLeftCell="K1" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="R1" sqref="R1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="16"/>
+  <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="12.1640625" style="8" customWidth="1"/>
     <col min="2" max="2" width="17.1640625" style="9" customWidth="1"/>
@@ -1010,9 +1019,12 @@
     <col min="9" max="9" width="14.6640625" customWidth="1"/>
     <col min="13" max="13" width="21.5" customWidth="1"/>
     <col min="14" max="14" width="10.6640625" style="19"/>
+    <col min="15" max="15" width="24.9140625" customWidth="1"/>
+    <col min="16" max="16" width="26.33203125" customWidth="1"/>
+    <col min="17" max="17" width="14.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" ht="34">
+    <row r="1" spans="1:17" ht="31" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>147</v>
       </c>
@@ -1061,8 +1073,11 @@
       <c r="P1" s="17" t="s">
         <v>162</v>
       </c>
-    </row>
-    <row r="2" spans="1:16">
+      <c r="Q1" s="17" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="2" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A2" s="8" t="s">
         <v>0</v>
       </c>
@@ -1105,8 +1120,11 @@
       <c r="P2">
         <v>3.66</v>
       </c>
-    </row>
-    <row r="3" spans="1:16">
+      <c r="Q2">
+        <v>11.838679042980118</v>
+      </c>
+    </row>
+    <row r="3" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A3" s="8" t="s">
         <v>1</v>
       </c>
@@ -1152,8 +1170,11 @@
       <c r="P3">
         <v>17.61</v>
       </c>
-    </row>
-    <row r="4" spans="1:16">
+      <c r="Q3">
+        <v>22.63868568587478</v>
+      </c>
+    </row>
+    <row r="4" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A4" s="8" t="s">
         <v>2</v>
       </c>
@@ -1199,8 +1220,11 @@
       <c r="P4">
         <v>29.5</v>
       </c>
-    </row>
-    <row r="5" spans="1:16">
+      <c r="Q4">
+        <v>3.1087357122576353</v>
+      </c>
+    </row>
+    <row r="5" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A5" s="8" t="s">
         <v>3</v>
       </c>
@@ -1250,8 +1274,11 @@
       <c r="P5">
         <v>13.49</v>
       </c>
-    </row>
-    <row r="6" spans="1:16">
+      <c r="Q5">
+        <v>14.3238729998648</v>
+      </c>
+    </row>
+    <row r="6" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A6" s="8" t="s">
         <v>4</v>
       </c>
@@ -1297,8 +1324,11 @@
       <c r="P6">
         <v>13.47</v>
       </c>
-    </row>
-    <row r="7" spans="1:16">
+      <c r="Q6">
+        <v>15.679662588566348</v>
+      </c>
+    </row>
+    <row r="7" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A7" s="8" t="s">
         <v>5</v>
       </c>
@@ -1348,8 +1378,11 @@
       <c r="P7">
         <v>16.88</v>
       </c>
-    </row>
-    <row r="8" spans="1:16">
+      <c r="Q7">
+        <v>5.986463893749626</v>
+      </c>
+    </row>
+    <row r="8" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A8" s="8" t="s">
         <v>6</v>
       </c>
@@ -1399,8 +1432,11 @@
       <c r="P8">
         <v>41.32</v>
       </c>
-    </row>
-    <row r="9" spans="1:16">
+      <c r="Q8">
+        <v>16.29230665457256</v>
+      </c>
+    </row>
+    <row r="9" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A9" s="8" t="s">
         <v>7</v>
       </c>
@@ -1450,8 +1486,11 @@
       <c r="P9">
         <v>39.1</v>
       </c>
-    </row>
-    <row r="10" spans="1:16">
+      <c r="Q9">
+        <v>24.180476593685736</v>
+      </c>
+    </row>
+    <row r="10" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A10" s="8" t="s">
         <v>8</v>
       </c>
@@ -1493,8 +1532,11 @@
       <c r="P10">
         <v>109.52</v>
       </c>
-    </row>
-    <row r="11" spans="1:16">
+      <c r="Q10">
+        <v>2.0565552198981694</v>
+      </c>
+    </row>
+    <row r="11" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A11" s="8" t="s">
         <v>9</v>
       </c>
@@ -1540,8 +1582,11 @@
       <c r="P11">
         <v>17.649999999999999</v>
       </c>
-    </row>
-    <row r="12" spans="1:16">
+      <c r="Q11">
+        <v>59.646692486267959</v>
+      </c>
+    </row>
+    <row r="12" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A12" s="8" t="s">
         <v>10</v>
       </c>
@@ -1591,8 +1636,11 @@
       <c r="P12">
         <v>47.36</v>
       </c>
-    </row>
-    <row r="13" spans="1:16">
+      <c r="Q12">
+        <v>28.000667950481215</v>
+      </c>
+    </row>
+    <row r="13" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A13" s="8" t="s">
         <v>11</v>
       </c>
@@ -1642,8 +1690,11 @@
       <c r="P13">
         <v>86.17</v>
       </c>
-    </row>
-    <row r="14" spans="1:16">
+      <c r="Q13">
+        <v>28.051519960834316</v>
+      </c>
+    </row>
+    <row r="14" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A14" s="8" t="s">
         <v>12</v>
       </c>
@@ -1689,8 +1740,11 @@
       <c r="P14">
         <v>20.99</v>
       </c>
-    </row>
-    <row r="15" spans="1:16">
+      <c r="Q14">
+        <v>23.944661227385598</v>
+      </c>
+    </row>
+    <row r="15" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A15" s="8" t="s">
         <v>13</v>
       </c>
@@ -1738,8 +1792,11 @@
       <c r="P15">
         <v>39.04</v>
       </c>
-    </row>
-    <row r="16" spans="1:16">
+      <c r="Q15">
+        <v>4.110588018092864</v>
+      </c>
+    </row>
+    <row r="16" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A16" s="8" t="s">
         <v>14</v>
       </c>
@@ -1785,8 +1842,11 @@
       <c r="P16">
         <v>31.81</v>
       </c>
-    </row>
-    <row r="17" spans="1:16">
+      <c r="Q16">
+        <v>20.0390625</v>
+      </c>
+    </row>
+    <row r="17" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A17" s="8" t="s">
         <v>15</v>
       </c>
@@ -1832,8 +1892,11 @@
       <c r="P17">
         <v>49.12</v>
       </c>
-    </row>
-    <row r="18" spans="1:16">
+      <c r="Q17">
+        <v>0.45806646216631558</v>
+      </c>
+    </row>
+    <row r="18" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A18" s="8" t="s">
         <v>16</v>
       </c>
@@ -1883,8 +1946,11 @@
       <c r="P18">
         <v>9.98</v>
       </c>
-    </row>
-    <row r="19" spans="1:16">
+      <c r="Q18">
+        <v>9.6882799283094077</v>
+      </c>
+    </row>
+    <row r="19" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A19" s="8" t="s">
         <v>17</v>
       </c>
@@ -1934,8 +2000,11 @@
       <c r="P19">
         <v>50.77</v>
       </c>
-    </row>
-    <row r="20" spans="1:16">
+      <c r="Q19">
+        <v>32.20338983050847</v>
+      </c>
+    </row>
+    <row r="20" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A20" s="8" t="s">
         <v>18</v>
       </c>
@@ -1985,8 +2054,11 @@
       <c r="P20">
         <v>19.41</v>
       </c>
-    </row>
-    <row r="21" spans="1:16">
+      <c r="Q20">
+        <v>21.929824561403507</v>
+      </c>
+    </row>
+    <row r="21" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A21" s="8" t="s">
         <v>19</v>
       </c>
@@ -2032,8 +2104,11 @@
       <c r="P21">
         <v>69.849999999999994</v>
       </c>
-    </row>
-    <row r="22" spans="1:16">
+      <c r="Q21">
+        <v>21.527305687740768</v>
+      </c>
+    </row>
+    <row r="22" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A22" s="8" t="s">
         <v>20</v>
       </c>
@@ -2077,8 +2152,11 @@
       <c r="P22">
         <v>17.920000000000002</v>
       </c>
-    </row>
-    <row r="23" spans="1:16">
+      <c r="Q22">
+        <v>13.115863848871401</v>
+      </c>
+    </row>
+    <row r="23" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A23" s="8" t="s">
         <v>21</v>
       </c>
@@ -2128,8 +2206,11 @@
       <c r="P23">
         <v>26.61</v>
       </c>
-    </row>
-    <row r="24" spans="1:16">
+      <c r="Q23">
+        <v>4.8128830341639253</v>
+      </c>
+    </row>
+    <row r="24" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A24" s="8" t="s">
         <v>22</v>
       </c>
@@ -2170,13 +2251,16 @@
       <c r="P24">
         <v>5.92</v>
       </c>
-    </row>
-    <row r="25" spans="1:16">
+      <c r="Q24">
+        <v>2.889338341519792</v>
+      </c>
+    </row>
+    <row r="25" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A25" s="8" t="s">
         <v>23</v>
       </c>
       <c r="B25" s="9">
-        <v>4.5589370727539062</v>
+        <v>4.5589370727539063</v>
       </c>
       <c r="C25" s="9">
         <f t="shared" si="0"/>
@@ -2215,8 +2299,11 @@
       <c r="P25">
         <v>30.17</v>
       </c>
-    </row>
-    <row r="26" spans="1:16">
+      <c r="Q25">
+        <v>3.8913595933926302</v>
+      </c>
+    </row>
+    <row r="26" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A26" s="8" t="s">
         <v>24</v>
       </c>
@@ -2262,8 +2349,11 @@
       <c r="P26">
         <v>29.85</v>
       </c>
-    </row>
-    <row r="27" spans="1:16">
+      <c r="Q26">
+        <v>1.7077946819498635</v>
+      </c>
+    </row>
+    <row r="27" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A27" s="8" t="s">
         <v>25</v>
       </c>
@@ -2310,8 +2400,11 @@
       <c r="P27">
         <v>22.89</v>
       </c>
-    </row>
-    <row r="28" spans="1:16">
+      <c r="Q27">
+        <v>12.664821089430253</v>
+      </c>
+    </row>
+    <row r="28" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A28" s="8" t="s">
         <v>26</v>
       </c>
@@ -2361,8 +2454,11 @@
       <c r="P28">
         <v>15.76</v>
       </c>
-    </row>
-    <row r="29" spans="1:16">
+      <c r="Q28">
+        <v>1.5219468008886345</v>
+      </c>
+    </row>
+    <row r="29" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A29" s="8" t="s">
         <v>27</v>
       </c>
@@ -2405,8 +2501,11 @@
       <c r="P29">
         <v>73.41</v>
       </c>
-    </row>
-    <row r="30" spans="1:16">
+      <c r="Q29">
+        <v>1.6105417276720351</v>
+      </c>
+    </row>
+    <row r="30" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A30" s="8" t="s">
         <v>28</v>
       </c>
@@ -2450,8 +2549,11 @@
       <c r="P30">
         <v>20.83</v>
       </c>
-    </row>
-    <row r="31" spans="1:16">
+      <c r="Q30">
+        <v>3.1318232945898852</v>
+      </c>
+    </row>
+    <row r="31" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A31" s="8" t="s">
         <v>29</v>
       </c>
@@ -2501,8 +2603,11 @@
       <c r="P31">
         <v>65.84</v>
       </c>
-    </row>
-    <row r="32" spans="1:16">
+      <c r="Q31">
+        <v>4.8472385428907163</v>
+      </c>
+    </row>
+    <row r="32" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A32" s="8" t="s">
         <v>30</v>
       </c>
@@ -2552,8 +2657,11 @@
       <c r="P32">
         <v>23.94</v>
       </c>
-    </row>
-    <row r="33" spans="1:16">
+      <c r="Q32">
+        <v>15.582558970693352</v>
+      </c>
+    </row>
+    <row r="33" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A33" s="8" t="s">
         <v>31</v>
       </c>
@@ -2603,8 +2711,11 @@
       <c r="P33">
         <v>16.059999999999999</v>
       </c>
-    </row>
-    <row r="34" spans="1:16">
+      <c r="Q33">
+        <v>9.1590906118417745</v>
+      </c>
+    </row>
+    <row r="34" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A34" s="8" t="s">
         <v>32</v>
       </c>
@@ -2650,8 +2761,11 @@
       <c r="P34">
         <v>83.7</v>
       </c>
-    </row>
-    <row r="35" spans="1:16">
+      <c r="Q34">
+        <v>32.297332297332296</v>
+      </c>
+    </row>
+    <row r="35" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A35" s="8" t="s">
         <v>33</v>
       </c>
@@ -2697,8 +2811,11 @@
       <c r="P35">
         <v>31.23</v>
       </c>
-    </row>
-    <row r="36" spans="1:16">
+      <c r="Q35">
+        <v>56.561085972850677</v>
+      </c>
+    </row>
+    <row r="36" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A36" s="8" t="s">
         <v>34</v>
       </c>
@@ -2748,8 +2865,11 @@
       <c r="P36">
         <v>16.440000000000001</v>
       </c>
-    </row>
-    <row r="37" spans="1:16">
+      <c r="Q36">
+        <v>16.559718484785758</v>
+      </c>
+    </row>
+    <row r="37" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A37" s="8" t="s">
         <v>35</v>
       </c>
@@ -2795,8 +2915,11 @@
       <c r="P37">
         <v>27.59</v>
       </c>
-    </row>
-    <row r="38" spans="1:16">
+      <c r="Q37">
+        <v>3.929779352552746</v>
+      </c>
+    </row>
+    <row r="38" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A38" s="8" t="s">
         <v>36</v>
       </c>
@@ -2840,8 +2963,11 @@
       <c r="P38">
         <v>10.57</v>
       </c>
-    </row>
-    <row r="39" spans="1:16">
+      <c r="Q38">
+        <v>2.7995077799299311</v>
+      </c>
+    </row>
+    <row r="39" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A39" s="8" t="s">
         <v>37</v>
       </c>
@@ -2887,8 +3013,11 @@
       <c r="P39">
         <v>21.38</v>
       </c>
-    </row>
-    <row r="40" spans="1:16">
+      <c r="Q39">
+        <v>35.569498069498067</v>
+      </c>
+    </row>
+    <row r="40" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A40" s="8" t="s">
         <v>38</v>
       </c>
@@ -2938,8 +3067,11 @@
       <c r="P40">
         <v>61.46</v>
       </c>
-    </row>
-    <row r="41" spans="1:16">
+      <c r="Q40">
+        <v>16.011042097998622</v>
+      </c>
+    </row>
+    <row r="41" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A41" s="8" t="s">
         <v>39</v>
       </c>
@@ -2983,8 +3115,11 @@
       <c r="P41">
         <v>4.68</v>
       </c>
-    </row>
-    <row r="42" spans="1:16">
+      <c r="Q41">
+        <v>15.119</v>
+      </c>
+    </row>
+    <row r="42" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A42" s="8" t="s">
         <v>40</v>
       </c>
@@ -3034,8 +3169,11 @@
       <c r="P42">
         <v>28.35</v>
       </c>
-    </row>
-    <row r="43" spans="1:16">
+      <c r="Q42">
+        <v>7.3903458260669286</v>
+      </c>
+    </row>
+    <row r="43" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A43" s="8" t="s">
         <v>41</v>
       </c>
@@ -3085,8 +3223,11 @@
       <c r="P43">
         <v>21.14</v>
       </c>
-    </row>
-    <row r="44" spans="1:16">
+      <c r="Q43">
+        <v>33.523304758729807</v>
+      </c>
+    </row>
+    <row r="44" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A44" s="8" t="s">
         <v>42</v>
       </c>
@@ -3127,8 +3268,11 @@
       <c r="P44">
         <v>51.19</v>
       </c>
-    </row>
-    <row r="45" spans="1:16">
+      <c r="Q44">
+        <v>1.2613032172934373</v>
+      </c>
+    </row>
+    <row r="45" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A45" s="8" t="s">
         <v>43</v>
       </c>
@@ -3171,8 +3315,11 @@
       <c r="P45">
         <v>13.04</v>
       </c>
-    </row>
-    <row r="46" spans="1:16">
+      <c r="Q45">
+        <v>43.478260869565219</v>
+      </c>
+    </row>
+    <row r="46" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A46" s="8" t="s">
         <v>44</v>
       </c>
@@ -3222,8 +3369,11 @@
       <c r="P46">
         <v>17.329999999999998</v>
       </c>
-    </row>
-    <row r="47" spans="1:16">
+      <c r="Q46">
+        <v>4.9503525687149237</v>
+      </c>
+    </row>
+    <row r="47" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A47" s="8" t="s">
         <v>45</v>
       </c>
@@ -3273,8 +3423,11 @@
       <c r="P47">
         <v>37.61</v>
       </c>
-    </row>
-    <row r="48" spans="1:16">
+      <c r="Q47">
+        <v>33.67013968399359</v>
+      </c>
+    </row>
+    <row r="48" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A48" s="8" t="s">
         <v>46</v>
       </c>
@@ -3324,8 +3477,11 @@
       <c r="P48">
         <v>25.55</v>
       </c>
-    </row>
-    <row r="49" spans="1:16">
+      <c r="Q48">
+        <v>20.655708886349654</v>
+      </c>
+    </row>
+    <row r="49" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A49" s="8" t="s">
         <v>47</v>
       </c>
@@ -3375,8 +3531,11 @@
       <c r="P49">
         <v>14.93</v>
       </c>
-    </row>
-    <row r="50" spans="1:16">
+      <c r="Q49">
+        <v>16.602017067494181</v>
+      </c>
+    </row>
+    <row r="50" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A50" s="8" t="s">
         <v>48</v>
       </c>
@@ -3420,8 +3579,11 @@
       <c r="P50">
         <v>19.440000000000001</v>
       </c>
-    </row>
-    <row r="51" spans="1:16">
+      <c r="Q50">
+        <v>8.0440462859275854</v>
+      </c>
+    </row>
+    <row r="51" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A51" s="8" t="s">
         <v>49</v>
       </c>
@@ -3465,8 +3627,11 @@
       <c r="P51">
         <v>37.67</v>
       </c>
-    </row>
-    <row r="52" spans="1:16">
+      <c r="Q51">
+        <v>12.615985674751752</v>
+      </c>
+    </row>
+    <row r="52" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A52" s="8" t="s">
         <v>50</v>
       </c>
@@ -3510,8 +3675,11 @@
       <c r="P52">
         <v>12.38</v>
       </c>
-    </row>
-    <row r="53" spans="1:16">
+      <c r="Q52">
+        <v>38.824383164005802</v>
+      </c>
+    </row>
+    <row r="53" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A53" s="8" t="s">
         <v>51</v>
       </c>
@@ -3557,8 +3725,11 @@
       <c r="P53">
         <v>44.73</v>
       </c>
-    </row>
-    <row r="54" spans="1:16">
+      <c r="Q53">
+        <v>9.1160961658772006</v>
+      </c>
+    </row>
+    <row r="54" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A54" s="8" t="s">
         <v>52</v>
       </c>
@@ -3592,8 +3763,11 @@
       <c r="P54">
         <v>162.75</v>
       </c>
-    </row>
-    <row r="55" spans="1:16">
+      <c r="Q54">
+        <v>2.8571428571428572</v>
+      </c>
+    </row>
+    <row r="55" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A55" s="8" t="s">
         <v>53</v>
       </c>
@@ -3643,8 +3817,11 @@
       <c r="P55">
         <v>78</v>
       </c>
-    </row>
-    <row r="56" spans="1:16">
+      <c r="Q55">
+        <v>47.763172429029048</v>
+      </c>
+    </row>
+    <row r="56" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A56" s="8" t="s">
         <v>54</v>
       </c>
@@ -3687,8 +3864,11 @@
       <c r="P56">
         <v>31.55</v>
       </c>
-    </row>
-    <row r="57" spans="1:16">
+      <c r="Q56">
+        <v>1.2069825436408979</v>
+      </c>
+    </row>
+    <row r="57" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A57" s="8" t="s">
         <v>55</v>
       </c>
@@ -3734,8 +3914,11 @@
       <c r="P57">
         <v>15.36</v>
       </c>
-    </row>
-    <row r="58" spans="1:16">
+      <c r="Q57">
+        <v>52.624622038954797</v>
+      </c>
+    </row>
+    <row r="58" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A58" s="8" t="s">
         <v>56</v>
       </c>
@@ -3781,8 +3964,11 @@
       <c r="P58">
         <v>21.86</v>
       </c>
-    </row>
-    <row r="59" spans="1:16">
+      <c r="Q58">
+        <v>12.9721733082354</v>
+      </c>
+    </row>
+    <row r="59" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A59" s="8" t="s">
         <v>57</v>
       </c>
@@ -3828,8 +4014,11 @@
       <c r="P59">
         <v>20.25</v>
       </c>
-    </row>
-    <row r="60" spans="1:16">
+      <c r="Q59">
+        <v>9.017289226159777</v>
+      </c>
+    </row>
+    <row r="60" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A60" s="8" t="s">
         <v>58</v>
       </c>
@@ -3873,8 +4062,11 @@
       <c r="P60">
         <v>37.549999999999997</v>
       </c>
-    </row>
-    <row r="61" spans="1:16">
+      <c r="Q60">
+        <v>11.517340300604381</v>
+      </c>
+    </row>
+    <row r="61" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A61" s="8" t="s">
         <v>59</v>
       </c>
@@ -3924,8 +4116,11 @@
       <c r="P61">
         <v>57.73</v>
       </c>
-    </row>
-    <row r="62" spans="1:16">
+      <c r="Q61">
+        <v>6.4740891275947163</v>
+      </c>
+    </row>
+    <row r="62" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A62" s="8" t="s">
         <v>60</v>
       </c>
@@ -3975,8 +4170,11 @@
       <c r="P62">
         <v>22.56</v>
       </c>
-    </row>
-    <row r="63" spans="1:16">
+      <c r="Q62">
+        <v>13.632162661737524</v>
+      </c>
+    </row>
+    <row r="63" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A63" s="8" t="s">
         <v>61</v>
       </c>
@@ -4026,8 +4224,11 @@
       <c r="P63">
         <v>24.39</v>
       </c>
-    </row>
-    <row r="64" spans="1:16">
+      <c r="Q63">
+        <v>22.445094172842865</v>
+      </c>
+    </row>
+    <row r="64" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A64" s="8" t="s">
         <v>62</v>
       </c>
@@ -4071,8 +4272,11 @@
       <c r="P64">
         <v>37.4</v>
       </c>
-    </row>
-    <row r="65" spans="1:16">
+      <c r="Q64">
+        <v>9.1194968553459113</v>
+      </c>
+    </row>
+    <row r="65" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A65" s="8" t="s">
         <v>63</v>
       </c>
@@ -4122,8 +4326,11 @@
       <c r="P65">
         <v>10.43</v>
       </c>
-    </row>
-    <row r="66" spans="1:16">
+      <c r="Q65">
+        <v>11.080332409972298</v>
+      </c>
+    </row>
+    <row r="66" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A66" s="8" t="s">
         <v>64</v>
       </c>
@@ -4173,13 +4380,16 @@
       <c r="P66">
         <v>15.6</v>
       </c>
-    </row>
-    <row r="67" spans="1:16">
+      <c r="Q66">
+        <v>11.476848804037743</v>
+      </c>
+    </row>
+    <row r="67" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A67" s="8" t="s">
         <v>65</v>
       </c>
       <c r="B67" s="9">
-        <v>4.8080825805664062</v>
+        <v>4.8080825805664063</v>
       </c>
       <c r="C67" s="9">
         <f t="shared" ref="C67:C130" si="1">ROUND(B67,0)</f>
@@ -4218,8 +4428,11 @@
       <c r="P67">
         <v>23.71</v>
       </c>
-    </row>
-    <row r="68" spans="1:16">
+      <c r="Q67">
+        <v>2.6724486878445144</v>
+      </c>
+    </row>
+    <row r="68" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A68" s="8" t="s">
         <v>66</v>
       </c>
@@ -4265,8 +4478,11 @@
       <c r="P68">
         <v>32.090000000000003</v>
       </c>
-    </row>
-    <row r="69" spans="1:16">
+      <c r="Q68">
+        <v>10.888246842241731</v>
+      </c>
+    </row>
+    <row r="69" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A69" s="8" t="s">
         <v>67</v>
       </c>
@@ -4312,8 +4528,11 @@
       <c r="P69">
         <v>11.93</v>
       </c>
-    </row>
-    <row r="70" spans="1:16">
+      <c r="Q69">
+        <v>10.190814210914713</v>
+      </c>
+    </row>
+    <row r="70" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A70" s="8" t="s">
         <v>68</v>
       </c>
@@ -4346,7 +4565,7 @@
         <v>26.5</v>
       </c>
     </row>
-    <row r="71" spans="1:16">
+    <row r="71" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A71" s="8" t="s">
         <v>69</v>
       </c>
@@ -4390,8 +4609,11 @@
       <c r="P71">
         <v>57.49</v>
       </c>
-    </row>
-    <row r="72" spans="1:16">
+      <c r="Q71">
+        <v>0.44893378226711567</v>
+      </c>
+    </row>
+    <row r="72" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A72" s="8" t="s">
         <v>70</v>
       </c>
@@ -4437,8 +4659,11 @@
       <c r="P72">
         <v>16.59</v>
       </c>
-    </row>
-    <row r="73" spans="1:16">
+      <c r="Q72">
+        <v>6.7153284671532854</v>
+      </c>
+    </row>
+    <row r="73" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A73" s="8" t="s">
         <v>71</v>
       </c>
@@ -4484,8 +4709,11 @@
       <c r="P73">
         <v>40</v>
       </c>
-    </row>
-    <row r="74" spans="1:16">
+      <c r="Q73">
+        <v>6.6074523396880416</v>
+      </c>
+    </row>
+    <row r="74" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A74" s="8" t="s">
         <v>72</v>
       </c>
@@ -4535,8 +4763,11 @@
       <c r="P74">
         <v>45.97</v>
       </c>
-    </row>
-    <row r="75" spans="1:16">
+      <c r="Q74">
+        <v>20.714055966548731</v>
+      </c>
+    </row>
+    <row r="75" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A75" s="8" t="s">
         <v>73</v>
       </c>
@@ -4580,8 +4811,11 @@
       <c r="P75">
         <v>7.61</v>
       </c>
-    </row>
-    <row r="76" spans="1:16">
+      <c r="Q75">
+        <v>12.903225806451612</v>
+      </c>
+    </row>
+    <row r="76" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A76" s="8" t="s">
         <v>74</v>
       </c>
@@ -4624,8 +4858,11 @@
       <c r="P76">
         <v>42.4</v>
       </c>
-    </row>
-    <row r="77" spans="1:16">
+      <c r="Q76">
+        <v>11.594202898550725</v>
+      </c>
+    </row>
+    <row r="77" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A77" s="8" t="s">
         <v>75</v>
       </c>
@@ -4669,8 +4906,11 @@
       <c r="P77">
         <v>48.32</v>
       </c>
-    </row>
-    <row r="78" spans="1:16">
+      <c r="Q77">
+        <v>5.191029900332226</v>
+      </c>
+    </row>
+    <row r="78" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A78" s="8" t="s">
         <v>76</v>
       </c>
@@ -4709,8 +4949,11 @@
       <c r="P78">
         <v>45.54</v>
       </c>
-    </row>
-    <row r="79" spans="1:16">
+      <c r="Q78">
+        <v>0.97752821760232789</v>
+      </c>
+    </row>
+    <row r="79" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A79" s="8" t="s">
         <v>77</v>
       </c>
@@ -4760,8 +5003,11 @@
       <c r="P79">
         <v>66.94</v>
       </c>
-    </row>
-    <row r="80" spans="1:16">
+      <c r="Q79">
+        <v>34.203889257236021</v>
+      </c>
+    </row>
+    <row r="80" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A80" s="8" t="s">
         <v>78</v>
       </c>
@@ -4811,8 +5057,11 @@
       <c r="P80">
         <v>42.35</v>
       </c>
-    </row>
-    <row r="81" spans="1:16">
+      <c r="Q80">
+        <v>25.456790374630287</v>
+      </c>
+    </row>
+    <row r="81" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A81" s="8" t="s">
         <v>79</v>
       </c>
@@ -4853,8 +5102,11 @@
       <c r="P81">
         <v>45.19</v>
       </c>
-    </row>
-    <row r="82" spans="1:16">
+      <c r="Q81">
+        <v>6.0158129941560672</v>
+      </c>
+    </row>
+    <row r="82" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A82" s="8" t="s">
         <v>80</v>
       </c>
@@ -4898,8 +5150,11 @@
       <c r="P82">
         <v>20.59</v>
       </c>
-    </row>
-    <row r="83" spans="1:16">
+      <c r="Q82">
+        <v>16.494845360824741</v>
+      </c>
+    </row>
+    <row r="83" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A83" s="8" t="s">
         <v>81</v>
       </c>
@@ -4945,8 +5200,11 @@
       <c r="P83">
         <v>18.329999999999998</v>
       </c>
-    </row>
-    <row r="84" spans="1:16">
+      <c r="Q83">
+        <v>40.305473058973277</v>
+      </c>
+    </row>
+    <row r="84" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A84" s="8" t="s">
         <v>82</v>
       </c>
@@ -4992,8 +5250,11 @@
       <c r="P84">
         <v>14.6</v>
       </c>
-    </row>
-    <row r="85" spans="1:16">
+      <c r="Q84">
+        <v>5.2540997713470849</v>
+      </c>
+    </row>
+    <row r="85" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A85" s="8" t="s">
         <v>83</v>
       </c>
@@ -5041,8 +5302,11 @@
       <c r="P85">
         <v>66.489999999999995</v>
       </c>
-    </row>
-    <row r="86" spans="1:16">
+      <c r="Q85">
+        <v>28.343749046325691</v>
+      </c>
+    </row>
+    <row r="86" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A86" s="8" t="s">
         <v>84</v>
       </c>
@@ -5086,8 +5350,11 @@
       <c r="P86">
         <v>48.86</v>
       </c>
-    </row>
-    <row r="87" spans="1:16">
+      <c r="Q86">
+        <v>0.43659648782380905</v>
+      </c>
+    </row>
+    <row r="87" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A87" s="8" t="s">
         <v>85</v>
       </c>
@@ -5134,8 +5401,11 @@
       <c r="P87">
         <v>22.48</v>
       </c>
-    </row>
-    <row r="88" spans="1:16">
+      <c r="Q87">
+        <v>36.945812807881772</v>
+      </c>
+    </row>
+    <row r="88" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A88" s="8" t="s">
         <v>86</v>
       </c>
@@ -5185,8 +5455,11 @@
       <c r="P88">
         <v>31.54</v>
       </c>
-    </row>
-    <row r="89" spans="1:16">
+      <c r="Q88">
+        <v>11.606265593250855</v>
+      </c>
+    </row>
+    <row r="89" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A89" s="8" t="s">
         <v>87</v>
       </c>
@@ -5236,8 +5509,11 @@
       <c r="P89">
         <v>33.090000000000003</v>
       </c>
-    </row>
-    <row r="90" spans="1:16">
+      <c r="Q89">
+        <v>55.557921825117958</v>
+      </c>
+    </row>
+    <row r="90" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A90" s="8" t="s">
         <v>88</v>
       </c>
@@ -5280,8 +5556,11 @@
       <c r="P90">
         <v>43.44</v>
       </c>
-    </row>
-    <row r="91" spans="1:16">
+      <c r="Q90">
+        <v>0.36509694650160346</v>
+      </c>
+    </row>
+    <row r="91" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A91" s="8" t="s">
         <v>89</v>
       </c>
@@ -5331,8 +5610,11 @@
       <c r="P91">
         <v>9.36</v>
       </c>
-    </row>
-    <row r="92" spans="1:16">
+      <c r="Q91">
+        <v>0.66914498141263945</v>
+      </c>
+    </row>
+    <row r="92" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A92" s="8" t="s">
         <v>90</v>
       </c>
@@ -5378,8 +5660,11 @@
       <c r="P92">
         <v>22.71</v>
       </c>
-    </row>
-    <row r="93" spans="1:16">
+      <c r="Q92">
+        <v>18.216446336544927</v>
+      </c>
+    </row>
+    <row r="93" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A93" s="8" t="s">
         <v>91</v>
       </c>
@@ -5425,8 +5710,11 @@
       <c r="P93">
         <v>33.17</v>
       </c>
-    </row>
-    <row r="94" spans="1:16">
+      <c r="Q93">
+        <v>7.184821587527658</v>
+      </c>
+    </row>
+    <row r="94" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A94" s="8" t="s">
         <v>92</v>
       </c>
@@ -5472,8 +5760,11 @@
       <c r="P94">
         <v>37.46</v>
       </c>
-    </row>
-    <row r="95" spans="1:16">
+      <c r="Q94">
+        <v>16.702394806149321</v>
+      </c>
+    </row>
+    <row r="95" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A95" s="8" t="s">
         <v>93</v>
       </c>
@@ -5519,8 +5810,11 @@
       <c r="P95">
         <v>37.090000000000003</v>
       </c>
-    </row>
-    <row r="96" spans="1:16">
+      <c r="Q95">
+        <v>0.97171106171579891</v>
+      </c>
+    </row>
+    <row r="96" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A96" s="8" t="s">
         <v>94</v>
       </c>
@@ -5566,8 +5860,11 @@
       <c r="P96">
         <v>4.93</v>
       </c>
-    </row>
-    <row r="97" spans="1:16">
+      <c r="Q96">
+        <v>14.745029307093688</v>
+      </c>
+    </row>
+    <row r="97" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A97" s="8" t="s">
         <v>95</v>
       </c>
@@ -5613,8 +5910,11 @@
       <c r="P97">
         <v>74.739999999999995</v>
       </c>
-    </row>
-    <row r="98" spans="1:16">
+      <c r="Q97">
+        <v>30.513505491243691</v>
+      </c>
+    </row>
+    <row r="98" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A98" s="8" t="s">
         <v>96</v>
       </c>
@@ -5662,13 +5962,16 @@
       <c r="P98">
         <v>21.54</v>
       </c>
-    </row>
-    <row r="99" spans="1:16">
+      <c r="Q98">
+        <v>2.1647487752079297</v>
+      </c>
+    </row>
+    <row r="99" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A99" s="8" t="s">
         <v>97</v>
       </c>
       <c r="B99" s="9">
-        <v>6.4763565063476562</v>
+        <v>6.4763565063476563</v>
       </c>
       <c r="C99" s="9">
         <f t="shared" si="1"/>
@@ -5705,8 +6008,11 @@
       <c r="P99">
         <v>48.12</v>
       </c>
-    </row>
-    <row r="100" spans="1:16">
+      <c r="Q99">
+        <v>12.497922552767161</v>
+      </c>
+    </row>
+    <row r="100" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A100" s="8" t="s">
         <v>98</v>
       </c>
@@ -5752,8 +6058,11 @@
       <c r="P100">
         <v>18.190000000000001</v>
       </c>
-    </row>
-    <row r="101" spans="1:16">
+      <c r="Q100">
+        <v>13.262808873450698</v>
+      </c>
+    </row>
+    <row r="101" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A101" s="8" t="s">
         <v>99</v>
       </c>
@@ -5799,8 +6108,11 @@
       <c r="P101">
         <v>17.64</v>
       </c>
-    </row>
-    <row r="102" spans="1:16">
+      <c r="Q101">
+        <v>37.331049551478415</v>
+      </c>
+    </row>
+    <row r="102" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A102" s="8" t="s">
         <v>100</v>
       </c>
@@ -5850,8 +6162,11 @@
       <c r="P102">
         <v>28.28</v>
       </c>
-    </row>
-    <row r="103" spans="1:16">
+      <c r="Q102">
+        <v>2.205092496653259</v>
+      </c>
+    </row>
+    <row r="103" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A103" s="8" t="s">
         <v>101</v>
       </c>
@@ -5897,8 +6212,11 @@
       <c r="P103">
         <v>11.68</v>
       </c>
-    </row>
-    <row r="104" spans="1:16">
+      <c r="Q103">
+        <v>40.265670402656703</v>
+      </c>
+    </row>
+    <row r="104" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A104" s="8" t="s">
         <v>102</v>
       </c>
@@ -5938,7 +6256,7 @@
         <v>53.67</v>
       </c>
     </row>
-    <row r="105" spans="1:16">
+    <row r="105" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A105" s="8" t="s">
         <v>103</v>
       </c>
@@ -5984,8 +6302,11 @@
       <c r="P105">
         <v>13.7</v>
       </c>
-    </row>
-    <row r="106" spans="1:16">
+      <c r="Q105">
+        <v>7.5733118105999457</v>
+      </c>
+    </row>
+    <row r="106" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A106" s="8" t="s">
         <v>104</v>
       </c>
@@ -6031,8 +6352,11 @@
       <c r="P106">
         <v>31.25</v>
       </c>
-    </row>
-    <row r="107" spans="1:16">
+      <c r="Q106">
+        <v>12.081550465643092</v>
+      </c>
+    </row>
+    <row r="107" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A107" s="8" t="s">
         <v>105</v>
       </c>
@@ -6078,8 +6402,11 @@
       <c r="P107">
         <v>18.920000000000002</v>
       </c>
-    </row>
-    <row r="108" spans="1:16">
+      <c r="Q107">
+        <v>2.7406250000000001</v>
+      </c>
+    </row>
+    <row r="108" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A108" s="8" t="s">
         <v>106</v>
       </c>
@@ -6125,8 +6452,11 @@
       <c r="P108">
         <v>27.24</v>
       </c>
-    </row>
-    <row r="109" spans="1:16">
+      <c r="Q108">
+        <v>18.747694268370392</v>
+      </c>
+    </row>
+    <row r="109" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A109" s="8" t="s">
         <v>107</v>
       </c>
@@ -6176,8 +6506,11 @@
       <c r="P109">
         <v>38.31</v>
       </c>
-    </row>
-    <row r="110" spans="1:16">
+      <c r="Q109">
+        <v>35.291812273425002</v>
+      </c>
+    </row>
+    <row r="110" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A110" s="8" t="s">
         <v>108</v>
       </c>
@@ -6227,8 +6560,11 @@
       <c r="P110">
         <v>27.61</v>
       </c>
-    </row>
-    <row r="111" spans="1:16">
+      <c r="Q110">
+        <v>10.68351747945426</v>
+      </c>
+    </row>
+    <row r="111" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A111" s="8" t="s">
         <v>109</v>
       </c>
@@ -6278,13 +6614,16 @@
       <c r="P111">
         <v>34.44</v>
       </c>
-    </row>
-    <row r="112" spans="1:16">
+      <c r="Q111">
+        <v>37.30006954102921</v>
+      </c>
+    </row>
+    <row r="112" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A112" s="8" t="s">
         <v>110</v>
       </c>
       <c r="B112" s="9">
-        <v>5.5787429809570312</v>
+        <v>5.5787429809570313</v>
       </c>
       <c r="C112" s="9">
         <f t="shared" si="1"/>
@@ -6329,8 +6668,11 @@
       <c r="P112">
         <v>24.5</v>
       </c>
-    </row>
-    <row r="113" spans="1:16">
+      <c r="Q112">
+        <v>7.5180312423863649</v>
+      </c>
+    </row>
+    <row r="113" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A113" s="8" t="s">
         <v>111</v>
       </c>
@@ -6376,8 +6718,11 @@
       <c r="P113">
         <v>5.57</v>
       </c>
-    </row>
-    <row r="114" spans="1:16">
+      <c r="Q113">
+        <v>46.684229881308468</v>
+      </c>
+    </row>
+    <row r="114" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A114" s="8" t="s">
         <v>112</v>
       </c>
@@ -6423,8 +6768,11 @@
       <c r="P114">
         <v>46.39</v>
       </c>
-    </row>
-    <row r="115" spans="1:16">
+      <c r="Q114">
+        <v>1.6174425149672742</v>
+      </c>
+    </row>
+    <row r="115" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A115" s="8" t="s">
         <v>113</v>
       </c>
@@ -6470,8 +6818,11 @@
       <c r="P115">
         <v>17.96</v>
       </c>
-    </row>
-    <row r="116" spans="1:16">
+      <c r="Q115">
+        <v>16.620786370955177</v>
+      </c>
+    </row>
+    <row r="116" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A116" s="8" t="s">
         <v>114</v>
       </c>
@@ -6518,8 +6869,11 @@
       <c r="O116">
         <v>53.5</v>
       </c>
-    </row>
-    <row r="117" spans="1:16">
+      <c r="Q116">
+        <v>29.705008003658818</v>
+      </c>
+    </row>
+    <row r="117" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A117" s="8" t="s">
         <v>115</v>
       </c>
@@ -6560,8 +6914,11 @@
       <c r="P117">
         <v>43.42</v>
       </c>
-    </row>
-    <row r="118" spans="1:16">
+      <c r="Q117">
+        <v>21.945137157107229</v>
+      </c>
+    </row>
+    <row r="118" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A118" s="8" t="s">
         <v>116</v>
       </c>
@@ -6609,8 +6966,11 @@
       <c r="P118">
         <v>133.76</v>
       </c>
-    </row>
-    <row r="119" spans="1:16">
+      <c r="Q118">
+        <v>0.78984483826813856</v>
+      </c>
+    </row>
+    <row r="119" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A119" s="8" t="s">
         <v>117</v>
       </c>
@@ -6660,8 +7020,11 @@
       <c r="P119">
         <v>81.709999999999994</v>
       </c>
-    </row>
-    <row r="120" spans="1:16">
+      <c r="Q119">
+        <v>28.015806988352743</v>
+      </c>
+    </row>
+    <row r="120" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A120" s="8" t="s">
         <v>118</v>
       </c>
@@ -6711,8 +7074,11 @@
       <c r="P120">
         <v>72.790000000000006</v>
       </c>
-    </row>
-    <row r="121" spans="1:16">
+      <c r="Q120">
+        <v>9.1291832658336602</v>
+      </c>
+    </row>
+    <row r="121" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A121" s="8" t="s">
         <v>119</v>
       </c>
@@ -6762,8 +7128,11 @@
       <c r="P121">
         <v>34.75</v>
       </c>
-    </row>
-    <row r="122" spans="1:16">
+      <c r="Q121">
+        <v>10.304264316744842</v>
+      </c>
+    </row>
+    <row r="122" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A122" s="8" t="s">
         <v>120</v>
       </c>
@@ -6813,8 +7182,11 @@
       <c r="P122">
         <v>41.87</v>
       </c>
-    </row>
-    <row r="123" spans="1:16">
+      <c r="Q122">
+        <v>14.576002862502321</v>
+      </c>
+    </row>
+    <row r="123" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A123" s="8" t="s">
         <v>121</v>
       </c>
@@ -6849,7 +7221,7 @@
         <v>15.9</v>
       </c>
     </row>
-    <row r="124" spans="1:16">
+    <row r="124" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A124" s="8" t="s">
         <v>122</v>
       </c>
@@ -6899,8 +7271,11 @@
       <c r="P124">
         <v>22.94</v>
       </c>
-    </row>
-    <row r="125" spans="1:16">
+      <c r="Q124">
+        <v>24.695894967158079</v>
+      </c>
+    </row>
+    <row r="125" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A125" s="8" t="s">
         <v>123</v>
       </c>
@@ -6946,8 +7321,11 @@
       <c r="P125">
         <v>13.62</v>
       </c>
-    </row>
-    <row r="126" spans="1:16">
+      <c r="Q125">
+        <v>20.730346037314622</v>
+      </c>
+    </row>
+    <row r="126" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A126" s="8" t="s">
         <v>124</v>
       </c>
@@ -6993,8 +7371,11 @@
       <c r="P126">
         <v>29.58</v>
       </c>
-    </row>
-    <row r="127" spans="1:16">
+      <c r="Q126">
+        <v>6.3209842568467511</v>
+      </c>
+    </row>
+    <row r="127" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A127" s="8" t="s">
         <v>125</v>
       </c>
@@ -7044,8 +7425,11 @@
       <c r="P127">
         <v>42.51</v>
       </c>
-    </row>
-    <row r="128" spans="1:16">
+      <c r="Q127">
+        <v>10.089584025557285</v>
+      </c>
+    </row>
+    <row r="128" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A128" s="8" t="s">
         <v>126</v>
       </c>
@@ -7079,7 +7463,7 @@
         <v>83.99</v>
       </c>
     </row>
-    <row r="129" spans="1:16">
+    <row r="129" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A129" s="8" t="s">
         <v>127</v>
       </c>
@@ -7123,8 +7507,11 @@
       <c r="P129">
         <v>8.8000000000000007</v>
       </c>
-    </row>
-    <row r="130" spans="1:16">
+      <c r="Q129">
+        <v>5.2597449383961381</v>
+      </c>
+    </row>
+    <row r="130" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A130" s="8" t="s">
         <v>128</v>
       </c>
@@ -7170,8 +7557,11 @@
       <c r="P130">
         <v>8.51</v>
       </c>
-    </row>
-    <row r="131" spans="1:16">
+      <c r="Q130">
+        <v>15.240460600587042</v>
+      </c>
+    </row>
+    <row r="131" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A131" s="8" t="s">
         <v>129</v>
       </c>
@@ -7221,8 +7611,11 @@
       <c r="P131">
         <v>60.39</v>
       </c>
-    </row>
-    <row r="132" spans="1:16">
+      <c r="Q131">
+        <v>32.903364716475167</v>
+      </c>
+    </row>
+    <row r="132" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A132" s="8" t="s">
         <v>130</v>
       </c>
@@ -7268,8 +7661,11 @@
       <c r="P132">
         <v>43.48</v>
       </c>
-    </row>
-    <row r="133" spans="1:16">
+      <c r="Q132">
+        <v>48.722191579334435</v>
+      </c>
+    </row>
+    <row r="133" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A133" s="8" t="s">
         <v>131</v>
       </c>
@@ -7313,8 +7709,11 @@
       <c r="P133">
         <v>69.27</v>
       </c>
-    </row>
-    <row r="134" spans="1:16">
+      <c r="Q133">
+        <v>4.8732943469785575</v>
+      </c>
+    </row>
+    <row r="134" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A134" s="8" t="s">
         <v>132</v>
       </c>
@@ -7360,8 +7759,11 @@
       <c r="P134">
         <v>35.43</v>
       </c>
-    </row>
-    <row r="135" spans="1:16">
+      <c r="Q134">
+        <v>18.666323377960865</v>
+      </c>
+    </row>
+    <row r="135" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A135" s="8" t="s">
         <v>133</v>
       </c>
@@ -7407,8 +7809,11 @@
       <c r="P135">
         <v>20.3</v>
       </c>
-    </row>
-    <row r="136" spans="1:16">
+      <c r="Q135">
+        <v>26.481556072398426</v>
+      </c>
+    </row>
+    <row r="136" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A136" s="8" t="s">
         <v>134</v>
       </c>
@@ -7452,8 +7857,11 @@
       <c r="P136">
         <v>30.72</v>
       </c>
-    </row>
-    <row r="137" spans="1:16">
+      <c r="Q136">
+        <v>4.1282744238503613</v>
+      </c>
+    </row>
+    <row r="137" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A137" s="8" t="s">
         <v>135</v>
       </c>
@@ -7499,8 +7907,11 @@
       <c r="P137">
         <v>8.41</v>
       </c>
-    </row>
-    <row r="138" spans="1:16">
+      <c r="Q137">
+        <v>34.410532615200481</v>
+      </c>
+    </row>
+    <row r="138" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A138" s="8" t="s">
         <v>136</v>
       </c>
@@ -7546,8 +7957,11 @@
       <c r="P138">
         <v>44.92</v>
       </c>
-    </row>
-    <row r="139" spans="1:16">
+      <c r="Q138">
+        <v>56.579606069498865</v>
+      </c>
+    </row>
+    <row r="139" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A139" s="8" t="s">
         <v>137</v>
       </c>
@@ -7591,8 +8005,11 @@
       <c r="P139">
         <v>89.87</v>
       </c>
-    </row>
-    <row r="140" spans="1:16">
+      <c r="Q139">
+        <v>0.62658406082793583</v>
+      </c>
+    </row>
+    <row r="140" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A140" s="8" t="s">
         <v>138</v>
       </c>
@@ -7642,8 +8059,11 @@
       <c r="P140">
         <v>15.45</v>
       </c>
-    </row>
-    <row r="141" spans="1:16">
+      <c r="Q140">
+        <v>24.908071614206591</v>
+      </c>
+    </row>
+    <row r="141" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A141" s="8" t="s">
         <v>139</v>
       </c>
@@ -7689,8 +8109,11 @@
       <c r="P141">
         <v>9.34</v>
       </c>
-    </row>
-    <row r="142" spans="1:16">
+      <c r="Q141">
+        <v>16.645403840645777</v>
+      </c>
+    </row>
+    <row r="142" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A142" s="8" t="s">
         <v>140</v>
       </c>
@@ -7740,8 +8163,11 @@
       <c r="P142">
         <v>20</v>
       </c>
-    </row>
-    <row r="143" spans="1:16">
+      <c r="Q142">
+        <v>13.773283611337275</v>
+      </c>
+    </row>
+    <row r="143" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A143" s="8" t="s">
         <v>141</v>
       </c>
@@ -7787,8 +8213,11 @@
       <c r="P143">
         <v>21.07</v>
       </c>
-    </row>
-    <row r="144" spans="1:16">
+      <c r="Q143">
+        <v>10.343206393982134</v>
+      </c>
+    </row>
+    <row r="144" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A144" s="8" t="s">
         <v>142</v>
       </c>
@@ -7832,8 +8261,11 @@
       <c r="P144">
         <v>23.96</v>
       </c>
-    </row>
-    <row r="145" spans="1:16">
+      <c r="Q144">
+        <v>3.0610509608298848</v>
+      </c>
+    </row>
+    <row r="145" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A145" s="8" t="s">
         <v>143</v>
       </c>
@@ -7879,8 +8311,11 @@
       <c r="P145">
         <v>85.95</v>
       </c>
-    </row>
-    <row r="146" spans="1:16">
+      <c r="Q145">
+        <v>22.569097300609538</v>
+      </c>
+    </row>
+    <row r="146" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A146" s="8" t="s">
         <v>144</v>
       </c>
@@ -7924,13 +8359,16 @@
       <c r="P146">
         <v>29.56</v>
       </c>
-    </row>
-    <row r="147" spans="1:16">
+      <c r="Q146">
+        <v>2.3637706687879994</v>
+      </c>
+    </row>
+    <row r="147" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A147" s="8" t="s">
         <v>145</v>
       </c>
       <c r="B147" s="9">
-        <v>3.9327774047851562</v>
+        <v>3.9327774047851563</v>
       </c>
       <c r="C147" s="9">
         <f t="shared" si="2"/>
@@ -7969,8 +8407,11 @@
       <c r="P147">
         <v>35.72</v>
       </c>
-    </row>
-    <row r="148" spans="1:16">
+      <c r="Q147">
+        <v>5.111717940784783</v>
+      </c>
+    </row>
+    <row r="148" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A148" s="8" t="s">
         <v>146</v>
       </c>
@@ -8016,6 +8457,9 @@
       <c r="P148">
         <v>24.22</v>
       </c>
+      <c r="Q148">
+        <v>10.339925035543493</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Added household data for sweden and 'kind of' for Denmark
</commit_message>
<xml_diff>
--- a/data_tables/Total_data_cleaned.xlsx
+++ b/data_tables/Total_data_cleaned.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Felix\.RapidMiner\repositories\Local Repository\DataMining-Group23\data_tables\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6CA08636-CF28-487E-B218-55B6D281908B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{31699B69-7E47-422B-A13A-11973FBD1A8D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{196242FC-4F62-234C-ABAE-90D7B6224D3F}"/>
   </bookViews>
@@ -1027,8 +1027,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{67CF83BE-F021-5E44-A4B8-2C5D9BB127DA}">
   <dimension ref="A1:Q148"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="G1" sqref="G1:H1048576"/>
+    <sheetView tabSelected="1" topLeftCell="A123" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="J146" sqref="J146"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.69921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -2852,6 +2852,12 @@
       <c r="F35" s="10">
         <v>55.67</v>
       </c>
+      <c r="G35" s="9">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="H35">
+        <v>39.5</v>
+      </c>
       <c r="I35" s="4">
         <v>4</v>
       </c>
@@ -7551,6 +7557,12 @@
       <c r="F126" s="10">
         <v>59.32</v>
       </c>
+      <c r="G126" s="9">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="H126">
+        <v>39.5</v>
+      </c>
       <c r="I126" s="4">
         <v>2.8</v>
       </c>

</xml_diff>